<commit_message>
Updated Functional Tests - System administration module.xlsx
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAF398D-5509-4DCF-B45C-CC0F76E147BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A590AE10-2CEC-451A-B97C-AA6E5921AA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
   <si>
     <t>Test scenario</t>
   </si>
@@ -309,10 +309,6 @@
     <t>LOG_05.02</t>
   </si>
   <si>
-    <t>1. The user remains not logged in.
-2. System blocks the ability to log in for 1 minute.</t>
-  </si>
-  <si>
     <t>1. The ability to try logging in again is unlocked for the user.</t>
   </si>
   <si>
@@ -323,12 +319,6 @@
   </si>
   <si>
     <t>1. The user can once again try to log in.</t>
-  </si>
-  <si>
-    <t>1. User enters login data: login and password.
-2. User presses the Login button.
-3. System verifies the entered data.
-4. After third unsuccessful attempt the system blocks input data fields and the login button and the system informs the user about the remaining time during which they cannot log in.</t>
   </si>
   <si>
     <t>1. System presents the error message: "Too many incorrect attempts. Login has been blocked. Please try again in Xm Xs"</t>
@@ -355,9 +345,6 @@
 </t>
   </si>
   <si>
-    <t>System blocks the ability to log in for a specified period of time after third unsuccesful attempt in a row.</t>
-  </si>
-  <si>
     <t>System presents the error message: "Too many incorrect attempts. Login has been blocked. Please try again in Xm Xs"</t>
   </si>
   <si>
@@ -365,6 +352,240 @@
   </si>
   <si>
     <t>24.03.2022</t>
+  </si>
+  <si>
+    <t>LOG_08</t>
+  </si>
+  <si>
+    <t>Setup the time to unlock login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The user is logged in into the system as an Administrator.
+2. User launches the Settings module from the Administrator's panel. 
+</t>
+  </si>
+  <si>
+    <t>1. The "Time to unlock page" parameter has been changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Administrator sets up the new time for the "Time to unlock page" parameter.
+2. Administrator changes the parameter. 
+</t>
+  </si>
+  <si>
+    <t>Administrator has the possibility of setting the time to unlock login page after it has been blocked.</t>
+  </si>
+  <si>
+    <t>1. System presents a message "The time to unlock page has been changed".</t>
+  </si>
+  <si>
+    <t>Administrator changes the time before the login form unlocks by inserting a correct value.</t>
+  </si>
+  <si>
+    <t>LOG_08.02</t>
+  </si>
+  <si>
+    <t>LOG_08.01</t>
+  </si>
+  <si>
+    <t>Administrator inserts an uncorrect value.</t>
+  </si>
+  <si>
+    <t>A non-negative integer</t>
+  </si>
+  <si>
+    <t>A negative integer</t>
+  </si>
+  <si>
+    <t>1. System presents an error message "Please select a correct value".</t>
+  </si>
+  <si>
+    <t>1. User enters login data: login and password.
+2. User presses the Login button.
+3. System verifies the entered data.
+4. After third unsuccessful attempt the system blocks input data fields and the login button. 
+5. The system informs the user about the remaining time during which they cannot log in.</t>
+  </si>
+  <si>
+    <t>1. The user remains not logged in.
+2. System blocks the ability to log in for X minutes.</t>
+  </si>
+  <si>
+    <t>1. Login: (empty)
+2. Password: (empty)</t>
+  </si>
+  <si>
+    <t>Application for changing password</t>
+  </si>
+  <si>
+    <t>PAS_01.01</t>
+  </si>
+  <si>
+    <t>PAS_01.02</t>
+  </si>
+  <si>
+    <t>PAS_01.03</t>
+  </si>
+  <si>
+    <t>1. Login: LMartin8096_x000D_
+2. E-mail: (correct e-mail)</t>
+  </si>
+  <si>
+    <t>1. Login: LMartin8096
+2. E-mail: lmartin@eksoc@com</t>
+  </si>
+  <si>
+    <t>PAS_02</t>
+  </si>
+  <si>
+    <t>Password change link</t>
+  </si>
+  <si>
+    <t>System gives non-logged users the possibility to change their passwords in case they forget them</t>
+  </si>
+  <si>
+    <t>PAS_02.01</t>
+  </si>
+  <si>
+    <t>PAS_03</t>
+  </si>
+  <si>
+    <t>Password change form launching</t>
+  </si>
+  <si>
+    <t>1. The non-logged user is able to change their password.</t>
+  </si>
+  <si>
+    <t>USER PODAJE DANE</t>
+  </si>
+  <si>
+    <t>SYSTEM JE WERYFIKUJE</t>
+  </si>
+  <si>
+    <t>GENERUJE I WYSYŁA LINK</t>
+  </si>
+  <si>
+    <t>UŻYTKOWNIK OTRZYMUJE LINK</t>
+  </si>
+  <si>
+    <t>MOŻE W NIEGO KLIKNĄĆ</t>
+  </si>
+  <si>
+    <t>UŻYTKOWNIK KLIKA W LINK</t>
+  </si>
+  <si>
+    <t>UŻYTKOWNK ZOSTAJE PRZENIESIONY DO FORMA GDZIE MOŻE ZMIENIĆ HASŁO</t>
+  </si>
+  <si>
+    <t>1. The non-logged user receives a mail with the password change link.</t>
+  </si>
+  <si>
+    <t>1. The non-logged user entered his username and e-mail address into the "Forgot password" form.
+2. System verified the mentioned details.</t>
+  </si>
+  <si>
+    <t>1. The non-logged user clicks the received link.
+2. The password change module is presented.</t>
+  </si>
+  <si>
+    <t>User clicks the link from the mail message.</t>
+  </si>
+  <si>
+    <t>1. System presents the password reset form.</t>
+  </si>
+  <si>
+    <t>PAS_03.01</t>
+  </si>
+  <si>
+    <t>The user gets the possibility to input a new password after opening the link to the form.</t>
+  </si>
+  <si>
+    <t>31.03.2022</t>
+  </si>
+  <si>
+    <t>System presents a message "The time to unlock page has been changed".</t>
+  </si>
+  <si>
+    <t>System presents an error message "Please select a correct value".</t>
+  </si>
+  <si>
+    <t>System presents the password reset form.</t>
+  </si>
+  <si>
+    <t>1. User is able to send the data to the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Users inserts his login and e-mail address.
+2. System verifies whether the format of entered data is correct.
+3. In case of a successful verification the system unlocks the "OK" button. In case of an unsuccessful verification the "OK" button remains blocked.</t>
+  </si>
+  <si>
+    <t>1. Login: LMartin8096
+2. E-mail: (empty)</t>
+  </si>
+  <si>
+    <t>1. System unlocks the "OK" button.</t>
+  </si>
+  <si>
+    <t>1. The "OK" button remains blocked.</t>
+  </si>
+  <si>
+    <t>1. User presses the "OK" button.
+2. System checks if the provided e-mail address is the same as the e-mail address corresponding to the provided user name. 
+In case of a successful verification:
+3. System generates an e-mail message that contains a link to the password change form.
+4. System sends an e-mail to the specified e-mail address.
+Alternative:
+3. The entered data is not matching the data in the database.
+4. The e-mail is not being sent.</t>
+  </si>
+  <si>
+    <t>PAS_02.02</t>
+  </si>
+  <si>
+    <t>Correct data format: user entered the login and an e-mail address with exactly one "@" character.</t>
+  </si>
+  <si>
+    <t>Incorrect data format: user entered the login and an e-mail address that didn't have exactly one "@" character.</t>
+  </si>
+  <si>
+    <t>Correct data: login and e-mail address are the same as the ones stored in the database.</t>
+  </si>
+  <si>
+    <t>Incorrect data: login and e-mail address are not the same as the ones stored in the database.</t>
+  </si>
+  <si>
+    <t>System verifies the entered data with the data stored in the database and generates a link that leads to the password change form.</t>
+  </si>
+  <si>
+    <t>1. Proper URL address exists.
+2. System is launched.
+3. Login form is presented.
+4. User picks the "Forgot password" option.
+5. The "Forgot password" form is launched.</t>
+  </si>
+  <si>
+    <t>1. Login: LMartin8096
+2. E-mail: admin@eksocmed.com</t>
+  </si>
+  <si>
+    <t>1. The non-logged user received the password change link.</t>
+  </si>
+  <si>
+    <t>System sends an e-mail to the user.</t>
+  </si>
+  <si>
+    <t>1. System presents an error message.
+2. The e-mail is not being sent.</t>
+  </si>
+  <si>
+    <t>1. System presents a message: "The e-mail has been sent. Please check your mailbox."
+2. System sends an e-mail to the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The e-mail is not being sent.</t>
   </si>
 </sst>
 </file>
@@ -374,7 +595,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,22 +647,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -722,6 +959,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -731,7 +979,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -830,15 +1078,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -851,59 +1090,152 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1224,61 +1556,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="48" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="54"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="80"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:12" ht="16.5" thickBot="1">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="36" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -1298,26 +1631,26 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A3" s="55" t="s">
+    <row r="3" spans="1:12" ht="47.25">
+      <c r="A3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="76" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="10" t="s">
@@ -1334,14 +1667,14 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="58"/>
+    <row r="4" spans="1:12" ht="47.25">
+      <c r="A4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="84"/>
       <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1356,14 +1689,14 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="52"/>
+    <row r="5" spans="1:12" ht="48" thickBot="1">
+      <c r="A5" s="79"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="77"/>
       <c r="H5" s="28" t="s">
         <v>38</v>
       </c>
@@ -1378,7 +1711,7 @@
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="108.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:12" ht="63.75" thickBot="1">
       <c r="A6" s="29" t="s">
         <v>29</v>
       </c>
@@ -1414,7 +1747,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="130.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:12" ht="79.5" thickBot="1">
       <c r="A7" s="29" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1783,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="102.75" customHeight="1" thickBot="1">
+    <row r="8" spans="1:12" ht="79.5" thickBot="1">
       <c r="A8" s="29" t="s">
         <v>28</v>
       </c>
@@ -1486,26 +1819,26 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="91.5" customHeight="1">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:12" ht="47.25">
+      <c r="A9" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="51" t="s">
+      <c r="F9" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="76" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -1522,14 +1855,14 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="91.5" customHeight="1" thickBot="1">
-      <c r="A10" s="48"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="52"/>
+    <row r="10" spans="1:12" ht="48" thickBot="1">
+      <c r="A10" s="78"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="29" t="s">
         <v>82</v>
       </c>
@@ -1539,12 +1872,12 @@
       <c r="J10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="34" t="s">
         <v>50</v>
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="161.25" customHeight="1" thickBot="1">
+    <row r="11" spans="1:12" ht="158.25" thickBot="1">
       <c r="A11" s="29" t="s">
         <v>69</v>
       </c>
@@ -1558,29 +1891,29 @@
         <v>12</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>88</v>
+        <v>111</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>110</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>17</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="37" t="s">
-        <v>89</v>
+        <v>112</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>87</v>
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="131.25" customHeight="1" thickBot="1">
+    <row r="12" spans="1:12" ht="111" thickBot="1">
       <c r="A12" s="29" t="s">
         <v>70</v>
       </c>
@@ -1594,45 +1927,313 @@
         <v>12</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="47.25">
+      <c r="A13" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="57"/>
+    </row>
+    <row r="14" spans="1:12" ht="32.25" thickBot="1">
+      <c r="A14" s="79"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="71.25" customHeight="1">
+      <c r="A15" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="71.25" customHeight="1">
+      <c r="A16" s="87"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="K16" s="47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="71.25" customHeight="1" thickBot="1">
+      <c r="A17" s="87"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="J17" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17" s="53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
+      <c r="A18" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
+      <c r="A19" s="78"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" s="70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+      <c r="A20" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="J20" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A13" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
+      <c r="K20" s="51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="60"/>
+      <c r="C28" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="37">
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H1:K1"/>
@@ -1647,8 +2248,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1656,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B269C-A11B-41F2-B2B7-9B8EF1E55741}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1702,7 +2301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="69.75" customHeight="1">
+    <row r="2" spans="1:13" ht="31.5">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1727,7 +2326,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:13" ht="69.75" customHeight="1">
+    <row r="3" spans="1:13" ht="63">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -1752,7 +2351,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:13" ht="63.75" thickBot="1">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1777,7 +2376,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="23"/>
     </row>
-    <row r="5" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+    <row r="5" spans="1:13" ht="32.25" thickBot="1">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -1802,7 +2401,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="27"/>
     </row>
-    <row r="6" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:13" ht="32.25" thickBot="1">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -1826,8 +2425,9 @@
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+      <c r="M6" s="64"/>
+    </row>
+    <row r="7" spans="1:13" ht="16.5" thickBot="1">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -1840,10 +2440,10 @@
       <c r="D7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="38" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="25" t="s">
@@ -1851,107 +2451,275 @@
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="27"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
-      <c r="A8" s="24">
-        <v>6</v>
-      </c>
-      <c r="B8" s="25" t="s">
+      <c r="M7" s="54"/>
+    </row>
+    <row r="8" spans="1:13" ht="63">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
-      <c r="A9" s="24">
-        <v>6</v>
-      </c>
-      <c r="B9" s="25" t="s">
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" ht="63.75" thickBot="1">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="44" t="s">
+      <c r="D9" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:13" ht="136.5" customHeight="1" thickBot="1">
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:13" ht="79.5" thickBot="1">
       <c r="A10" s="24">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="40" t="s">
         <v>63</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:13" ht="69.75" customHeight="1" thickBot="1">
+    <row r="11" spans="1:13" ht="32.25" thickBot="1">
       <c r="A11" s="24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G11" s="22" t="s">
         <v>63</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="47.25">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:13" ht="48" thickBot="1">
+      <c r="A13" s="21">
+        <v>12</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="1:13" ht="31.5">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" ht="31.5">
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:13" ht="32.25" thickBot="1">
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" ht="31.5">
+      <c r="A17" s="15">
+        <v>17</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" ht="63.75" thickBot="1">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="62"/>
+    </row>
+    <row r="19" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Functional Tests - System administration module.xlsx - updated the additional cases of incorrect passwords in PAS_04
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98361466-0008-40F3-8C2D-89C0AD78AA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCA3581-A585-44D1-B328-2BDF4E198ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="206">
   <si>
     <t>Test scenario</t>
   </si>
@@ -603,14 +603,79 @@
 1234</t>
   </si>
   <si>
-    <t>1. New password: 
-1234zaq1
-2. Confirm password:
-1234zaq1</t>
-  </si>
-  <si>
     <t>1. The "OK" button is unlocked
 2. The system informs the user that "Password must include at least one lowercase, uppercase, number and special character (-, _, !, #, $, *)"</t>
+  </si>
+  <si>
+    <t>PAS_05</t>
+  </si>
+  <si>
+    <t>Password change cancellation</t>
+  </si>
+  <si>
+    <t>1. The non-logged user has cancelled the process of changing the password.</t>
+  </si>
+  <si>
+    <t>1. The non-logged user clicks the "Cancel" button.
+2. The system opens a confirmation window.
+3. The non-logged user clicks the "OK" button, confirming his will to cancel the process.
+4. The system closes the form.</t>
+  </si>
+  <si>
+    <t>PAS_05.01</t>
+  </si>
+  <si>
+    <t>1. The system closes the password change  form.</t>
+  </si>
+  <si>
+    <t>PAS_06</t>
+  </si>
+  <si>
+    <t>PAS_06.01</t>
+  </si>
+  <si>
+    <t>Cancellation of password change cancellation</t>
+  </si>
+  <si>
+    <t>1. The non-logged user has pressed the "Cancel" button in the password changing form.</t>
+  </si>
+  <si>
+    <t>1. The non-logged user has returned to the password changing form.</t>
+  </si>
+  <si>
+    <t>Successful cancellation of the password changing process.</t>
+  </si>
+  <si>
+    <t>Successful cancellation  of the password change cancellation process.</t>
+  </si>
+  <si>
+    <t>1. The system closes the pop-up window.
+2. The system returns to the password change form with cleared fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The non-logged user clicks the "Cancel" button.
+2. The system returns to the password change form with emptied fields.</t>
+  </si>
+  <si>
+    <t>The non-logged user has the possibility to resign from password changing at any time.</t>
+  </si>
+  <si>
+    <t>The non-logged user has the possibility to return to the password change form in case of pressing the "Cancel" button by accident.</t>
+  </si>
+  <si>
+    <t>21.04.2022</t>
+  </si>
+  <si>
+    <t>1. The "OK" button is unlocked
+2. The password is changed.
+3. The password change form is closed.</t>
+  </si>
+  <si>
+    <t>The system closes the password change  form.</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are not the same</t>
   </si>
   <si>
     <t>1. The non-logged user enters their new password into "New password" and "Confirm password" fields.
@@ -620,87 +685,76 @@
 5. The system checks the validation criteria.
 6. The system informs the non-logged user that the passwords are meeting the criteria by displaying a success message in a pop-up window.
 7. The non-logged user confirms their decision by pressing the "OK" button in the pop-up window.
-8. The password is changed and the form closes itself.
-Alternative:
-3. The system informs the non-logged user that the passwords in the fields are not matching by keeping the "OK" button locked.
-Alternative:
-6. The system informs the non-logged user that the passwords are not meeting the criteria by displaying an error message in a pop-up window.
-7. The non-logged user presses the "OK" button in the newly opened pop-up window.
-8. The system returns to the password change form.</t>
-  </si>
-  <si>
-    <t>PAS_05</t>
-  </si>
-  <si>
-    <t>Password change cancellation</t>
-  </si>
-  <si>
-    <t>1. The non-logged user has cancelled the process of changing the password.</t>
-  </si>
-  <si>
-    <t>1. The non-logged user clicks the "Cancel" button.
-2. The system opens a confirmation window.
-3. The non-logged user clicks the "OK" button, confirming his will to cancel the process.
-4. The system closes the form.</t>
-  </si>
-  <si>
-    <t>PAS_05.01</t>
-  </si>
-  <si>
-    <t>1. The system closes the password change  form.</t>
-  </si>
-  <si>
-    <t>PAS_06</t>
-  </si>
-  <si>
-    <t>PAS_06.01</t>
-  </si>
-  <si>
-    <t>Cancellation of password change cancellation</t>
-  </si>
-  <si>
-    <t>1. The non-logged user has pressed the "Cancel" button in the password changing form.</t>
-  </si>
-  <si>
-    <t>1. The non-logged user has returned to the password changing form.</t>
-  </si>
-  <si>
-    <t>Successful cancellation of the password changing process.</t>
-  </si>
-  <si>
-    <t>Successful cancellation  of the password change cancellation process.</t>
-  </si>
-  <si>
-    <t>1. The system closes the pop-up window.
-2. The system returns to the password change form with cleared fields.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. The non-logged user clicks the "Cancel" button.
-2. The system returns to the password change form with emptied fields.</t>
-  </si>
-  <si>
-    <t>The non-logged user has the possibility to resign from password changing at any time.</t>
-  </si>
-  <si>
-    <t>The non-logged user has the possibility to return to the password change form in case of pressing the "Cancel" button by accident.</t>
-  </si>
-  <si>
-    <t>21.04.2022</t>
-  </si>
-  <si>
-    <t>1. The "OK" button is unlocked
-2. The password is changed.
-3. The password change form is closed.</t>
-  </si>
-  <si>
-    <t>The system closes the password change  form.</t>
-  </si>
-  <si>
-    <t>Incorrect data: user enters two passwords that are not the same</t>
-  </si>
-  <si>
-    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria</t>
+8. The password is changed and the form closes itself.</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the lack of a special character</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the password is too short (less than 8 characters)</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the password is too long (more than 15 characters)</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the lack of a lowercase character</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the lack of an uppercase character</t>
+  </si>
+  <si>
+    <t>Incorrect data: user enters two passwords that are the same but they are not matching the acceptance criteria - the lack of a number</t>
+  </si>
+  <si>
+    <t>PAS_04.04</t>
+  </si>
+  <si>
+    <t>PAS_04.05</t>
+  </si>
+  <si>
+    <t>PAS_04.06</t>
+  </si>
+  <si>
+    <t>PAS_04.07</t>
+  </si>
+  <si>
+    <t>PAS_04.08</t>
+  </si>
+  <si>
+    <t>1. New password: 
+qwerty
+2. Confirm password:
+qwerty</t>
+  </si>
+  <si>
+    <t>1. New password: 
+qwertyuiopasdfghjkl
+2. Confirm password:
+qwertyuiopasdfghjkl</t>
+  </si>
+  <si>
+    <t>1. New password: 
+PASSW0RD!
+2. Confirm password:
+PASSW0RD!</t>
+  </si>
+  <si>
+    <t>1. New password: 
+hasl0-haslo
+2. Confirm password:
+hasl0-haslo</t>
+  </si>
+  <si>
+    <t>1. New password: 
+Password_
+2. Confirm password:
+Password_</t>
+  </si>
+  <si>
+    <t>1. New password: 
+1234Zaq1
+2. Confirm password:
+1234Zaq1</t>
   </si>
 </sst>
 </file>
@@ -710,7 +764,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,13 +817,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -782,13 +829,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1090,7 +1130,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1259,10 +1299,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,10 +1321,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1306,7 +1342,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,12 +1360,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1347,6 +1376,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1361,10 +1449,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1382,38 +1476,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1733,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A23"/>
+      <selection activeCell="A21" sqref="A21:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1755,21 +1823,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="92" t="s">
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="117"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
@@ -1809,25 +1877,25 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="47.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="114" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="10" t="s">
@@ -1845,13 +1913,13 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="47.25">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="88"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="121"/>
       <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1867,13 +1935,13 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="48" thickBot="1">
-      <c r="A5" s="96"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="89"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="28" t="s">
         <v>38</v>
       </c>
@@ -1997,25 +2065,25 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="47.25">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="87" t="s">
+      <c r="G9" s="114" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -2033,13 +2101,13 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="48" thickBot="1">
-      <c r="A10" s="92"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="89"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="115"/>
       <c r="H10" s="29" t="s">
         <v>82</v>
       </c>
@@ -2127,25 +2195,25 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="47.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="105" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="105" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="105" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="84" t="s">
+      <c r="F13" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="87" t="s">
+      <c r="G13" s="114" t="s">
         <v>100</v>
       </c>
       <c r="H13" s="54" t="s">
@@ -2163,13 +2231,13 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="32.25" thickBot="1">
-      <c r="A14" s="96"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="89"/>
+      <c r="A14" s="116"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="115"/>
       <c r="H14" s="54" t="s">
         <v>104</v>
       </c>
@@ -2184,25 +2252,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="87" t="s">
+      <c r="G15" s="114" t="s">
         <v>136</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -2219,13 +2287,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A16" s="91"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="88"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="45" t="s">
         <v>115</v>
       </c>
@@ -2240,13 +2308,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A17" s="91"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="88"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="121"/>
       <c r="H17" s="57" t="s">
         <v>116</v>
       </c>
@@ -2261,28 +2329,28 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="93" t="s">
+      <c r="C18" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="111" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="94" t="s">
+      <c r="G18" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="66" t="s">
+      <c r="H18" s="65" t="s">
         <v>122</v>
       </c>
       <c r="I18" s="47" t="s">
@@ -2296,13 +2364,13 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A19" s="92"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="95"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="113"/>
       <c r="H19" s="11" t="s">
         <v>141</v>
       </c>
@@ -2312,7 +2380,7 @@
       <c r="J19" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="K19" s="67" t="s">
+      <c r="K19" s="66" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2351,184 +2419,261 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="225.75" customHeight="1" thickBot="1">
-      <c r="A21" s="90" t="s">
+    <row r="21" spans="1:11" ht="96.6" customHeight="1">
+      <c r="A21" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="105" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="105" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="84" t="s">
+      <c r="D21" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="84" t="s">
+      <c r="E21" s="105" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="84" t="s">
+      <c r="F21" s="105" t="s">
         <v>160</v>
       </c>
-      <c r="G21" s="87" t="s">
+      <c r="G21" s="105" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="I21" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="J21" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" s="82" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="69" customHeight="1">
+      <c r="A22" s="109"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="80" t="s">
+        <v>187</v>
+      </c>
+      <c r="J22" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="83" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A23" s="109"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="97" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" s="80" t="s">
+        <v>200</v>
+      </c>
+      <c r="K23" s="83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A24" s="109"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="106"/>
+      <c r="G24" s="106"/>
+      <c r="H24" s="97" t="s">
+        <v>195</v>
+      </c>
+      <c r="I24" s="80" t="s">
+        <v>191</v>
+      </c>
+      <c r="J24" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="K24" s="83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A25" s="109"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="97" t="s">
+        <v>196</v>
+      </c>
+      <c r="I25" s="80" t="s">
+        <v>192</v>
+      </c>
+      <c r="J25" s="80" t="s">
+        <v>202</v>
+      </c>
+      <c r="K25" s="83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A26" s="109"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="97" t="s">
+        <v>197</v>
+      </c>
+      <c r="I26" s="80" t="s">
+        <v>193</v>
+      </c>
+      <c r="J26" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="K26" s="83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A27" s="109"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="97" t="s">
+        <v>198</v>
+      </c>
+      <c r="I27" s="80" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" s="80" t="s">
+        <v>204</v>
+      </c>
+      <c r="K27" s="83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="99.75" customHeight="1" thickBot="1">
+      <c r="A28" s="110"/>
+      <c r="B28" s="107"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="I28" s="81" t="s">
+        <v>189</v>
+      </c>
+      <c r="J28" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="K28" s="84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="139.5" customHeight="1" thickBot="1">
+      <c r="A29" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="67" t="s">
         <v>168</v>
       </c>
-      <c r="H21" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="I21" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="J21" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="225.75" customHeight="1" thickBot="1">
-      <c r="A22" s="91"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="85"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I22" s="69" t="s">
-        <v>189</v>
-      </c>
-      <c r="J22" s="69" t="s">
-        <v>165</v>
-      </c>
-      <c r="K22" s="71" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="225.75" customHeight="1" thickBot="1">
-      <c r="A23" s="92"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="I23" s="68" t="s">
-        <v>190</v>
-      </c>
-      <c r="J23" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="146.25" customHeight="1" thickBot="1">
-      <c r="A24" s="72" t="s">
+      <c r="C29" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="F29" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="G29" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="69" t="s">
-        <v>184</v>
-      </c>
-      <c r="D24" s="69" t="s">
+      <c r="H29" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="J29" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="87" customHeight="1" thickBot="1">
+      <c r="A30" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="F24" s="69" t="s">
-        <v>171</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I24" s="69" t="s">
+      <c r="E30" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="J30" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="J24" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="71" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="135" customHeight="1" thickBot="1">
-      <c r="A25" s="72" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="69" t="s">
-        <v>177</v>
-      </c>
-      <c r="C25" s="69" t="s">
-        <v>185</v>
-      </c>
-      <c r="D25" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="69" t="s">
-        <v>178</v>
-      </c>
-      <c r="F25" s="69" t="s">
-        <v>179</v>
-      </c>
-      <c r="G25" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="I25" s="69" t="s">
-        <v>181</v>
-      </c>
-      <c r="J25" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="71" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="B28" s="59"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="B29" s="59"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="B30" s="59"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="B15:B17"/>
@@ -2536,24 +2681,12 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="D15:D17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A5"/>
@@ -2563,27 +2696,39 @@
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="G3:G5"/>
+    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="G21:G28"/>
+    <mergeCell ref="F21:F28"/>
+    <mergeCell ref="E21:E28"/>
+    <mergeCell ref="D21:D28"/>
+    <mergeCell ref="C21:C28"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B269C-A11B-41F2-B2B7-9B8EF1E55741}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2749,7 +2894,7 @@
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="27"/>
-      <c r="M6" s="61"/>
+      <c r="M6" s="60"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1">
       <c r="A7" s="24">
@@ -2793,7 +2938,7 @@
       <c r="E8" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -2818,7 +2963,7 @@
       <c r="E9" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="61" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="40" t="s">
@@ -2890,10 +3035,10 @@
       <c r="D12" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="64" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="16" t="s">
@@ -2906,19 +3051,19 @@
       <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="63" t="s">
         <v>96</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="59" t="s">
         <v>132</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="67" t="s">
         <v>134</v>
       </c>
       <c r="G13" s="22" t="s">
@@ -2940,10 +3085,10 @@
       <c r="D14" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="F14" s="70" t="s">
+      <c r="F14" s="68" t="s">
         <v>138</v>
       </c>
       <c r="G14" s="16" t="s">
@@ -2956,50 +3101,50 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="64" t="s">
+      <c r="G15" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="64"/>
+      <c r="H15" s="63"/>
       <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:13" ht="32.25" thickBot="1">
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="67" t="s">
         <v>139</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="64"/>
+      <c r="H16" s="63"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:12" ht="32.25" thickBot="1">
@@ -3015,10 +3160,10 @@
       <c r="D17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="F17" s="68" t="s">
         <v>150</v>
       </c>
       <c r="G17" s="16" t="s">
@@ -3028,180 +3173,305 @@
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:12" ht="48" thickBot="1">
-      <c r="A18" s="104">
+      <c r="A18" s="87">
         <v>17</v>
       </c>
-      <c r="B18" s="105" t="s">
+      <c r="B18" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="106" t="s">
+      <c r="D18" s="89" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="74" t="s">
+      <c r="E18" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="105" t="s">
+      <c r="G18" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="107"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="90"/>
     </row>
     <row r="19" spans="1:12" ht="35.25" customHeight="1" thickBot="1">
-      <c r="A19" s="108">
+      <c r="A19" s="91">
         <v>18</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="110" t="s">
+      <c r="D19" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="G19" s="109" t="s">
+      <c r="G19" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="111"/>
-      <c r="I19" s="112"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="95"/>
     </row>
     <row r="20" spans="1:12" ht="108" customHeight="1">
-      <c r="A20" s="76">
+      <c r="A20" s="73">
         <v>19</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E20" s="70" t="s">
-        <v>187</v>
-      </c>
-      <c r="F20" s="70" t="s">
-        <v>187</v>
-      </c>
-      <c r="G20" s="77" t="s">
+      <c r="D20" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="77"/>
-      <c r="I20" s="79"/>
-      <c r="L20" s="61"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="76"/>
+      <c r="L20" s="60"/>
     </row>
     <row r="21" spans="1:12" ht="27" customHeight="1">
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="63"/>
+      <c r="I21" s="77"/>
+    </row>
+    <row r="22" spans="1:12" ht="113.25" customHeight="1">
+      <c r="A22" s="86">
+        <v>21</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="63"/>
+      <c r="I22" s="77"/>
+    </row>
+    <row r="23" spans="1:12" ht="45.75" customHeight="1">
+      <c r="A23" s="63">
+        <v>22</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="96" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="96" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="60"/>
+      <c r="I23" s="100"/>
+    </row>
+    <row r="24" spans="1:12" ht="94.5">
+      <c r="A24" s="98">
+        <v>23</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="60"/>
+      <c r="I24" s="100"/>
+    </row>
+    <row r="25" spans="1:12" ht="94.5">
+      <c r="A25" s="101">
+        <v>24</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F25" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="60"/>
+      <c r="I25" s="100"/>
+    </row>
+    <row r="26" spans="1:12" ht="94.5">
+      <c r="A26" s="98">
+        <v>25</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F26" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="60"/>
+      <c r="I26" s="100"/>
+    </row>
+    <row r="27" spans="1:12" ht="95.25" thickBot="1">
+      <c r="A27" s="102">
+        <v>26</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="78" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="103"/>
+      <c r="I27" s="104"/>
+    </row>
+    <row r="28" spans="1:12" ht="32.25" thickBot="1">
+      <c r="A28" s="91">
+        <v>27</v>
+      </c>
+      <c r="B28" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="F21" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="G21" s="64" t="s">
+      <c r="F28" s="99" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="64"/>
-      <c r="I21" s="80"/>
-    </row>
-    <row r="22" spans="1:12" ht="113.25" customHeight="1" thickBot="1">
-      <c r="A22" s="102">
-        <v>21</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="81" t="s">
-        <v>186</v>
-      </c>
-      <c r="E22" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="G22" s="40" t="s">
+      <c r="H28" s="88"/>
+      <c r="I28" s="90"/>
+    </row>
+    <row r="29" spans="1:12" ht="79.5" thickBot="1">
+      <c r="A29" s="73">
+        <v>28</v>
+      </c>
+      <c r="B29" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="82"/>
-    </row>
-    <row r="23" spans="1:12" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A23" s="76">
-        <v>22</v>
-      </c>
-      <c r="B23" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="103" t="s">
-        <v>188</v>
-      </c>
-      <c r="F23" s="103" t="s">
-        <v>188</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="1:12" ht="79.5" thickBot="1">
-      <c r="A24" s="104">
-        <v>23</v>
-      </c>
-      <c r="B24" s="105" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="105" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="106" t="s">
-        <v>186</v>
-      </c>
-      <c r="E24" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="F24" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="G24" s="105" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="105"/>
-      <c r="I24" s="107"/>
+      <c r="H29" s="88"/>
+      <c r="I29" s="90"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Functional Tests - System administration module.xlsx - added tests for viewing, sorting and filtering the list of users.
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\03.05.2022 testowanie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCA3581-A585-44D1-B328-2BDF4E198ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E230CE0B-6655-4B6B-B928-C6312E08A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="253">
   <si>
     <t>Test scenario</t>
   </si>
@@ -653,11 +653,6 @@
 2. The system returns to the password change form with cleared fields.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1. The non-logged user clicks the "Cancel" button.
-2. The system returns to the password change form with emptied fields.</t>
-  </si>
-  <si>
     <t>The non-logged user has the possibility to resign from password changing at any time.</t>
   </si>
   <si>
@@ -755,6 +750,154 @@
 1234Zaq1
 2. Confirm password:
 1234Zaq1</t>
+  </si>
+  <si>
+    <t>LIS_01</t>
+  </si>
+  <si>
+    <t>View list of users</t>
+  </si>
+  <si>
+    <t>The administrator has the possibility to access a list of users and their details.</t>
+  </si>
+  <si>
+    <t>1. An administrator is logged into the system.</t>
+  </si>
+  <si>
+    <t>1. The non-logged user clicks the "Cancel" button.
+2. The system returns to the password change form with emptied fields.</t>
+  </si>
+  <si>
+    <t>LIS_01.01</t>
+  </si>
+  <si>
+    <t>Successful display of the user list.</t>
+  </si>
+  <si>
+    <t>1. The system shows a form with the list of users.</t>
+  </si>
+  <si>
+    <t>Filtering the list of users</t>
+  </si>
+  <si>
+    <t>LIS_02</t>
+  </si>
+  <si>
+    <t>LIS_02.01</t>
+  </si>
+  <si>
+    <t>The administrator has the possibility to filter the list of users by their names and the role in the system.</t>
+  </si>
+  <si>
+    <t>1. The list of users has been opened.</t>
+  </si>
+  <si>
+    <t>1. The system presents a filtered list of users based on conditions specified by the administrator.</t>
+  </si>
+  <si>
+    <t>1. The system presents a list of users, their details and additional buttons.</t>
+  </si>
+  <si>
+    <t>Sorting the list of users</t>
+  </si>
+  <si>
+    <t>The administrator has the possibility to sort the list of users in an ascending or a descending order by all the available fields in the list.</t>
+  </si>
+  <si>
+    <t>1. The system presents a sorted list of users based on the column selected by the administrator.</t>
+  </si>
+  <si>
+    <t>1. An administrator chooses the "Users Management" option from the Administrator Panel. 
+2. The system displays the list of users.</t>
+  </si>
+  <si>
+    <t>LIS_03.01</t>
+  </si>
+  <si>
+    <t>LIS_03</t>
+  </si>
+  <si>
+    <t>1. The administrator selects the set of data on the basis of which the list is to be filtered.
+2. The system displays the filtered list of users that match the selected criteria.</t>
+  </si>
+  <si>
+    <t>1. Administrator clicks the name of a column.</t>
+  </si>
+  <si>
+    <t>Successful display of the user list sorted in a descending order.</t>
+  </si>
+  <si>
+    <t>Successful display of the user list sorted in a ascending order.</t>
+  </si>
+  <si>
+    <t>1. Administrator clicks the name of a column once again.</t>
+  </si>
+  <si>
+    <t>1. System shows the list of users sorted in a descending order by the selected column.</t>
+  </si>
+  <si>
+    <t>1. System shows the list of users sorted in a ascending order by the selected column.</t>
+  </si>
+  <si>
+    <t>LIS_02.02</t>
+  </si>
+  <si>
+    <t>LIS_02.03</t>
+  </si>
+  <si>
+    <t>Successful display of the user list filtered by the first name of the employee.</t>
+  </si>
+  <si>
+    <t>Successful display of the user list filtered by the role in the system.</t>
+  </si>
+  <si>
+    <t>Successful display of the user list filtered by the second name of the employee.</t>
+  </si>
+  <si>
+    <t>1. First name: "A"</t>
+  </si>
+  <si>
+    <t>1. The system shows a list of users whose first names begin with "A".</t>
+  </si>
+  <si>
+    <t>1. Second name: "F"</t>
+  </si>
+  <si>
+    <t>1. The system shows a list of users whose second names begin with "F".</t>
+  </si>
+  <si>
+    <t>1. Position: "manager"</t>
+  </si>
+  <si>
+    <t>1. The system shows a list of users whose role is manager.</t>
+  </si>
+  <si>
+    <t>1. The administrator selects and clicks the name of the column on the basis of which he wants to sort all the users currently shown.
+2. The system displays a sorted list of  all the users currently shown.</t>
+  </si>
+  <si>
+    <t>LIS_03.02</t>
+  </si>
+  <si>
+    <t>03.05.2022</t>
+  </si>
+  <si>
+    <t>The system shows a form with the list of users.</t>
+  </si>
+  <si>
+    <t>The system shows a list of users whose first names begin with "A".</t>
+  </si>
+  <si>
+    <t>The system shows a list of users whose second names begin with "F".</t>
+  </si>
+  <si>
+    <t>The system shows a list of users whose role is manager.</t>
+  </si>
+  <si>
+    <t>System shows the list of users sorted in a descending order by the selected column.</t>
+  </si>
+  <si>
+    <t>System shows the list of users sorted in a ascending order by the selected column.</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1273,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1437,28 +1580,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1476,10 +1646,76 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1801,10 +2037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="10" ySplit="2" topLeftCell="K31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1823,21 +2062,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="110" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="117"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="126"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
@@ -1877,25 +2116,25 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="47.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="114" t="s">
+      <c r="G3" s="123" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="10" t="s">
@@ -1907,19 +2146,19 @@
       <c r="J3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="111" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="47.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="121"/>
+      <c r="A4" s="128"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="124"/>
       <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1929,19 +2168,19 @@
       <c r="J4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="114" t="s">
         <v>50</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="48" thickBot="1">
-      <c r="A5" s="116"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="115"/>
+      <c r="A5" s="125"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="130"/>
       <c r="H5" s="28" t="s">
         <v>38</v>
       </c>
@@ -2065,25 +2304,25 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="47.25">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="115" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="105" t="s">
+      <c r="E9" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="115" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="114" t="s">
+      <c r="G9" s="123" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -2101,13 +2340,13 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="48" thickBot="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="115"/>
+      <c r="A10" s="122"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="130"/>
       <c r="H10" s="29" t="s">
         <v>82</v>
       </c>
@@ -2195,25 +2434,25 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="47.25">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="115" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="105" t="s">
+      <c r="E13" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="105" t="s">
+      <c r="F13" s="115" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="114" t="s">
+      <c r="G13" s="123" t="s">
         <v>100</v>
       </c>
       <c r="H13" s="54" t="s">
@@ -2231,13 +2470,13 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="32.25" thickBot="1">
-      <c r="A14" s="116"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="115"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="130"/>
       <c r="H14" s="54" t="s">
         <v>104</v>
       </c>
@@ -2252,25 +2491,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="115" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="115" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="105" t="s">
+      <c r="E15" s="115" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="105" t="s">
+      <c r="F15" s="115" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="114" t="s">
+      <c r="G15" s="123" t="s">
         <v>136</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -2287,13 +2526,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A16" s="109"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106"/>
-      <c r="G16" s="121"/>
+      <c r="A16" s="120"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="45" t="s">
         <v>115</v>
       </c>
@@ -2308,13 +2547,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A17" s="109"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="121"/>
+      <c r="A17" s="120"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="124"/>
       <c r="H17" s="57" t="s">
         <v>116</v>
       </c>
@@ -2329,25 +2568,25 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="121" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="117" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="117" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="111" t="s">
+      <c r="D18" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="111" t="s">
+      <c r="E18" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="111" t="s">
+      <c r="F18" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="112" t="s">
+      <c r="G18" s="131" t="s">
         <v>140</v>
       </c>
       <c r="H18" s="65" t="s">
@@ -2364,13 +2603,13 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A19" s="110"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="113"/>
+      <c r="A19" s="122"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="132"/>
       <c r="H19" s="11" t="s">
         <v>141</v>
       </c>
@@ -2420,26 +2659,26 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="96.6" customHeight="1">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="119" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="115" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="105" t="s">
+      <c r="C21" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="105" t="s">
+      <c r="E21" s="115" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="105" t="s">
+      <c r="F21" s="115" t="s">
         <v>160</v>
       </c>
-      <c r="G21" s="105" t="s">
-        <v>188</v>
+      <c r="G21" s="115" t="s">
+        <v>187</v>
       </c>
       <c r="H21" s="65" t="s">
         <v>159</v>
@@ -2451,22 +2690,22 @@
         <v>164</v>
       </c>
       <c r="K21" s="82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="69" customHeight="1">
-      <c r="A22" s="109"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="106"/>
+      <c r="A22" s="120"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="116"/>
       <c r="H22" s="97" t="s">
         <v>161</v>
       </c>
       <c r="I22" s="80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J22" s="80" t="s">
         <v>165</v>
@@ -2476,126 +2715,126 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A23" s="109"/>
-      <c r="B23" s="106"/>
-      <c r="C23" s="106"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="106"/>
+      <c r="A23" s="120"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="116"/>
       <c r="H23" s="97" t="s">
         <v>162</v>
       </c>
       <c r="I23" s="80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J23" s="80" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K23" s="83" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="106"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="106"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
       <c r="H24" s="97" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I24" s="80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J24" s="80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K24" s="83" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
+      <c r="A25" s="120"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
       <c r="H25" s="97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I25" s="80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J25" s="80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K25" s="83" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A26" s="109"/>
-      <c r="B26" s="106"/>
-      <c r="C26" s="106"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106"/>
+      <c r="A26" s="120"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
       <c r="H26" s="97" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I26" s="80" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J26" s="80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K26" s="83" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A27" s="109"/>
-      <c r="B27" s="106"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
       <c r="H27" s="97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I27" s="80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J27" s="80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K27" s="83" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="99.75" customHeight="1" thickBot="1">
-      <c r="A28" s="110"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
+      <c r="A28" s="122"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="118"/>
       <c r="H28" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I28" s="81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J28" s="81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K28" s="84" t="s">
         <v>166</v>
@@ -2609,7 +2848,7 @@
         <v>168</v>
       </c>
       <c r="C29" s="67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D29" s="67" t="s">
         <v>12</v>
@@ -2636,7 +2875,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="87" customHeight="1" thickBot="1">
+    <row r="30" spans="1:11" ht="108" customHeight="1" thickBot="1">
       <c r="A30" s="70" t="s">
         <v>173</v>
       </c>
@@ -2644,7 +2883,7 @@
         <v>175</v>
       </c>
       <c r="C30" s="67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>12</v>
@@ -2656,7 +2895,7 @@
         <v>177</v>
       </c>
       <c r="G30" s="58" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>174</v>
@@ -2671,31 +2910,195 @@
         <v>180</v>
       </c>
     </row>
+    <row r="31" spans="1:11" ht="99" customHeight="1" thickBot="1">
+      <c r="A31" s="113" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="107" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="107" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="107" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="107" t="s">
+        <v>219</v>
+      </c>
+      <c r="G31" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="107" t="s">
+        <v>211</v>
+      </c>
+      <c r="J31" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="112" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="117.75" customHeight="1">
+      <c r="A32" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" s="115" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" s="115" t="s">
+        <v>216</v>
+      </c>
+      <c r="D32" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="115" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32" s="115" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="134" t="s">
+        <v>226</v>
+      </c>
+      <c r="H32" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="I32" s="105" t="s">
+        <v>235</v>
+      </c>
+      <c r="J32" s="105" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" s="111" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="87" customHeight="1">
+      <c r="A33" s="133"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="97" t="s">
+        <v>233</v>
+      </c>
+      <c r="I33" s="137" t="s">
+        <v>237</v>
+      </c>
+      <c r="J33" s="137" t="s">
+        <v>240</v>
+      </c>
+      <c r="K33" s="139" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="74.25" customHeight="1" thickBot="1">
+      <c r="A34" s="125"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="136"/>
+      <c r="H34" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I34" s="138" t="s">
+        <v>236</v>
+      </c>
+      <c r="J34" s="138" t="s">
+        <v>242</v>
+      </c>
+      <c r="K34" s="139" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="59.25" customHeight="1">
+      <c r="A35" s="119" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" s="115" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="115" t="s">
+        <v>217</v>
+      </c>
+      <c r="F35" s="115" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" s="131" t="s">
+        <v>244</v>
+      </c>
+      <c r="H35" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="I35" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="J35" s="105" t="s">
+        <v>227</v>
+      </c>
+      <c r="K35" s="111" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="59.25" customHeight="1" thickBot="1">
+      <c r="A36" s="122"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="132"/>
+      <c r="H36" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="I36" s="107" t="s">
+        <v>229</v>
+      </c>
+      <c r="J36" s="107" t="s">
+        <v>230</v>
+      </c>
+      <c r="K36" s="112" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
+  <mergeCells count="58">
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="G21:G28"/>
+    <mergeCell ref="F21:F28"/>
+    <mergeCell ref="E21:E28"/>
+    <mergeCell ref="D21:D28"/>
+    <mergeCell ref="C21:C28"/>
     <mergeCell ref="B21:B28"/>
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="F18:F19"/>
@@ -2712,11 +3115,29 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="G21:G28"/>
-    <mergeCell ref="F21:F28"/>
-    <mergeCell ref="E21:E28"/>
-    <mergeCell ref="D21:D28"/>
-    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2725,10 +3146,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B269C-A11B-41F2-B2B7-9B8EF1E55741}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3233,13 +3655,13 @@
         <v>159</v>
       </c>
       <c r="D20" s="75" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="68" t="s">
         <v>184</v>
       </c>
-      <c r="E20" s="68" t="s">
-        <v>185</v>
-      </c>
       <c r="F20" s="68" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G20" s="74" t="s">
         <v>63</v>
@@ -3259,7 +3681,7 @@
         <v>161</v>
       </c>
       <c r="D21" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E21" s="71" t="s">
         <v>139</v>
@@ -3284,7 +3706,7 @@
         <v>162</v>
       </c>
       <c r="D22" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E22" s="80" t="s">
         <v>166</v>
@@ -3306,10 +3728,10 @@
         <v>154</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D23" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E23" s="96" t="s">
         <v>166</v>
@@ -3331,10 +3753,10 @@
         <v>154</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D24" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E24" s="80" t="s">
         <v>166</v>
@@ -3356,10 +3778,10 @@
         <v>154</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E25" s="80" t="s">
         <v>166</v>
@@ -3381,10 +3803,10 @@
         <v>154</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E26" s="80" t="s">
         <v>166</v>
@@ -3406,10 +3828,10 @@
         <v>154</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E27" s="81" t="s">
         <v>166</v>
@@ -3431,16 +3853,16 @@
         <v>167</v>
       </c>
       <c r="C28" s="88" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="D28" s="89" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E28" s="99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F28" s="99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G28" s="88" t="s">
         <v>63</v>
@@ -3449,22 +3871,22 @@
       <c r="I28" s="90"/>
     </row>
     <row r="29" spans="1:12" ht="79.5" thickBot="1">
-      <c r="A29" s="73">
+      <c r="A29" s="87">
         <v>28</v>
       </c>
       <c r="B29" s="88" t="s">
         <v>173</v>
       </c>
       <c r="C29" s="88" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="D29" s="89" t="s">
-        <v>184</v>
-      </c>
-      <c r="E29" s="72" t="s">
+        <v>183</v>
+      </c>
+      <c r="E29" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="72" t="s">
+      <c r="F29" s="108" t="s">
         <v>180</v>
       </c>
       <c r="G29" s="88" t="s">
@@ -3472,6 +3894,1325 @@
       </c>
       <c r="H29" s="88"/>
       <c r="I29" s="90"/>
+    </row>
+    <row r="30" spans="1:12" ht="67.5" customHeight="1" thickBot="1">
+      <c r="A30" s="87">
+        <v>29</v>
+      </c>
+      <c r="B30" s="146" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="146" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="146" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="108" t="s">
+        <v>247</v>
+      </c>
+      <c r="F30" s="108" t="s">
+        <v>247</v>
+      </c>
+      <c r="G30" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="88"/>
+      <c r="I30" s="90"/>
+    </row>
+    <row r="31" spans="1:12" ht="54.75" customHeight="1">
+      <c r="A31" s="147">
+        <v>30</v>
+      </c>
+      <c r="B31" s="148" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="148" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" s="148" t="s">
+        <v>246</v>
+      </c>
+      <c r="E31" s="105" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31" s="105" t="s">
+        <v>248</v>
+      </c>
+      <c r="G31" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="148"/>
+      <c r="I31" s="109"/>
+    </row>
+    <row r="32" spans="1:12" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A32" s="149">
+        <v>31</v>
+      </c>
+      <c r="B32" s="150" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="150" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="150" t="s">
+        <v>246</v>
+      </c>
+      <c r="E32" s="138" t="s">
+        <v>249</v>
+      </c>
+      <c r="F32" s="138" t="s">
+        <v>249</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="150"/>
+      <c r="I32" s="110"/>
+    </row>
+    <row r="33" spans="1:9" ht="54.75" customHeight="1">
+      <c r="A33" s="151">
+        <v>32</v>
+      </c>
+      <c r="B33" s="148" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" s="148" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" s="148" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="152" t="s">
+        <v>250</v>
+      </c>
+      <c r="F33" s="152" t="s">
+        <v>250</v>
+      </c>
+      <c r="G33" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="148"/>
+      <c r="I33" s="109"/>
+    </row>
+    <row r="34" spans="1:9" ht="54.75" customHeight="1">
+      <c r="A34" s="142">
+        <v>33</v>
+      </c>
+      <c r="B34" s="141" t="s">
+        <v>225</v>
+      </c>
+      <c r="C34" s="141" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="141" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="F34" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="141"/>
+      <c r="I34" s="139"/>
+    </row>
+    <row r="35" spans="1:9" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A35" s="153">
+        <v>34</v>
+      </c>
+      <c r="B35" s="150" t="s">
+        <v>225</v>
+      </c>
+      <c r="C35" s="150" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" s="150" t="s">
+        <v>246</v>
+      </c>
+      <c r="E35" s="107" t="s">
+        <v>252</v>
+      </c>
+      <c r="F35" s="107" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="150"/>
+      <c r="I35" s="110"/>
+    </row>
+    <row r="36" spans="1:9" ht="29.25" customHeight="1">
+      <c r="A36" s="143">
+        <v>35</v>
+      </c>
+      <c r="E36" s="140"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="140"/>
+      <c r="I36" s="145"/>
+    </row>
+    <row r="37" spans="1:9" ht="29.25" customHeight="1">
+      <c r="A37" s="143">
+        <v>36</v>
+      </c>
+      <c r="B37" s="141"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="140"/>
+      <c r="F37" s="140"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="140"/>
+      <c r="I37" s="145"/>
+    </row>
+    <row r="38" spans="1:9" ht="29.25" customHeight="1">
+      <c r="A38" s="144">
+        <v>37</v>
+      </c>
+      <c r="B38" s="141"/>
+      <c r="C38" s="140"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="140"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="140"/>
+      <c r="I38" s="145"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75">
+      <c r="A39" s="141"/>
+      <c r="B39" s="141"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="140"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="140"/>
+      <c r="I39" s="145"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75">
+      <c r="A40" s="141"/>
+      <c r="B40" s="141"/>
+      <c r="C40" s="140"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="145"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75">
+      <c r="A41" s="141"/>
+      <c r="B41" s="141"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="140"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="140"/>
+      <c r="I41" s="145"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75">
+      <c r="A42" s="140"/>
+      <c r="B42" s="140"/>
+      <c r="C42" s="140"/>
+      <c r="D42" s="140"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="145"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75">
+      <c r="A43" s="140"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="140"/>
+      <c r="D43" s="140"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="140"/>
+      <c r="G43" s="140"/>
+      <c r="H43" s="140"/>
+      <c r="I43" s="145"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75">
+      <c r="A44" s="140"/>
+      <c r="B44" s="140"/>
+      <c r="C44" s="140"/>
+      <c r="D44" s="140"/>
+      <c r="E44" s="140"/>
+      <c r="F44" s="140"/>
+      <c r="G44" s="140"/>
+      <c r="H44" s="140"/>
+      <c r="I44" s="145"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75">
+      <c r="A45" s="140"/>
+      <c r="B45" s="140"/>
+      <c r="C45" s="140"/>
+      <c r="D45" s="140"/>
+      <c r="E45" s="140"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="140"/>
+      <c r="I45" s="145"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75">
+      <c r="A46" s="140"/>
+      <c r="B46" s="140"/>
+      <c r="C46" s="140"/>
+      <c r="D46" s="140"/>
+      <c r="E46" s="140"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="140"/>
+      <c r="H46" s="140"/>
+      <c r="I46" s="145"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75">
+      <c r="A47" s="140"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="140"/>
+      <c r="D47" s="140"/>
+      <c r="E47" s="140"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="140"/>
+      <c r="H47" s="140"/>
+      <c r="I47" s="145"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75">
+      <c r="A48" s="140"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="140"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="140"/>
+      <c r="I48" s="145"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75">
+      <c r="A49" s="140"/>
+      <c r="B49" s="140"/>
+      <c r="C49" s="140"/>
+      <c r="D49" s="140"/>
+      <c r="E49" s="140"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="140"/>
+      <c r="I49" s="145"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75">
+      <c r="A50" s="140"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="145"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75">
+      <c r="A51" s="140"/>
+      <c r="B51" s="140"/>
+      <c r="C51" s="140"/>
+      <c r="D51" s="140"/>
+      <c r="E51" s="140"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="140"/>
+      <c r="I51" s="145"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75">
+      <c r="A52" s="140"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="140"/>
+      <c r="D52" s="140"/>
+      <c r="E52" s="140"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="140"/>
+      <c r="I52" s="145"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75">
+      <c r="A53" s="140"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="140"/>
+      <c r="D53" s="140"/>
+      <c r="E53" s="140"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="140"/>
+      <c r="H53" s="140"/>
+      <c r="I53" s="145"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75">
+      <c r="A54" s="140"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="140"/>
+      <c r="D54" s="140"/>
+      <c r="E54" s="140"/>
+      <c r="F54" s="140"/>
+      <c r="G54" s="140"/>
+      <c r="H54" s="140"/>
+      <c r="I54" s="145"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75">
+      <c r="A55" s="140"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="140"/>
+      <c r="D55" s="140"/>
+      <c r="E55" s="140"/>
+      <c r="F55" s="140"/>
+      <c r="G55" s="140"/>
+      <c r="H55" s="140"/>
+      <c r="I55" s="145"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75">
+      <c r="A56" s="140"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="140"/>
+      <c r="D56" s="140"/>
+      <c r="E56" s="140"/>
+      <c r="F56" s="140"/>
+      <c r="G56" s="140"/>
+      <c r="H56" s="140"/>
+      <c r="I56" s="145"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75">
+      <c r="A57" s="140"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="140"/>
+      <c r="D57" s="140"/>
+      <c r="E57" s="140"/>
+      <c r="F57" s="140"/>
+      <c r="G57" s="140"/>
+      <c r="H57" s="140"/>
+      <c r="I57" s="145"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75">
+      <c r="A58" s="140"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="140"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="140"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="140"/>
+      <c r="I58" s="145"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75">
+      <c r="A59" s="140"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="140"/>
+      <c r="D59" s="140"/>
+      <c r="E59" s="140"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="140"/>
+      <c r="H59" s="140"/>
+      <c r="I59" s="145"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75">
+      <c r="A60" s="140"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="140"/>
+      <c r="D60" s="140"/>
+      <c r="E60" s="140"/>
+      <c r="F60" s="140"/>
+      <c r="G60" s="140"/>
+      <c r="H60" s="140"/>
+      <c r="I60" s="145"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75">
+      <c r="A61" s="140"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="140"/>
+      <c r="D61" s="140"/>
+      <c r="E61" s="140"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="140"/>
+      <c r="I61" s="145"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75">
+      <c r="A62" s="140"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="140"/>
+      <c r="D62" s="140"/>
+      <c r="E62" s="140"/>
+      <c r="F62" s="140"/>
+      <c r="G62" s="140"/>
+      <c r="H62" s="140"/>
+      <c r="I62" s="145"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75">
+      <c r="A63" s="140"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="140"/>
+      <c r="D63" s="140"/>
+      <c r="E63" s="140"/>
+      <c r="F63" s="140"/>
+      <c r="G63" s="140"/>
+      <c r="H63" s="140"/>
+      <c r="I63" s="145"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75">
+      <c r="A64" s="140"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="140"/>
+      <c r="D64" s="140"/>
+      <c r="E64" s="140"/>
+      <c r="F64" s="140"/>
+      <c r="G64" s="140"/>
+      <c r="H64" s="140"/>
+      <c r="I64" s="145"/>
+    </row>
+    <row r="65" spans="1:9" ht="15.75">
+      <c r="A65" s="140"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="140"/>
+      <c r="D65" s="140"/>
+      <c r="E65" s="140"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="140"/>
+      <c r="H65" s="140"/>
+      <c r="I65" s="145"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75">
+      <c r="A66" s="140"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="140"/>
+      <c r="D66" s="140"/>
+      <c r="E66" s="140"/>
+      <c r="F66" s="140"/>
+      <c r="G66" s="140"/>
+      <c r="H66" s="140"/>
+      <c r="I66" s="145"/>
+    </row>
+    <row r="67" spans="1:9" ht="15.75">
+      <c r="A67" s="140"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="140"/>
+      <c r="D67" s="140"/>
+      <c r="E67" s="140"/>
+      <c r="F67" s="140"/>
+      <c r="G67" s="140"/>
+      <c r="H67" s="140"/>
+      <c r="I67" s="145"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75">
+      <c r="A68" s="140"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="140"/>
+      <c r="D68" s="140"/>
+      <c r="E68" s="140"/>
+      <c r="F68" s="140"/>
+      <c r="G68" s="140"/>
+      <c r="H68" s="140"/>
+      <c r="I68" s="145"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75">
+      <c r="A69" s="140"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="140"/>
+      <c r="D69" s="140"/>
+      <c r="E69" s="140"/>
+      <c r="F69" s="140"/>
+      <c r="G69" s="140"/>
+      <c r="H69" s="140"/>
+      <c r="I69" s="145"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75">
+      <c r="A70" s="140"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="140"/>
+      <c r="D70" s="140"/>
+      <c r="E70" s="140"/>
+      <c r="F70" s="140"/>
+      <c r="G70" s="140"/>
+      <c r="H70" s="140"/>
+      <c r="I70" s="145"/>
+    </row>
+    <row r="71" spans="1:9" ht="15.75">
+      <c r="A71" s="140"/>
+      <c r="B71" s="140"/>
+      <c r="C71" s="140"/>
+      <c r="D71" s="140"/>
+      <c r="E71" s="140"/>
+      <c r="F71" s="140"/>
+      <c r="G71" s="140"/>
+      <c r="H71" s="140"/>
+      <c r="I71" s="145"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75">
+      <c r="A72" s="140"/>
+      <c r="B72" s="140"/>
+      <c r="C72" s="140"/>
+      <c r="D72" s="140"/>
+      <c r="E72" s="140"/>
+      <c r="F72" s="140"/>
+      <c r="G72" s="140"/>
+      <c r="H72" s="140"/>
+      <c r="I72" s="145"/>
+    </row>
+    <row r="73" spans="1:9" ht="15.75">
+      <c r="A73" s="140"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="140"/>
+      <c r="D73" s="140"/>
+      <c r="E73" s="140"/>
+      <c r="F73" s="140"/>
+      <c r="G73" s="140"/>
+      <c r="H73" s="140"/>
+      <c r="I73" s="145"/>
+    </row>
+    <row r="74" spans="1:9" ht="15.75">
+      <c r="A74" s="140"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="140"/>
+      <c r="D74" s="140"/>
+      <c r="E74" s="140"/>
+      <c r="F74" s="140"/>
+      <c r="G74" s="140"/>
+      <c r="H74" s="140"/>
+      <c r="I74" s="145"/>
+    </row>
+    <row r="75" spans="1:9" ht="15.75">
+      <c r="A75" s="140"/>
+      <c r="B75" s="140"/>
+      <c r="C75" s="140"/>
+      <c r="D75" s="140"/>
+      <c r="E75" s="140"/>
+      <c r="F75" s="140"/>
+      <c r="G75" s="140"/>
+      <c r="H75" s="140"/>
+      <c r="I75" s="145"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75">
+      <c r="A76" s="140"/>
+      <c r="B76" s="140"/>
+      <c r="C76" s="140"/>
+      <c r="D76" s="140"/>
+      <c r="E76" s="140"/>
+      <c r="F76" s="140"/>
+      <c r="G76" s="140"/>
+      <c r="H76" s="140"/>
+      <c r="I76" s="145"/>
+    </row>
+    <row r="77" spans="1:9" ht="15.75">
+      <c r="A77" s="140"/>
+      <c r="B77" s="140"/>
+      <c r="C77" s="140"/>
+      <c r="D77" s="140"/>
+      <c r="E77" s="140"/>
+      <c r="F77" s="140"/>
+      <c r="G77" s="140"/>
+      <c r="H77" s="140"/>
+      <c r="I77" s="145"/>
+    </row>
+    <row r="78" spans="1:9" ht="15.75">
+      <c r="A78" s="140"/>
+      <c r="B78" s="140"/>
+      <c r="C78" s="140"/>
+      <c r="D78" s="140"/>
+      <c r="E78" s="140"/>
+      <c r="F78" s="140"/>
+      <c r="G78" s="140"/>
+      <c r="H78" s="140"/>
+      <c r="I78" s="145"/>
+    </row>
+    <row r="79" spans="1:9" ht="15.75">
+      <c r="A79" s="140"/>
+      <c r="B79" s="140"/>
+      <c r="C79" s="140"/>
+      <c r="D79" s="140"/>
+      <c r="E79" s="140"/>
+      <c r="F79" s="140"/>
+      <c r="G79" s="140"/>
+      <c r="H79" s="140"/>
+      <c r="I79" s="145"/>
+    </row>
+    <row r="80" spans="1:9" ht="15.75">
+      <c r="A80" s="140"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="140"/>
+      <c r="D80" s="140"/>
+      <c r="E80" s="140"/>
+      <c r="F80" s="140"/>
+      <c r="G80" s="140"/>
+      <c r="H80" s="140"/>
+      <c r="I80" s="145"/>
+    </row>
+    <row r="81" spans="1:9" ht="15.75">
+      <c r="A81" s="140"/>
+      <c r="B81" s="140"/>
+      <c r="C81" s="140"/>
+      <c r="D81" s="140"/>
+      <c r="E81" s="140"/>
+      <c r="F81" s="140"/>
+      <c r="G81" s="140"/>
+      <c r="H81" s="140"/>
+      <c r="I81" s="145"/>
+    </row>
+    <row r="82" spans="1:9" ht="15.75">
+      <c r="A82" s="140"/>
+      <c r="B82" s="140"/>
+      <c r="C82" s="140"/>
+      <c r="D82" s="140"/>
+      <c r="E82" s="140"/>
+      <c r="F82" s="140"/>
+      <c r="G82" s="140"/>
+      <c r="H82" s="140"/>
+      <c r="I82" s="145"/>
+    </row>
+    <row r="83" spans="1:9" ht="15.75">
+      <c r="A83" s="140"/>
+      <c r="B83" s="140"/>
+      <c r="C83" s="140"/>
+      <c r="D83" s="140"/>
+      <c r="E83" s="140"/>
+      <c r="F83" s="140"/>
+      <c r="G83" s="140"/>
+      <c r="H83" s="140"/>
+      <c r="I83" s="145"/>
+    </row>
+    <row r="84" spans="1:9" ht="15.75">
+      <c r="A84" s="140"/>
+      <c r="B84" s="140"/>
+      <c r="C84" s="140"/>
+      <c r="D84" s="140"/>
+      <c r="E84" s="140"/>
+      <c r="F84" s="140"/>
+      <c r="G84" s="140"/>
+      <c r="H84" s="140"/>
+      <c r="I84" s="145"/>
+    </row>
+    <row r="85" spans="1:9" ht="15.75">
+      <c r="A85" s="140"/>
+      <c r="B85" s="140"/>
+      <c r="C85" s="140"/>
+      <c r="D85" s="140"/>
+      <c r="E85" s="140"/>
+      <c r="F85" s="140"/>
+      <c r="G85" s="140"/>
+      <c r="H85" s="140"/>
+      <c r="I85" s="145"/>
+    </row>
+    <row r="86" spans="1:9" ht="15.75">
+      <c r="A86" s="140"/>
+      <c r="B86" s="140"/>
+      <c r="C86" s="140"/>
+      <c r="D86" s="140"/>
+      <c r="E86" s="140"/>
+      <c r="F86" s="140"/>
+      <c r="G86" s="140"/>
+      <c r="H86" s="140"/>
+      <c r="I86" s="145"/>
+    </row>
+    <row r="87" spans="1:9" ht="15.75">
+      <c r="A87" s="140"/>
+      <c r="B87" s="140"/>
+      <c r="C87" s="140"/>
+      <c r="D87" s="140"/>
+      <c r="E87" s="140"/>
+      <c r="F87" s="140"/>
+      <c r="G87" s="140"/>
+      <c r="H87" s="140"/>
+      <c r="I87" s="145"/>
+    </row>
+    <row r="88" spans="1:9" ht="15.75">
+      <c r="A88" s="140"/>
+      <c r="B88" s="140"/>
+      <c r="C88" s="140"/>
+      <c r="D88" s="140"/>
+      <c r="E88" s="140"/>
+      <c r="F88" s="140"/>
+      <c r="G88" s="140"/>
+      <c r="H88" s="140"/>
+      <c r="I88" s="145"/>
+    </row>
+    <row r="89" spans="1:9" ht="15.75">
+      <c r="A89" s="140"/>
+      <c r="B89" s="140"/>
+      <c r="C89" s="140"/>
+      <c r="D89" s="140"/>
+      <c r="E89" s="140"/>
+      <c r="F89" s="140"/>
+      <c r="G89" s="140"/>
+      <c r="H89" s="140"/>
+      <c r="I89" s="145"/>
+    </row>
+    <row r="90" spans="1:9" ht="15.75">
+      <c r="A90" s="140"/>
+      <c r="B90" s="140"/>
+      <c r="C90" s="140"/>
+      <c r="D90" s="140"/>
+      <c r="E90" s="140"/>
+      <c r="F90" s="140"/>
+      <c r="G90" s="140"/>
+      <c r="H90" s="140"/>
+      <c r="I90" s="145"/>
+    </row>
+    <row r="91" spans="1:9" ht="15.75">
+      <c r="A91" s="140"/>
+      <c r="B91" s="140"/>
+      <c r="C91" s="140"/>
+      <c r="D91" s="140"/>
+      <c r="E91" s="140"/>
+      <c r="F91" s="140"/>
+      <c r="G91" s="140"/>
+      <c r="H91" s="140"/>
+      <c r="I91" s="145"/>
+    </row>
+    <row r="92" spans="1:9" ht="15.75">
+      <c r="A92" s="140"/>
+      <c r="B92" s="140"/>
+      <c r="C92" s="140"/>
+      <c r="D92" s="140"/>
+      <c r="E92" s="140"/>
+      <c r="F92" s="140"/>
+      <c r="G92" s="140"/>
+      <c r="H92" s="140"/>
+      <c r="I92" s="145"/>
+    </row>
+    <row r="93" spans="1:9" ht="15.75">
+      <c r="A93" s="140"/>
+      <c r="B93" s="140"/>
+      <c r="C93" s="140"/>
+      <c r="D93" s="140"/>
+      <c r="E93" s="140"/>
+      <c r="F93" s="140"/>
+      <c r="G93" s="140"/>
+      <c r="H93" s="140"/>
+      <c r="I93" s="145"/>
+    </row>
+    <row r="94" spans="1:9" ht="15.75">
+      <c r="A94" s="140"/>
+      <c r="B94" s="140"/>
+      <c r="C94" s="140"/>
+      <c r="D94" s="140"/>
+      <c r="E94" s="140"/>
+      <c r="F94" s="140"/>
+      <c r="G94" s="140"/>
+      <c r="H94" s="140"/>
+      <c r="I94" s="145"/>
+    </row>
+    <row r="95" spans="1:9" ht="15.75">
+      <c r="A95" s="140"/>
+      <c r="B95" s="140"/>
+      <c r="C95" s="140"/>
+      <c r="D95" s="140"/>
+      <c r="E95" s="140"/>
+      <c r="F95" s="140"/>
+      <c r="G95" s="140"/>
+      <c r="H95" s="140"/>
+      <c r="I95" s="145"/>
+    </row>
+    <row r="96" spans="1:9" ht="15.75">
+      <c r="A96" s="140"/>
+      <c r="B96" s="140"/>
+      <c r="C96" s="140"/>
+      <c r="D96" s="140"/>
+      <c r="E96" s="140"/>
+      <c r="F96" s="140"/>
+      <c r="G96" s="140"/>
+      <c r="H96" s="140"/>
+      <c r="I96" s="145"/>
+    </row>
+    <row r="97" spans="1:9" ht="15.75">
+      <c r="A97" s="140"/>
+      <c r="B97" s="140"/>
+      <c r="C97" s="140"/>
+      <c r="D97" s="140"/>
+      <c r="E97" s="140"/>
+      <c r="F97" s="140"/>
+      <c r="G97" s="140"/>
+      <c r="H97" s="140"/>
+      <c r="I97" s="145"/>
+    </row>
+    <row r="98" spans="1:9" ht="15.75">
+      <c r="A98" s="140"/>
+      <c r="B98" s="140"/>
+      <c r="C98" s="140"/>
+      <c r="D98" s="140"/>
+      <c r="E98" s="140"/>
+      <c r="F98" s="140"/>
+      <c r="G98" s="140"/>
+      <c r="H98" s="140"/>
+      <c r="I98" s="145"/>
+    </row>
+    <row r="99" spans="1:9" ht="15.75">
+      <c r="A99" s="140"/>
+      <c r="B99" s="140"/>
+      <c r="C99" s="140"/>
+      <c r="D99" s="140"/>
+      <c r="E99" s="140"/>
+      <c r="F99" s="140"/>
+      <c r="G99" s="140"/>
+      <c r="H99" s="140"/>
+      <c r="I99" s="145"/>
+    </row>
+    <row r="100" spans="1:9" ht="15.75">
+      <c r="A100" s="140"/>
+      <c r="B100" s="140"/>
+      <c r="C100" s="140"/>
+      <c r="D100" s="140"/>
+      <c r="E100" s="140"/>
+      <c r="F100" s="140"/>
+      <c r="G100" s="140"/>
+      <c r="H100" s="140"/>
+      <c r="I100" s="145"/>
+    </row>
+    <row r="101" spans="1:9" ht="15.75">
+      <c r="A101" s="140"/>
+      <c r="B101" s="140"/>
+      <c r="C101" s="140"/>
+      <c r="D101" s="140"/>
+      <c r="E101" s="140"/>
+      <c r="F101" s="140"/>
+      <c r="G101" s="140"/>
+      <c r="H101" s="140"/>
+      <c r="I101" s="145"/>
+    </row>
+    <row r="102" spans="1:9" ht="15.75">
+      <c r="A102" s="140"/>
+      <c r="B102" s="140"/>
+      <c r="C102" s="140"/>
+      <c r="D102" s="140"/>
+      <c r="E102" s="140"/>
+      <c r="F102" s="140"/>
+      <c r="G102" s="140"/>
+      <c r="H102" s="140"/>
+      <c r="I102" s="145"/>
+    </row>
+    <row r="103" spans="1:9" ht="15.75">
+      <c r="A103" s="140"/>
+      <c r="B103" s="140"/>
+      <c r="C103" s="140"/>
+      <c r="D103" s="140"/>
+      <c r="E103" s="140"/>
+      <c r="F103" s="140"/>
+      <c r="G103" s="140"/>
+      <c r="H103" s="140"/>
+      <c r="I103" s="145"/>
+    </row>
+    <row r="104" spans="1:9" ht="15.75">
+      <c r="A104" s="140"/>
+      <c r="B104" s="140"/>
+      <c r="C104" s="140"/>
+      <c r="D104" s="140"/>
+      <c r="E104" s="140"/>
+      <c r="F104" s="140"/>
+      <c r="G104" s="140"/>
+      <c r="H104" s="140"/>
+      <c r="I104" s="145"/>
+    </row>
+    <row r="105" spans="1:9" ht="15.75">
+      <c r="A105" s="140"/>
+      <c r="B105" s="140"/>
+      <c r="C105" s="140"/>
+      <c r="D105" s="140"/>
+      <c r="E105" s="140"/>
+      <c r="F105" s="140"/>
+      <c r="G105" s="140"/>
+      <c r="H105" s="140"/>
+      <c r="I105" s="145"/>
+    </row>
+    <row r="106" spans="1:9" ht="15.75">
+      <c r="A106" s="140"/>
+      <c r="B106" s="140"/>
+      <c r="C106" s="140"/>
+      <c r="D106" s="140"/>
+      <c r="E106" s="140"/>
+      <c r="F106" s="140"/>
+      <c r="G106" s="140"/>
+      <c r="H106" s="140"/>
+      <c r="I106" s="145"/>
+    </row>
+    <row r="107" spans="1:9" ht="15.75">
+      <c r="A107" s="140"/>
+      <c r="B107" s="140"/>
+      <c r="C107" s="140"/>
+      <c r="D107" s="140"/>
+      <c r="E107" s="140"/>
+      <c r="F107" s="140"/>
+      <c r="G107" s="140"/>
+      <c r="H107" s="140"/>
+      <c r="I107" s="145"/>
+    </row>
+    <row r="108" spans="1:9" ht="15.75">
+      <c r="A108" s="140"/>
+      <c r="B108" s="140"/>
+      <c r="C108" s="140"/>
+      <c r="D108" s="140"/>
+      <c r="E108" s="140"/>
+      <c r="F108" s="140"/>
+      <c r="G108" s="140"/>
+      <c r="H108" s="140"/>
+      <c r="I108" s="145"/>
+    </row>
+    <row r="109" spans="1:9" ht="15.75">
+      <c r="A109" s="140"/>
+      <c r="B109" s="140"/>
+      <c r="C109" s="140"/>
+      <c r="D109" s="140"/>
+      <c r="E109" s="140"/>
+      <c r="F109" s="140"/>
+      <c r="G109" s="140"/>
+      <c r="H109" s="140"/>
+      <c r="I109" s="145"/>
+    </row>
+    <row r="110" spans="1:9" ht="15.75">
+      <c r="A110" s="140"/>
+      <c r="B110" s="140"/>
+      <c r="C110" s="140"/>
+      <c r="D110" s="140"/>
+      <c r="E110" s="140"/>
+      <c r="F110" s="140"/>
+      <c r="G110" s="140"/>
+      <c r="H110" s="140"/>
+      <c r="I110" s="145"/>
+    </row>
+    <row r="111" spans="1:9" ht="15.75">
+      <c r="A111" s="140"/>
+      <c r="B111" s="140"/>
+      <c r="C111" s="140"/>
+      <c r="D111" s="140"/>
+      <c r="E111" s="140"/>
+      <c r="F111" s="140"/>
+      <c r="G111" s="140"/>
+      <c r="H111" s="140"/>
+      <c r="I111" s="145"/>
+    </row>
+    <row r="112" spans="1:9" ht="15.75">
+      <c r="A112" s="140"/>
+      <c r="B112" s="140"/>
+      <c r="C112" s="140"/>
+      <c r="D112" s="140"/>
+      <c r="E112" s="140"/>
+      <c r="F112" s="140"/>
+      <c r="G112" s="140"/>
+      <c r="H112" s="140"/>
+      <c r="I112" s="145"/>
+    </row>
+    <row r="113" spans="1:9" ht="15.75">
+      <c r="A113" s="140"/>
+      <c r="B113" s="140"/>
+      <c r="C113" s="140"/>
+      <c r="D113" s="140"/>
+      <c r="E113" s="140"/>
+      <c r="F113" s="140"/>
+      <c r="G113" s="140"/>
+      <c r="H113" s="140"/>
+      <c r="I113" s="145"/>
+    </row>
+    <row r="114" spans="1:9" ht="15.75">
+      <c r="A114" s="140"/>
+      <c r="B114" s="140"/>
+      <c r="C114" s="140"/>
+      <c r="D114" s="140"/>
+      <c r="E114" s="140"/>
+      <c r="F114" s="140"/>
+      <c r="G114" s="140"/>
+      <c r="H114" s="140"/>
+      <c r="I114" s="145"/>
+    </row>
+    <row r="115" spans="1:9" ht="15.75">
+      <c r="A115" s="140"/>
+      <c r="B115" s="140"/>
+      <c r="C115" s="140"/>
+      <c r="D115" s="140"/>
+      <c r="E115" s="140"/>
+      <c r="F115" s="140"/>
+      <c r="G115" s="140"/>
+      <c r="H115" s="140"/>
+      <c r="I115" s="145"/>
+    </row>
+    <row r="116" spans="1:9" ht="15.75">
+      <c r="A116" s="140"/>
+      <c r="B116" s="140"/>
+      <c r="C116" s="140"/>
+      <c r="D116" s="140"/>
+      <c r="E116" s="140"/>
+      <c r="F116" s="140"/>
+      <c r="G116" s="140"/>
+      <c r="H116" s="140"/>
+      <c r="I116" s="145"/>
+    </row>
+    <row r="117" spans="1:9" ht="15.75">
+      <c r="A117" s="140"/>
+      <c r="B117" s="140"/>
+      <c r="C117" s="140"/>
+      <c r="D117" s="140"/>
+      <c r="E117" s="140"/>
+      <c r="F117" s="140"/>
+      <c r="G117" s="140"/>
+      <c r="H117" s="140"/>
+      <c r="I117" s="145"/>
+    </row>
+    <row r="118" spans="1:9" ht="15.75">
+      <c r="A118" s="140"/>
+      <c r="B118" s="140"/>
+      <c r="C118" s="140"/>
+      <c r="D118" s="140"/>
+      <c r="E118" s="140"/>
+      <c r="F118" s="140"/>
+      <c r="G118" s="140"/>
+      <c r="H118" s="140"/>
+      <c r="I118" s="145"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.75">
+      <c r="A119" s="140"/>
+      <c r="B119" s="140"/>
+      <c r="C119" s="140"/>
+      <c r="D119" s="140"/>
+      <c r="E119" s="140"/>
+      <c r="F119" s="140"/>
+      <c r="G119" s="140"/>
+      <c r="H119" s="140"/>
+      <c r="I119" s="145"/>
+    </row>
+    <row r="120" spans="1:9" ht="15.75">
+      <c r="A120" s="140"/>
+      <c r="B120" s="140"/>
+      <c r="C120" s="140"/>
+      <c r="D120" s="140"/>
+      <c r="E120" s="140"/>
+      <c r="F120" s="140"/>
+      <c r="G120" s="140"/>
+      <c r="H120" s="140"/>
+      <c r="I120" s="145"/>
+    </row>
+    <row r="121" spans="1:9" ht="15.75">
+      <c r="A121" s="140"/>
+      <c r="B121" s="140"/>
+      <c r="C121" s="140"/>
+      <c r="D121" s="140"/>
+      <c r="E121" s="140"/>
+      <c r="F121" s="140"/>
+      <c r="G121" s="140"/>
+      <c r="H121" s="140"/>
+      <c r="I121" s="145"/>
+    </row>
+    <row r="122" spans="1:9" ht="15.75">
+      <c r="A122" s="140"/>
+      <c r="B122" s="140"/>
+      <c r="C122" s="140"/>
+      <c r="D122" s="140"/>
+      <c r="E122" s="140"/>
+      <c r="F122" s="140"/>
+      <c r="G122" s="140"/>
+      <c r="H122" s="140"/>
+      <c r="I122" s="145"/>
+    </row>
+    <row r="123" spans="1:9" ht="15.75">
+      <c r="A123" s="140"/>
+      <c r="B123" s="140"/>
+      <c r="C123" s="140"/>
+      <c r="D123" s="140"/>
+      <c r="E123" s="140"/>
+      <c r="F123" s="140"/>
+      <c r="G123" s="140"/>
+      <c r="H123" s="140"/>
+      <c r="I123" s="145"/>
+    </row>
+    <row r="124" spans="1:9" ht="15.75">
+      <c r="A124" s="140"/>
+      <c r="B124" s="140"/>
+      <c r="C124" s="140"/>
+      <c r="D124" s="140"/>
+      <c r="E124" s="140"/>
+      <c r="F124" s="140"/>
+      <c r="G124" s="140"/>
+      <c r="H124" s="140"/>
+      <c r="I124" s="145"/>
+    </row>
+    <row r="125" spans="1:9" ht="15.75">
+      <c r="A125" s="140"/>
+      <c r="B125" s="140"/>
+      <c r="C125" s="140"/>
+      <c r="D125" s="140"/>
+      <c r="E125" s="140"/>
+      <c r="F125" s="140"/>
+      <c r="G125" s="140"/>
+      <c r="H125" s="140"/>
+      <c r="I125" s="145"/>
+    </row>
+    <row r="126" spans="1:9" ht="15.75">
+      <c r="A126" s="140"/>
+      <c r="B126" s="140"/>
+      <c r="C126" s="140"/>
+      <c r="D126" s="140"/>
+      <c r="E126" s="140"/>
+      <c r="F126" s="140"/>
+      <c r="G126" s="140"/>
+      <c r="H126" s="140"/>
+      <c r="I126" s="145"/>
+    </row>
+    <row r="127" spans="1:9" ht="15.75">
+      <c r="A127" s="140"/>
+      <c r="B127" s="140"/>
+      <c r="C127" s="140"/>
+      <c r="D127" s="140"/>
+      <c r="E127" s="140"/>
+      <c r="F127" s="140"/>
+      <c r="G127" s="140"/>
+      <c r="H127" s="140"/>
+      <c r="I127" s="145"/>
+    </row>
+    <row r="128" spans="1:9" ht="15.75">
+      <c r="A128" s="140"/>
+      <c r="B128" s="140"/>
+      <c r="C128" s="140"/>
+      <c r="D128" s="140"/>
+      <c r="E128" s="140"/>
+      <c r="F128" s="140"/>
+      <c r="G128" s="140"/>
+      <c r="H128" s="140"/>
+      <c r="I128" s="145"/>
+    </row>
+    <row r="129" spans="1:9" ht="15.75">
+      <c r="A129" s="140"/>
+      <c r="B129" s="140"/>
+      <c r="C129" s="140"/>
+      <c r="D129" s="140"/>
+      <c r="E129" s="140"/>
+      <c r="F129" s="140"/>
+      <c r="G129" s="140"/>
+      <c r="H129" s="140"/>
+      <c r="I129" s="145"/>
+    </row>
+    <row r="130" spans="1:9" ht="15.75">
+      <c r="A130" s="140"/>
+      <c r="B130" s="140"/>
+      <c r="C130" s="140"/>
+      <c r="D130" s="140"/>
+      <c r="E130" s="140"/>
+      <c r="F130" s="140"/>
+      <c r="G130" s="140"/>
+      <c r="H130" s="140"/>
+      <c r="I130" s="145"/>
+    </row>
+    <row r="131" spans="1:9" ht="15.75">
+      <c r="A131" s="140"/>
+      <c r="B131" s="140"/>
+      <c r="C131" s="140"/>
+      <c r="D131" s="140"/>
+      <c r="E131" s="140"/>
+      <c r="F131" s="140"/>
+      <c r="G131" s="140"/>
+      <c r="H131" s="140"/>
+      <c r="I131" s="145"/>
+    </row>
+    <row r="132" spans="1:9" ht="15.75">
+      <c r="A132" s="140"/>
+      <c r="B132" s="140"/>
+      <c r="C132" s="140"/>
+      <c r="D132" s="140"/>
+      <c r="E132" s="140"/>
+      <c r="F132" s="140"/>
+      <c r="G132" s="140"/>
+      <c r="H132" s="140"/>
+      <c r="I132" s="145"/>
+    </row>
+    <row r="133" spans="1:9" ht="15.75">
+      <c r="A133" s="140"/>
+      <c r="B133" s="140"/>
+      <c r="C133" s="140"/>
+      <c r="D133" s="140"/>
+      <c r="E133" s="140"/>
+      <c r="F133" s="140"/>
+      <c r="G133" s="140"/>
+      <c r="H133" s="140"/>
+      <c r="I133" s="145"/>
+    </row>
+    <row r="134" spans="1:9" ht="15.75">
+      <c r="A134" s="140"/>
+      <c r="B134" s="140"/>
+      <c r="C134" s="140"/>
+      <c r="D134" s="140"/>
+      <c r="E134" s="140"/>
+      <c r="F134" s="140"/>
+      <c r="G134" s="140"/>
+      <c r="H134" s="140"/>
+      <c r="I134" s="145"/>
+    </row>
+    <row r="135" spans="1:9" ht="15.75">
+      <c r="A135" s="140"/>
+      <c r="B135" s="140"/>
+      <c r="C135" s="140"/>
+      <c r="D135" s="140"/>
+      <c r="E135" s="140"/>
+      <c r="F135" s="140"/>
+      <c r="G135" s="140"/>
+      <c r="H135" s="140"/>
+      <c r="I135" s="145"/>
+    </row>
+    <row r="136" spans="1:9" ht="15.75">
+      <c r="A136" s="140"/>
+      <c r="B136" s="140"/>
+      <c r="C136" s="140"/>
+      <c r="D136" s="140"/>
+      <c r="E136" s="140"/>
+      <c r="F136" s="140"/>
+      <c r="G136" s="140"/>
+      <c r="H136" s="140"/>
+      <c r="I136" s="145"/>
+    </row>
+    <row r="137" spans="1:9" ht="15.75">
+      <c r="A137" s="140"/>
+      <c r="B137" s="140"/>
+      <c r="C137" s="140"/>
+      <c r="D137" s="140"/>
+      <c r="E137" s="140"/>
+      <c r="F137" s="140"/>
+      <c r="G137" s="140"/>
+      <c r="H137" s="140"/>
+      <c r="I137" s="145"/>
+    </row>
+    <row r="138" spans="1:9" ht="15.75">
+      <c r="A138" s="140"/>
+      <c r="B138" s="140"/>
+      <c r="C138" s="140"/>
+      <c r="D138" s="140"/>
+      <c r="E138" s="140"/>
+      <c r="F138" s="140"/>
+      <c r="G138" s="140"/>
+      <c r="H138" s="140"/>
+      <c r="I138" s="145"/>
+    </row>
+    <row r="139" spans="1:9" ht="15.75">
+      <c r="A139" s="140"/>
+      <c r="B139" s="140"/>
+      <c r="C139" s="140"/>
+      <c r="D139" s="140"/>
+      <c r="E139" s="140"/>
+      <c r="F139" s="140"/>
+      <c r="G139" s="140"/>
+      <c r="H139" s="140"/>
+      <c r="I139" s="145"/>
+    </row>
+    <row r="140" spans="1:9" ht="15.75">
+      <c r="A140" s="140"/>
+      <c r="B140" s="140"/>
+      <c r="C140" s="140"/>
+      <c r="D140" s="140"/>
+      <c r="E140" s="140"/>
+      <c r="F140" s="140"/>
+      <c r="G140" s="140"/>
+      <c r="H140" s="140"/>
+      <c r="I140" s="145"/>
+    </row>
+    <row r="141" spans="1:9" ht="15.75">
+      <c r="A141" s="140"/>
+      <c r="B141" s="140"/>
+      <c r="C141" s="140"/>
+      <c r="D141" s="140"/>
+      <c r="E141" s="140"/>
+      <c r="F141" s="140"/>
+      <c r="G141" s="140"/>
+      <c r="H141" s="140"/>
+      <c r="I141" s="140"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Functional Tests - System administration module.xlsx - added two cases after presenting the unit tests
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\Testowanie 12.05.2022\Documents\System administration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59772632-4CE5-4946-A3A1-E1DCCBA53DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C8F08D-4E3E-4091-99F1-DA9C9ABD815D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="258">
   <si>
     <t>Test scenario</t>
   </si>
@@ -592,12 +592,6 @@
   </si>
   <si>
     <t>1. New password: 
-123zaq1@WSX
-2. Confirm password:
-123zaq1@WSX</t>
-  </si>
-  <si>
-    <t>1. New password: 
 123
 2. Confirm password:
 1234</t>
@@ -902,6 +896,28 @@
 qwertyuiopasdfgh
 2. Confirm password:
 qwertyuiopasdfgh</t>
+  </si>
+  <si>
+    <t>PAS_01.04</t>
+  </si>
+  <si>
+    <t>1. Login: LMartin8096
+2. E-mail: lmartin@@eksoc.com</t>
+  </si>
+  <si>
+    <t>PAS_04.09</t>
+  </si>
+  <si>
+    <t>1. New password: 
+zaq1@WSX
+2. Confirm password:
+zaq1@WSX</t>
+  </si>
+  <si>
+    <t>1. New password: 
+123zaq1@WSX4567
+2. Confirm password:
+123zaq1@WSX4567</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1293,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1443,9 +1459,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1507,22 +1520,10 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1599,62 +1600,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1674,13 +1699,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1689,19 +1711,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1715,12 +1731,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2041,13 +2051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K31" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2066,20 +2073,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
       <c r="G1" s="149"/>
-      <c r="H1" s="142" t="s">
+      <c r="H1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
       <c r="K1" s="149"/>
       <c r="L1" s="1"/>
     </row>
@@ -2120,25 +2127,25 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="47.25">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="C3" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="132" t="s">
+      <c r="E3" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="147" t="s">
+      <c r="G3" s="146" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="10" t="s">
@@ -2150,7 +2157,7 @@
       <c r="J3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="111" t="s">
+      <c r="K3" s="106" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="1"/>
@@ -2162,7 +2169,7 @@
       <c r="D4" s="151"/>
       <c r="E4" s="151"/>
       <c r="F4" s="151"/>
-      <c r="G4" s="152"/>
+      <c r="G4" s="147"/>
       <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
@@ -2172,18 +2179,18 @@
       <c r="J4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="114" t="s">
+      <c r="K4" s="108" t="s">
         <v>50</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="48" thickBot="1">
-      <c r="A5" s="137"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
+      <c r="A5" s="140"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
       <c r="G5" s="148"/>
       <c r="H5" s="28" t="s">
         <v>38</v>
@@ -2308,25 +2315,25 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="47.25">
-      <c r="A9" s="141" t="s">
+      <c r="A9" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="132" t="s">
+      <c r="B9" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D9" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="132" t="s">
+      <c r="E9" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="132" t="s">
+      <c r="F9" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="147" t="s">
+      <c r="G9" s="146" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -2344,12 +2351,12 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="48" thickBot="1">
-      <c r="A10" s="142"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="137"/>
+      <c r="C10" s="137"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="137"/>
       <c r="G10" s="148"/>
       <c r="H10" s="29" t="s">
         <v>82</v>
@@ -2438,25 +2445,25 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="47.25">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="132" t="s">
+      <c r="B13" s="135" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="135" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="132" t="s">
+      <c r="D13" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="132" t="s">
+      <c r="E13" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="132" t="s">
+      <c r="F13" s="135" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="147" t="s">
+      <c r="G13" s="146" t="s">
         <v>100</v>
       </c>
       <c r="H13" s="54" t="s">
@@ -2474,12 +2481,12 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="32.25" thickBot="1">
-      <c r="A14" s="137"/>
-      <c r="B14" s="133"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="137"/>
       <c r="G14" s="148"/>
       <c r="H14" s="54" t="s">
         <v>104</v>
@@ -2495,25 +2502,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A15" s="141" t="s">
+      <c r="A15" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="132" t="s">
+      <c r="B15" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="135" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="132" t="s">
+      <c r="D15" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="132" t="s">
+      <c r="E15" s="135" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="132" t="s">
+      <c r="F15" s="135" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="147" t="s">
+      <c r="G15" s="146" t="s">
         <v>136</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -2523,20 +2530,20 @@
         <v>142</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K15" s="43" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A16" s="145"/>
-      <c r="B16" s="133"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="152"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="147"/>
       <c r="H16" s="45" t="s">
         <v>115</v>
       </c>
@@ -2550,554 +2557,586 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A17" s="145"/>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="152"/>
-      <c r="H17" s="57" t="s">
+    <row r="17" spans="1:11" ht="87.75" customHeight="1">
+      <c r="A17" s="139"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="51" t="s">
+      <c r="I17" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="J17" s="53" t="s">
+      <c r="J17" s="127" t="s">
+        <v>254</v>
+      </c>
+      <c r="K17" s="134" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="87.75" customHeight="1" thickBot="1">
+      <c r="A18" s="140"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="130" t="s">
+        <v>253</v>
+      </c>
+      <c r="I18" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="K17" s="52" t="s">
+      <c r="K18" s="52" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A18" s="153" t="s">
+    <row r="19" spans="1:11" ht="145.5" customHeight="1">
+      <c r="A19" s="143" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="146" t="s">
+      <c r="B19" s="135" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="146" t="s">
+      <c r="C19" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="146" t="s">
+      <c r="D19" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="146" t="s">
+      <c r="E19" s="135" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="146" t="s">
+      <c r="F19" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="143" t="s">
+      <c r="G19" s="141" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H19" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I19" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J19" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="K18" s="49" t="s">
+      <c r="K19" s="49" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="145.5" customHeight="1" thickBot="1">
-      <c r="A19" s="142"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="11" t="s">
+    <row r="20" spans="1:11" ht="74.25" customHeight="1" thickBot="1">
+      <c r="A20" s="144"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="142"/>
+      <c r="H20" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="I19" s="48" t="s">
+      <c r="I20" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="J19" s="48" t="s">
+      <c r="J20" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="K19" s="66" t="s">
+      <c r="K20" s="65" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="74.25" customHeight="1" thickBot="1">
-      <c r="A20" s="44" t="s">
+    <row r="21" spans="1:11" ht="96.6" customHeight="1" thickBot="1">
+      <c r="A21" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B21" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C21" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D21" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E21" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F21" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G21" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I21" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K21" s="50" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="96.6" customHeight="1">
-      <c r="A21" s="141" t="s">
+    <row r="22" spans="1:11" ht="69" customHeight="1">
+      <c r="A22" s="138" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="132" t="s">
+      <c r="B22" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="132" t="s">
+      <c r="C22" s="135" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="132" t="s">
+      <c r="D22" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="132" t="s">
+      <c r="E22" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="132" t="s">
+      <c r="F22" s="135" t="s">
         <v>160</v>
       </c>
-      <c r="G21" s="132" t="s">
+      <c r="G22" s="135" t="s">
+        <v>186</v>
+      </c>
+      <c r="H22" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" s="126" t="s">
+        <v>163</v>
+      </c>
+      <c r="J22" s="126" t="s">
+        <v>256</v>
+      </c>
+      <c r="K22" s="131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A23" s="139"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="92" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" s="127" t="s">
+        <v>163</v>
+      </c>
+      <c r="J23" s="127" t="s">
+        <v>257</v>
+      </c>
+      <c r="K23" s="134" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A24" s="139"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="136"/>
+      <c r="H24" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="I24" s="127" t="s">
+        <v>185</v>
+      </c>
+      <c r="J24" s="127" t="s">
+        <v>164</v>
+      </c>
+      <c r="K24" s="134" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A25" s="139"/>
+      <c r="B25" s="136"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="136"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="136"/>
+      <c r="G25" s="136"/>
+      <c r="H25" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="I25" s="127" t="s">
+        <v>188</v>
+      </c>
+      <c r="J25" s="127" t="s">
+        <v>251</v>
+      </c>
+      <c r="K25" s="134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A26" s="139"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="136"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="127" t="s">
+        <v>189</v>
+      </c>
+      <c r="J26" s="127" t="s">
+        <v>252</v>
+      </c>
+      <c r="K26" s="134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A27" s="139"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="92" t="s">
+        <v>195</v>
+      </c>
+      <c r="I27" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="J27" s="127" t="s">
+        <v>198</v>
+      </c>
+      <c r="K27" s="134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="99.75" customHeight="1">
+      <c r="A28" s="139"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="136"/>
+      <c r="G28" s="136"/>
+      <c r="H28" s="92" t="s">
+        <v>196</v>
+      </c>
+      <c r="I28" s="127" t="s">
+        <v>191</v>
+      </c>
+      <c r="J28" s="127" t="s">
+        <v>199</v>
+      </c>
+      <c r="K28" s="134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="139.5" customHeight="1">
+      <c r="A29" s="139"/>
+      <c r="B29" s="136"/>
+      <c r="C29" s="136"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="92" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="127" t="s">
+        <v>192</v>
+      </c>
+      <c r="J29" s="127" t="s">
+        <v>200</v>
+      </c>
+      <c r="K29" s="134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="108" customHeight="1" thickBot="1">
+      <c r="A30" s="140"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I30" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="H21" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="I21" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="J21" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="K21" s="82" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="69" customHeight="1">
-      <c r="A22" s="145"/>
-      <c r="B22" s="133"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="97" t="s">
-        <v>161</v>
-      </c>
-      <c r="I22" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="J22" s="80" t="s">
+      <c r="J30" s="128" t="s">
+        <v>201</v>
+      </c>
+      <c r="K30" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="K22" s="83" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A23" s="145"/>
-      <c r="B23" s="133"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="133"/>
-      <c r="G23" s="133"/>
-      <c r="H23" s="97" t="s">
-        <v>162</v>
-      </c>
-      <c r="I23" s="80" t="s">
-        <v>189</v>
-      </c>
-      <c r="J23" s="80" t="s">
-        <v>252</v>
-      </c>
-      <c r="K23" s="83" t="s">
+    </row>
+    <row r="31" spans="1:11" ht="99" customHeight="1" thickBot="1">
+      <c r="A31" s="69" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A24" s="145"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="I24" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="J24" s="80" t="s">
-        <v>253</v>
-      </c>
-      <c r="K24" s="83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A25" s="145"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="133"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="133"/>
-      <c r="H25" s="97" t="s">
-        <v>195</v>
-      </c>
-      <c r="I25" s="80" t="s">
-        <v>191</v>
-      </c>
-      <c r="J25" s="80" t="s">
-        <v>199</v>
-      </c>
-      <c r="K25" s="83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A26" s="145"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="97" t="s">
-        <v>196</v>
-      </c>
-      <c r="I26" s="80" t="s">
-        <v>192</v>
-      </c>
-      <c r="J26" s="80" t="s">
-        <v>200</v>
-      </c>
-      <c r="K26" s="83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="99.75" customHeight="1">
-      <c r="A27" s="145"/>
-      <c r="B27" s="133"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="133"/>
-      <c r="G27" s="133"/>
-      <c r="H27" s="97" t="s">
-        <v>197</v>
-      </c>
-      <c r="I27" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="J27" s="80" t="s">
-        <v>201</v>
-      </c>
-      <c r="K27" s="83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="99.75" customHeight="1" thickBot="1">
-      <c r="A28" s="142"/>
-      <c r="B28" s="134"/>
-      <c r="C28" s="134"/>
-      <c r="D28" s="134"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I28" s="81" t="s">
-        <v>188</v>
-      </c>
-      <c r="J28" s="81" t="s">
+      <c r="B31" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I31" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="J31" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="117.75" customHeight="1" thickBot="1">
+      <c r="A32" s="69" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="J32" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="68" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="87" customHeight="1" thickBot="1">
+      <c r="A33" s="129" t="s">
         <v>202</v>
       </c>
-      <c r="K28" s="84" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="139.5" customHeight="1" thickBot="1">
-      <c r="A29" s="70" t="s">
-        <v>167</v>
-      </c>
-      <c r="B29" s="67" t="s">
-        <v>168</v>
-      </c>
-      <c r="C29" s="67" t="s">
-        <v>181</v>
-      </c>
-      <c r="D29" s="67" t="s">
+      <c r="B33" s="102" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="67" t="s">
-        <v>158</v>
-      </c>
-      <c r="F29" s="67" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="85" t="s">
-        <v>170</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="I29" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="J29" s="67" t="s">
+      <c r="E33" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" s="102" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="I33" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="J33" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="K29" s="69" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="108" customHeight="1" thickBot="1">
-      <c r="A30" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="67" t="s">
-        <v>182</v>
-      </c>
-      <c r="D30" s="67" t="s">
+      <c r="K33" s="107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="74.25" customHeight="1">
+      <c r="A34" s="138" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="135" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="135" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="67" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I30" s="67" t="s">
-        <v>179</v>
-      </c>
-      <c r="J30" s="67" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="69" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="99" customHeight="1" thickBot="1">
-      <c r="A31" s="113" t="s">
-        <v>203</v>
-      </c>
-      <c r="B31" s="107" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" s="107" t="s">
-        <v>205</v>
-      </c>
-      <c r="D31" s="107" t="s">
+      <c r="E34" s="135" t="s">
+        <v>214</v>
+      </c>
+      <c r="F34" s="135" t="s">
+        <v>215</v>
+      </c>
+      <c r="G34" s="141" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" s="64" t="s">
+        <v>212</v>
+      </c>
+      <c r="I34" s="100" t="s">
+        <v>232</v>
+      </c>
+      <c r="J34" s="100" t="s">
+        <v>235</v>
+      </c>
+      <c r="K34" s="106" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="59.25" customHeight="1">
+      <c r="A35" s="139"/>
+      <c r="B35" s="136"/>
+      <c r="C35" s="136"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="136"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="92" t="s">
+        <v>230</v>
+      </c>
+      <c r="I35" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="J35" s="109" t="s">
+        <v>237</v>
+      </c>
+      <c r="K35" s="111" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="59.25" customHeight="1" thickBot="1">
+      <c r="A36" s="140"/>
+      <c r="B36" s="137"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I36" s="110" t="s">
+        <v>233</v>
+      </c>
+      <c r="J36" s="110" t="s">
+        <v>239</v>
+      </c>
+      <c r="K36" s="111" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="94.5" customHeight="1">
+      <c r="A37" s="143" t="s">
+        <v>222</v>
+      </c>
+      <c r="B37" s="135" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="135" t="s">
+        <v>218</v>
+      </c>
+      <c r="D37" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="107" t="s">
-        <v>206</v>
-      </c>
-      <c r="F31" s="107" t="s">
-        <v>217</v>
-      </c>
-      <c r="G31" s="58" t="s">
+      <c r="E37" s="135" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="135" t="s">
+        <v>219</v>
+      </c>
+      <c r="G37" s="141" t="s">
+        <v>241</v>
+      </c>
+      <c r="H37" s="64" t="s">
         <v>221</v>
       </c>
-      <c r="H31" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="I31" s="107" t="s">
-        <v>209</v>
-      </c>
-      <c r="J31" s="107" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="112" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="117.75" customHeight="1">
-      <c r="A32" s="135" t="s">
-        <v>212</v>
-      </c>
-      <c r="B32" s="132" t="s">
-        <v>211</v>
-      </c>
-      <c r="C32" s="132" t="s">
-        <v>214</v>
-      </c>
-      <c r="D32" s="132" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="132" t="s">
-        <v>215</v>
-      </c>
-      <c r="F32" s="132" t="s">
-        <v>216</v>
-      </c>
-      <c r="G32" s="138" t="s">
+      <c r="I37" s="100" t="s">
+        <v>225</v>
+      </c>
+      <c r="J37" s="100" t="s">
         <v>224</v>
       </c>
-      <c r="H32" s="65" t="s">
-        <v>213</v>
-      </c>
-      <c r="I32" s="105" t="s">
-        <v>233</v>
-      </c>
-      <c r="J32" s="105" t="s">
-        <v>236</v>
-      </c>
-      <c r="K32" s="111" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="87" customHeight="1">
-      <c r="A33" s="136"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="133"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="97" t="s">
-        <v>231</v>
-      </c>
-      <c r="I33" s="115" t="s">
-        <v>235</v>
-      </c>
-      <c r="J33" s="115" t="s">
-        <v>238</v>
-      </c>
-      <c r="K33" s="117" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="74.25" customHeight="1" thickBot="1">
-      <c r="A34" s="137"/>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="I34" s="116" t="s">
-        <v>234</v>
-      </c>
-      <c r="J34" s="116" t="s">
-        <v>240</v>
-      </c>
-      <c r="K34" s="117" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="59.25" customHeight="1">
-      <c r="A35" s="141" t="s">
-        <v>223</v>
-      </c>
-      <c r="B35" s="132" t="s">
-        <v>218</v>
-      </c>
-      <c r="C35" s="132" t="s">
-        <v>219</v>
-      </c>
-      <c r="D35" s="132" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="132" t="s">
-        <v>215</v>
-      </c>
-      <c r="F35" s="132" t="s">
-        <v>220</v>
-      </c>
-      <c r="G35" s="143" t="s">
+      <c r="K37" s="106" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="48" thickBot="1">
+      <c r="A38" s="144"/>
+      <c r="B38" s="137"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="137"/>
+      <c r="G38" s="142"/>
+      <c r="H38" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="H35" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="I35" s="105" t="s">
+      <c r="I38" s="102" t="s">
         <v>226</v>
       </c>
-      <c r="J35" s="105" t="s">
-        <v>225</v>
-      </c>
-      <c r="K35" s="111" t="s">
+      <c r="J38" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="K38" s="107" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A36" s="142"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="134"/>
-      <c r="G36" s="144"/>
-      <c r="H36" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="I36" s="107" t="s">
-        <v>227</v>
-      </c>
-      <c r="J36" s="107" t="s">
-        <v>228</v>
-      </c>
-      <c r="K36" s="112" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A5"/>
@@ -3107,10 +3146,13 @@
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="G3:G5"/>
-    <mergeCell ref="B21:B28"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="A9:A10"/>
@@ -3118,30 +3160,37 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="G21:G28"/>
-    <mergeCell ref="F21:F28"/>
-    <mergeCell ref="E21:E28"/>
-    <mergeCell ref="D21:D28"/>
-    <mergeCell ref="C21:C28"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="G22:G30"/>
+    <mergeCell ref="F22:F30"/>
+    <mergeCell ref="E22:E30"/>
+    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="G34:G36"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3320,7 +3369,7 @@
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="27"/>
-      <c r="M6" s="60"/>
+      <c r="M6" s="59"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1">
       <c r="A7" s="24">
@@ -3364,7 +3413,7 @@
       <c r="E8" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="61" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -3389,7 +3438,7 @@
       <c r="E9" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="60" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="40" t="s">
@@ -3461,10 +3510,10 @@
       <c r="D12" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="63" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="16" t="s">
@@ -3477,19 +3526,19 @@
       <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="62" t="s">
         <v>96</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="58" t="s">
         <v>132</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="66" t="s">
         <v>134</v>
       </c>
       <c r="G13" s="22" t="s">
@@ -3511,10 +3560,10 @@
       <c r="D14" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="67" t="s">
         <v>138</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="67" t="s">
         <v>138</v>
       </c>
       <c r="G14" s="16" t="s">
@@ -3527,50 +3576,50 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="63" t="s">
+      <c r="G15" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="63"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:13" ht="32.25" thickBot="1">
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="66" t="s">
         <v>139</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="63"/>
+      <c r="H16" s="62"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:12" ht="32.25" thickBot="1">
@@ -3586,10 +3635,10 @@
       <c r="D17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="F17" s="67" t="s">
         <v>150</v>
       </c>
       <c r="G17" s="16" t="s">
@@ -3599,1624 +3648,1624 @@
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:12" ht="48" thickBot="1">
-      <c r="A18" s="87">
+      <c r="A18" s="82">
         <v>17</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="D18" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="88" t="s">
+      <c r="G18" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="88"/>
-      <c r="I18" s="90"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="85"/>
     </row>
     <row r="19" spans="1:12" ht="35.25" customHeight="1" thickBot="1">
-      <c r="A19" s="91">
+      <c r="A19" s="86">
         <v>18</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="G19" s="92" t="s">
+      <c r="G19" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="94"/>
-      <c r="I19" s="95"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="90"/>
     </row>
     <row r="20" spans="1:12" ht="108" customHeight="1">
-      <c r="A20" s="73">
+      <c r="A20" s="72">
         <v>19</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="67" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="F20" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="G20" s="74" t="s">
+      <c r="F20" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="76"/>
-      <c r="L20" s="60"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="75"/>
+      <c r="L20" s="59"/>
     </row>
     <row r="21" spans="1:12" ht="27" customHeight="1">
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" s="71" t="s">
+      <c r="D21" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="F21" s="71" t="s">
+      <c r="F21" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="G21" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="77"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1">
-      <c r="A22" s="86">
+      <c r="A22" s="81">
         <v>21</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E22" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="G22" s="63" t="s">
+      <c r="D22" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="63"/>
-      <c r="I22" s="77"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:12" ht="45.75" customHeight="1">
-      <c r="A23" s="63">
+      <c r="A23" s="62">
         <v>22</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="59"/>
+      <c r="I23" s="95"/>
+    </row>
+    <row r="24" spans="1:12" ht="94.5">
+      <c r="A24" s="93">
+        <v>23</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="D23" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="96" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="96" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" s="63" t="s">
+      <c r="D24" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="60"/>
-      <c r="I23" s="100"/>
-    </row>
-    <row r="24" spans="1:12" ht="94.5">
-      <c r="A24" s="98">
-        <v>23</v>
-      </c>
-      <c r="B24" s="63" t="s">
+      <c r="H24" s="59"/>
+      <c r="I24" s="95"/>
+    </row>
+    <row r="25" spans="1:12" ht="94.5">
+      <c r="A25" s="96">
+        <v>24</v>
+      </c>
+      <c r="B25" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="D24" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E24" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="G24" s="63" t="s">
+      <c r="D25" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="60"/>
-      <c r="I24" s="100"/>
-    </row>
-    <row r="25" spans="1:12" ht="94.5">
-      <c r="A25" s="101">
-        <v>24</v>
-      </c>
-      <c r="B25" s="63" t="s">
+      <c r="H25" s="59"/>
+      <c r="I25" s="95"/>
+    </row>
+    <row r="26" spans="1:12" ht="94.5">
+      <c r="A26" s="93">
+        <v>25</v>
+      </c>
+      <c r="B26" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="D25" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E25" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="63" t="s">
+      <c r="D26" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="100"/>
-    </row>
-    <row r="26" spans="1:12" ht="94.5">
-      <c r="A26" s="98">
-        <v>25</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="D26" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="E26" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="F26" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="G26" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="100"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="95"/>
     </row>
     <row r="27" spans="1:12" ht="95.25" thickBot="1">
-      <c r="A27" s="102">
+      <c r="A27" s="97">
         <v>26</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>154</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="D27" s="78" t="s">
-        <v>183</v>
-      </c>
-      <c r="E27" s="81" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="81" t="s">
-        <v>166</v>
+        <v>197</v>
+      </c>
+      <c r="D27" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="79" t="s">
+        <v>165</v>
       </c>
       <c r="G27" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="103"/>
-      <c r="I27" s="104"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="99"/>
     </row>
     <row r="28" spans="1:12" ht="32.25" thickBot="1">
-      <c r="A28" s="91">
+      <c r="A28" s="86">
         <v>27</v>
       </c>
-      <c r="B28" s="88" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" s="88" t="s">
-        <v>171</v>
-      </c>
-      <c r="D28" s="89" t="s">
-        <v>183</v>
-      </c>
-      <c r="E28" s="99" t="s">
-        <v>185</v>
-      </c>
-      <c r="F28" s="99" t="s">
-        <v>185</v>
-      </c>
-      <c r="G28" s="88" t="s">
+      <c r="B28" s="83" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="84" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="G28" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="88"/>
-      <c r="I28" s="90"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="85"/>
     </row>
     <row r="29" spans="1:12" ht="79.5" thickBot="1">
-      <c r="A29" s="87">
+      <c r="A29" s="82">
         <v>28</v>
       </c>
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="83" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="88" t="s">
-        <v>174</v>
-      </c>
-      <c r="D29" s="89" t="s">
-        <v>183</v>
-      </c>
-      <c r="E29" s="108" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="108" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="88" t="s">
+      <c r="D29" s="84" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="103" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="103" t="s">
+        <v>179</v>
+      </c>
+      <c r="G29" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="88"/>
-      <c r="I29" s="90"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="85"/>
     </row>
     <row r="30" spans="1:12" ht="67.5" customHeight="1" thickBot="1">
-      <c r="A30" s="87">
+      <c r="A30" s="82">
         <v>29</v>
       </c>
-      <c r="B30" s="124" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="124" t="s">
-        <v>208</v>
-      </c>
-      <c r="D30" s="124" t="s">
+      <c r="B30" s="118" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="118" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" s="118" t="s">
+        <v>243</v>
+      </c>
+      <c r="E30" s="103" t="s">
         <v>244</v>
       </c>
-      <c r="E30" s="108" t="s">
+      <c r="F30" s="103" t="s">
+        <v>244</v>
+      </c>
+      <c r="G30" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="83"/>
+      <c r="I30" s="85"/>
+    </row>
+    <row r="31" spans="1:12" ht="54.75" customHeight="1">
+      <c r="A31" s="119">
+        <v>30</v>
+      </c>
+      <c r="B31" s="120" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="120" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" s="100" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="108" t="s">
+      <c r="F31" s="100" t="s">
         <v>245</v>
       </c>
-      <c r="G30" s="88" t="s">
+      <c r="G31" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="88"/>
-      <c r="I30" s="90"/>
-    </row>
-    <row r="31" spans="1:12" ht="54.75" customHeight="1">
-      <c r="A31" s="125">
-        <v>30</v>
-      </c>
-      <c r="B31" s="126" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" s="126" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" s="126" t="s">
-        <v>244</v>
-      </c>
-      <c r="E31" s="105" t="s">
+      <c r="H31" s="120"/>
+      <c r="I31" s="104"/>
+    </row>
+    <row r="32" spans="1:12" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A32" s="121">
+        <v>31</v>
+      </c>
+      <c r="B32" s="122" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="122" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="E32" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="F31" s="105" t="s">
+      <c r="F32" s="110" t="s">
         <v>246</v>
-      </c>
-      <c r="G31" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="126"/>
-      <c r="I31" s="109"/>
-    </row>
-    <row r="32" spans="1:12" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A32" s="127">
-        <v>31</v>
-      </c>
-      <c r="B32" s="128" t="s">
-        <v>212</v>
-      </c>
-      <c r="C32" s="128" t="s">
-        <v>231</v>
-      </c>
-      <c r="D32" s="128" t="s">
-        <v>244</v>
-      </c>
-      <c r="E32" s="116" t="s">
-        <v>247</v>
-      </c>
-      <c r="F32" s="116" t="s">
-        <v>247</v>
       </c>
       <c r="G32" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="128"/>
-      <c r="I32" s="110"/>
+      <c r="H32" s="122"/>
+      <c r="I32" s="105"/>
     </row>
     <row r="33" spans="1:9" ht="54.75" customHeight="1">
-      <c r="A33" s="129">
+      <c r="A33" s="123">
         <v>32</v>
       </c>
-      <c r="B33" s="126" t="s">
-        <v>212</v>
-      </c>
-      <c r="C33" s="126" t="s">
-        <v>232</v>
-      </c>
-      <c r="D33" s="126" t="s">
-        <v>244</v>
-      </c>
-      <c r="E33" s="130" t="s">
+      <c r="B33" s="120" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="120" t="s">
+        <v>231</v>
+      </c>
+      <c r="D33" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="124" t="s">
+        <v>247</v>
+      </c>
+      <c r="F33" s="124" t="s">
+        <v>247</v>
+      </c>
+      <c r="G33" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="120"/>
+      <c r="I33" s="104"/>
+    </row>
+    <row r="34" spans="1:9" ht="54.75" customHeight="1">
+      <c r="A34" s="114">
+        <v>33</v>
+      </c>
+      <c r="B34" s="113" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="113" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="113" t="s">
+        <v>243</v>
+      </c>
+      <c r="E34" s="101" t="s">
         <v>248</v>
       </c>
-      <c r="F33" s="130" t="s">
+      <c r="F34" s="101" t="s">
         <v>248</v>
       </c>
-      <c r="G33" s="74" t="s">
+      <c r="G34" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="H33" s="126"/>
-      <c r="I33" s="109"/>
-    </row>
-    <row r="34" spans="1:9" ht="54.75" customHeight="1">
-      <c r="A34" s="120">
-        <v>33</v>
-      </c>
-      <c r="B34" s="119" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="119" t="s">
+      <c r="H34" s="113"/>
+      <c r="I34" s="111"/>
+    </row>
+    <row r="35" spans="1:9" ht="54.75" customHeight="1" thickBot="1">
+      <c r="A35" s="125">
+        <v>34</v>
+      </c>
+      <c r="B35" s="122" t="s">
         <v>222</v>
       </c>
-      <c r="D34" s="119" t="s">
-        <v>244</v>
-      </c>
-      <c r="E34" s="106" t="s">
+      <c r="C35" s="122" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="E35" s="102" t="s">
         <v>249</v>
       </c>
-      <c r="F34" s="106" t="s">
+      <c r="F35" s="102" t="s">
         <v>249</v>
-      </c>
-      <c r="G34" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H34" s="119"/>
-      <c r="I34" s="117"/>
-    </row>
-    <row r="35" spans="1:9" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A35" s="131">
-        <v>34</v>
-      </c>
-      <c r="B35" s="128" t="s">
-        <v>223</v>
-      </c>
-      <c r="C35" s="128" t="s">
-        <v>243</v>
-      </c>
-      <c r="D35" s="128" t="s">
-        <v>244</v>
-      </c>
-      <c r="E35" s="107" t="s">
-        <v>250</v>
-      </c>
-      <c r="F35" s="107" t="s">
-        <v>250</v>
       </c>
       <c r="G35" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H35" s="128"/>
-      <c r="I35" s="110"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="105"/>
     </row>
     <row r="36" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A36" s="121">
+      <c r="A36" s="115">
         <v>35</v>
       </c>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="123"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
+      <c r="G36" s="112"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="117"/>
     </row>
     <row r="37" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A37" s="121">
+      <c r="A37" s="115">
         <v>36</v>
       </c>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="123"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="117"/>
     </row>
     <row r="38" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A38" s="122">
+      <c r="A38" s="116">
         <v>37</v>
       </c>
-      <c r="B38" s="119"/>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="123"/>
+      <c r="B38" s="113"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="117"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="119"/>
-      <c r="B39" s="119"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="123"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="117"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="119"/>
-      <c r="B40" s="119"/>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="123"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
+      <c r="C40" s="112"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="112"/>
+      <c r="G40" s="112"/>
+      <c r="H40" s="112"/>
+      <c r="I40" s="117"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="119"/>
-      <c r="B41" s="119"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
-      <c r="I41" s="123"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="117"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="118"/>
-      <c r="B42" s="118"/>
-      <c r="C42" s="118"/>
-      <c r="D42" s="118"/>
-      <c r="E42" s="118"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="123"/>
+      <c r="A42" s="112"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="117"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="118"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="118"/>
-      <c r="D43" s="118"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
-      <c r="G43" s="118"/>
-      <c r="H43" s="118"/>
-      <c r="I43" s="123"/>
+      <c r="A43" s="112"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="112"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="117"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="118"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="123"/>
+      <c r="A44" s="112"/>
+      <c r="B44" s="112"/>
+      <c r="C44" s="112"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="112"/>
+      <c r="G44" s="112"/>
+      <c r="H44" s="112"/>
+      <c r="I44" s="117"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="118"/>
-      <c r="B45" s="118"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="118"/>
-      <c r="H45" s="118"/>
-      <c r="I45" s="123"/>
+      <c r="A45" s="112"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="117"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="118"/>
-      <c r="B46" s="118"/>
-      <c r="C46" s="118"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="123"/>
+      <c r="A46" s="112"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="117"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="118"/>
-      <c r="B47" s="118"/>
-      <c r="C47" s="118"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
-      <c r="I47" s="123"/>
+      <c r="A47" s="112"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="112"/>
+      <c r="F47" s="112"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="117"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="118"/>
-      <c r="B48" s="118"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="118"/>
-      <c r="G48" s="118"/>
-      <c r="H48" s="118"/>
-      <c r="I48" s="123"/>
+      <c r="A48" s="112"/>
+      <c r="B48" s="112"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="117"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="118"/>
-      <c r="B49" s="118"/>
-      <c r="C49" s="118"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="118"/>
-      <c r="G49" s="118"/>
-      <c r="H49" s="118"/>
-      <c r="I49" s="123"/>
+      <c r="A49" s="112"/>
+      <c r="B49" s="112"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="117"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="118"/>
-      <c r="B50" s="118"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="118"/>
-      <c r="H50" s="118"/>
-      <c r="I50" s="123"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="112"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="117"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="118"/>
-      <c r="B51" s="118"/>
-      <c r="C51" s="118"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
-      <c r="I51" s="123"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="112"/>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="117"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="118"/>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="118"/>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="123"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112"/>
+      <c r="F52" s="112"/>
+      <c r="G52" s="112"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="117"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="118"/>
-      <c r="B53" s="118"/>
-      <c r="C53" s="118"/>
-      <c r="D53" s="118"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="118"/>
-      <c r="I53" s="123"/>
+      <c r="A53" s="112"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="112"/>
+      <c r="D53" s="112"/>
+      <c r="E53" s="112"/>
+      <c r="F53" s="112"/>
+      <c r="G53" s="112"/>
+      <c r="H53" s="112"/>
+      <c r="I53" s="117"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="118"/>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
-      <c r="G54" s="118"/>
-      <c r="H54" s="118"/>
-      <c r="I54" s="123"/>
+      <c r="A54" s="112"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="112"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="112"/>
+      <c r="F54" s="112"/>
+      <c r="G54" s="112"/>
+      <c r="H54" s="112"/>
+      <c r="I54" s="117"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="118"/>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
-      <c r="G55" s="118"/>
-      <c r="H55" s="118"/>
-      <c r="I55" s="123"/>
+      <c r="A55" s="112"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="112"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="112"/>
+      <c r="G55" s="112"/>
+      <c r="H55" s="112"/>
+      <c r="I55" s="117"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="118"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="118"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="118"/>
-      <c r="G56" s="118"/>
-      <c r="H56" s="118"/>
-      <c r="I56" s="123"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="112"/>
+      <c r="D56" s="112"/>
+      <c r="E56" s="112"/>
+      <c r="F56" s="112"/>
+      <c r="G56" s="112"/>
+      <c r="H56" s="112"/>
+      <c r="I56" s="117"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="118"/>
-      <c r="B57" s="118"/>
-      <c r="C57" s="118"/>
-      <c r="D57" s="118"/>
-      <c r="E57" s="118"/>
-      <c r="F57" s="118"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="118"/>
-      <c r="I57" s="123"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="112"/>
+      <c r="C57" s="112"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="112"/>
+      <c r="F57" s="112"/>
+      <c r="G57" s="112"/>
+      <c r="H57" s="112"/>
+      <c r="I57" s="117"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="118"/>
-      <c r="B58" s="118"/>
-      <c r="C58" s="118"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="118"/>
-      <c r="G58" s="118"/>
-      <c r="H58" s="118"/>
-      <c r="I58" s="123"/>
+      <c r="A58" s="112"/>
+      <c r="B58" s="112"/>
+      <c r="C58" s="112"/>
+      <c r="D58" s="112"/>
+      <c r="E58" s="112"/>
+      <c r="F58" s="112"/>
+      <c r="G58" s="112"/>
+      <c r="H58" s="112"/>
+      <c r="I58" s="117"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="118"/>
-      <c r="B59" s="118"/>
-      <c r="C59" s="118"/>
-      <c r="D59" s="118"/>
-      <c r="E59" s="118"/>
-      <c r="F59" s="118"/>
-      <c r="G59" s="118"/>
-      <c r="H59" s="118"/>
-      <c r="I59" s="123"/>
+      <c r="A59" s="112"/>
+      <c r="B59" s="112"/>
+      <c r="C59" s="112"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="112"/>
+      <c r="G59" s="112"/>
+      <c r="H59" s="112"/>
+      <c r="I59" s="117"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="118"/>
-      <c r="B60" s="118"/>
-      <c r="C60" s="118"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="118"/>
-      <c r="F60" s="118"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="118"/>
-      <c r="I60" s="123"/>
+      <c r="A60" s="112"/>
+      <c r="B60" s="112"/>
+      <c r="C60" s="112"/>
+      <c r="D60" s="112"/>
+      <c r="E60" s="112"/>
+      <c r="F60" s="112"/>
+      <c r="G60" s="112"/>
+      <c r="H60" s="112"/>
+      <c r="I60" s="117"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="118"/>
-      <c r="B61" s="118"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="118"/>
-      <c r="E61" s="118"/>
-      <c r="F61" s="118"/>
-      <c r="G61" s="118"/>
-      <c r="H61" s="118"/>
-      <c r="I61" s="123"/>
+      <c r="A61" s="112"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="112"/>
+      <c r="D61" s="112"/>
+      <c r="E61" s="112"/>
+      <c r="F61" s="112"/>
+      <c r="G61" s="112"/>
+      <c r="H61" s="112"/>
+      <c r="I61" s="117"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="118"/>
-      <c r="B62" s="118"/>
-      <c r="C62" s="118"/>
-      <c r="D62" s="118"/>
-      <c r="E62" s="118"/>
-      <c r="F62" s="118"/>
-      <c r="G62" s="118"/>
-      <c r="H62" s="118"/>
-      <c r="I62" s="123"/>
+      <c r="A62" s="112"/>
+      <c r="B62" s="112"/>
+      <c r="C62" s="112"/>
+      <c r="D62" s="112"/>
+      <c r="E62" s="112"/>
+      <c r="F62" s="112"/>
+      <c r="G62" s="112"/>
+      <c r="H62" s="112"/>
+      <c r="I62" s="117"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="118"/>
-      <c r="B63" s="118"/>
-      <c r="C63" s="118"/>
-      <c r="D63" s="118"/>
-      <c r="E63" s="118"/>
-      <c r="F63" s="118"/>
-      <c r="G63" s="118"/>
-      <c r="H63" s="118"/>
-      <c r="I63" s="123"/>
+      <c r="A63" s="112"/>
+      <c r="B63" s="112"/>
+      <c r="C63" s="112"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="112"/>
+      <c r="F63" s="112"/>
+      <c r="G63" s="112"/>
+      <c r="H63" s="112"/>
+      <c r="I63" s="117"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="118"/>
-      <c r="B64" s="118"/>
-      <c r="C64" s="118"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="118"/>
-      <c r="F64" s="118"/>
-      <c r="G64" s="118"/>
-      <c r="H64" s="118"/>
-      <c r="I64" s="123"/>
+      <c r="A64" s="112"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="112"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="117"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="118"/>
-      <c r="B65" s="118"/>
-      <c r="C65" s="118"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="118"/>
-      <c r="F65" s="118"/>
-      <c r="G65" s="118"/>
-      <c r="H65" s="118"/>
-      <c r="I65" s="123"/>
+      <c r="A65" s="112"/>
+      <c r="B65" s="112"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="112"/>
+      <c r="E65" s="112"/>
+      <c r="F65" s="112"/>
+      <c r="G65" s="112"/>
+      <c r="H65" s="112"/>
+      <c r="I65" s="117"/>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="118"/>
-      <c r="B66" s="118"/>
-      <c r="C66" s="118"/>
-      <c r="D66" s="118"/>
-      <c r="E66" s="118"/>
-      <c r="F66" s="118"/>
-      <c r="G66" s="118"/>
-      <c r="H66" s="118"/>
-      <c r="I66" s="123"/>
+      <c r="A66" s="112"/>
+      <c r="B66" s="112"/>
+      <c r="C66" s="112"/>
+      <c r="D66" s="112"/>
+      <c r="E66" s="112"/>
+      <c r="F66" s="112"/>
+      <c r="G66" s="112"/>
+      <c r="H66" s="112"/>
+      <c r="I66" s="117"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="118"/>
-      <c r="B67" s="118"/>
-      <c r="C67" s="118"/>
-      <c r="D67" s="118"/>
-      <c r="E67" s="118"/>
-      <c r="F67" s="118"/>
-      <c r="G67" s="118"/>
-      <c r="H67" s="118"/>
-      <c r="I67" s="123"/>
+      <c r="A67" s="112"/>
+      <c r="B67" s="112"/>
+      <c r="C67" s="112"/>
+      <c r="D67" s="112"/>
+      <c r="E67" s="112"/>
+      <c r="F67" s="112"/>
+      <c r="G67" s="112"/>
+      <c r="H67" s="112"/>
+      <c r="I67" s="117"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="118"/>
-      <c r="B68" s="118"/>
-      <c r="C68" s="118"/>
-      <c r="D68" s="118"/>
-      <c r="E68" s="118"/>
-      <c r="F68" s="118"/>
-      <c r="G68" s="118"/>
-      <c r="H68" s="118"/>
-      <c r="I68" s="123"/>
+      <c r="A68" s="112"/>
+      <c r="B68" s="112"/>
+      <c r="C68" s="112"/>
+      <c r="D68" s="112"/>
+      <c r="E68" s="112"/>
+      <c r="F68" s="112"/>
+      <c r="G68" s="112"/>
+      <c r="H68" s="112"/>
+      <c r="I68" s="117"/>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="118"/>
-      <c r="B69" s="118"/>
-      <c r="C69" s="118"/>
-      <c r="D69" s="118"/>
-      <c r="E69" s="118"/>
-      <c r="F69" s="118"/>
-      <c r="G69" s="118"/>
-      <c r="H69" s="118"/>
-      <c r="I69" s="123"/>
+      <c r="A69" s="112"/>
+      <c r="B69" s="112"/>
+      <c r="C69" s="112"/>
+      <c r="D69" s="112"/>
+      <c r="E69" s="112"/>
+      <c r="F69" s="112"/>
+      <c r="G69" s="112"/>
+      <c r="H69" s="112"/>
+      <c r="I69" s="117"/>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="118"/>
-      <c r="B70" s="118"/>
-      <c r="C70" s="118"/>
-      <c r="D70" s="118"/>
-      <c r="E70" s="118"/>
-      <c r="F70" s="118"/>
-      <c r="G70" s="118"/>
-      <c r="H70" s="118"/>
-      <c r="I70" s="123"/>
+      <c r="A70" s="112"/>
+      <c r="B70" s="112"/>
+      <c r="C70" s="112"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="112"/>
+      <c r="G70" s="112"/>
+      <c r="H70" s="112"/>
+      <c r="I70" s="117"/>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="118"/>
-      <c r="B71" s="118"/>
-      <c r="C71" s="118"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="118"/>
-      <c r="F71" s="118"/>
-      <c r="G71" s="118"/>
-      <c r="H71" s="118"/>
-      <c r="I71" s="123"/>
+      <c r="A71" s="112"/>
+      <c r="B71" s="112"/>
+      <c r="C71" s="112"/>
+      <c r="D71" s="112"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
+      <c r="G71" s="112"/>
+      <c r="H71" s="112"/>
+      <c r="I71" s="117"/>
     </row>
     <row r="72" spans="1:9" ht="15.75">
-      <c r="A72" s="118"/>
-      <c r="B72" s="118"/>
-      <c r="C72" s="118"/>
-      <c r="D72" s="118"/>
-      <c r="E72" s="118"/>
-      <c r="F72" s="118"/>
-      <c r="G72" s="118"/>
-      <c r="H72" s="118"/>
-      <c r="I72" s="123"/>
+      <c r="A72" s="112"/>
+      <c r="B72" s="112"/>
+      <c r="C72" s="112"/>
+      <c r="D72" s="112"/>
+      <c r="E72" s="112"/>
+      <c r="F72" s="112"/>
+      <c r="G72" s="112"/>
+      <c r="H72" s="112"/>
+      <c r="I72" s="117"/>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="118"/>
-      <c r="B73" s="118"/>
-      <c r="C73" s="118"/>
-      <c r="D73" s="118"/>
-      <c r="E73" s="118"/>
-      <c r="F73" s="118"/>
-      <c r="G73" s="118"/>
-      <c r="H73" s="118"/>
-      <c r="I73" s="123"/>
+      <c r="A73" s="112"/>
+      <c r="B73" s="112"/>
+      <c r="C73" s="112"/>
+      <c r="D73" s="112"/>
+      <c r="E73" s="112"/>
+      <c r="F73" s="112"/>
+      <c r="G73" s="112"/>
+      <c r="H73" s="112"/>
+      <c r="I73" s="117"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="118"/>
-      <c r="B74" s="118"/>
-      <c r="C74" s="118"/>
-      <c r="D74" s="118"/>
-      <c r="E74" s="118"/>
-      <c r="F74" s="118"/>
-      <c r="G74" s="118"/>
-      <c r="H74" s="118"/>
-      <c r="I74" s="123"/>
+      <c r="A74" s="112"/>
+      <c r="B74" s="112"/>
+      <c r="C74" s="112"/>
+      <c r="D74" s="112"/>
+      <c r="E74" s="112"/>
+      <c r="F74" s="112"/>
+      <c r="G74" s="112"/>
+      <c r="H74" s="112"/>
+      <c r="I74" s="117"/>
     </row>
     <row r="75" spans="1:9" ht="15.75">
-      <c r="A75" s="118"/>
-      <c r="B75" s="118"/>
-      <c r="C75" s="118"/>
-      <c r="D75" s="118"/>
-      <c r="E75" s="118"/>
-      <c r="F75" s="118"/>
-      <c r="G75" s="118"/>
-      <c r="H75" s="118"/>
-      <c r="I75" s="123"/>
+      <c r="A75" s="112"/>
+      <c r="B75" s="112"/>
+      <c r="C75" s="112"/>
+      <c r="D75" s="112"/>
+      <c r="E75" s="112"/>
+      <c r="F75" s="112"/>
+      <c r="G75" s="112"/>
+      <c r="H75" s="112"/>
+      <c r="I75" s="117"/>
     </row>
     <row r="76" spans="1:9" ht="15.75">
-      <c r="A76" s="118"/>
-      <c r="B76" s="118"/>
-      <c r="C76" s="118"/>
-      <c r="D76" s="118"/>
-      <c r="E76" s="118"/>
-      <c r="F76" s="118"/>
-      <c r="G76" s="118"/>
-      <c r="H76" s="118"/>
-      <c r="I76" s="123"/>
+      <c r="A76" s="112"/>
+      <c r="B76" s="112"/>
+      <c r="C76" s="112"/>
+      <c r="D76" s="112"/>
+      <c r="E76" s="112"/>
+      <c r="F76" s="112"/>
+      <c r="G76" s="112"/>
+      <c r="H76" s="112"/>
+      <c r="I76" s="117"/>
     </row>
     <row r="77" spans="1:9" ht="15.75">
-      <c r="A77" s="118"/>
-      <c r="B77" s="118"/>
-      <c r="C77" s="118"/>
-      <c r="D77" s="118"/>
-      <c r="E77" s="118"/>
-      <c r="F77" s="118"/>
-      <c r="G77" s="118"/>
-      <c r="H77" s="118"/>
-      <c r="I77" s="123"/>
+      <c r="A77" s="112"/>
+      <c r="B77" s="112"/>
+      <c r="C77" s="112"/>
+      <c r="D77" s="112"/>
+      <c r="E77" s="112"/>
+      <c r="F77" s="112"/>
+      <c r="G77" s="112"/>
+      <c r="H77" s="112"/>
+      <c r="I77" s="117"/>
     </row>
     <row r="78" spans="1:9" ht="15.75">
-      <c r="A78" s="118"/>
-      <c r="B78" s="118"/>
-      <c r="C78" s="118"/>
-      <c r="D78" s="118"/>
-      <c r="E78" s="118"/>
-      <c r="F78" s="118"/>
-      <c r="G78" s="118"/>
-      <c r="H78" s="118"/>
-      <c r="I78" s="123"/>
+      <c r="A78" s="112"/>
+      <c r="B78" s="112"/>
+      <c r="C78" s="112"/>
+      <c r="D78" s="112"/>
+      <c r="E78" s="112"/>
+      <c r="F78" s="112"/>
+      <c r="G78" s="112"/>
+      <c r="H78" s="112"/>
+      <c r="I78" s="117"/>
     </row>
     <row r="79" spans="1:9" ht="15.75">
-      <c r="A79" s="118"/>
-      <c r="B79" s="118"/>
-      <c r="C79" s="118"/>
-      <c r="D79" s="118"/>
-      <c r="E79" s="118"/>
-      <c r="F79" s="118"/>
-      <c r="G79" s="118"/>
-      <c r="H79" s="118"/>
-      <c r="I79" s="123"/>
+      <c r="A79" s="112"/>
+      <c r="B79" s="112"/>
+      <c r="C79" s="112"/>
+      <c r="D79" s="112"/>
+      <c r="E79" s="112"/>
+      <c r="F79" s="112"/>
+      <c r="G79" s="112"/>
+      <c r="H79" s="112"/>
+      <c r="I79" s="117"/>
     </row>
     <row r="80" spans="1:9" ht="15.75">
-      <c r="A80" s="118"/>
-      <c r="B80" s="118"/>
-      <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="118"/>
-      <c r="F80" s="118"/>
-      <c r="G80" s="118"/>
-      <c r="H80" s="118"/>
-      <c r="I80" s="123"/>
+      <c r="A80" s="112"/>
+      <c r="B80" s="112"/>
+      <c r="C80" s="112"/>
+      <c r="D80" s="112"/>
+      <c r="E80" s="112"/>
+      <c r="F80" s="112"/>
+      <c r="G80" s="112"/>
+      <c r="H80" s="112"/>
+      <c r="I80" s="117"/>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="118"/>
-      <c r="B81" s="118"/>
-      <c r="C81" s="118"/>
-      <c r="D81" s="118"/>
-      <c r="E81" s="118"/>
-      <c r="F81" s="118"/>
-      <c r="G81" s="118"/>
-      <c r="H81" s="118"/>
-      <c r="I81" s="123"/>
+      <c r="A81" s="112"/>
+      <c r="B81" s="112"/>
+      <c r="C81" s="112"/>
+      <c r="D81" s="112"/>
+      <c r="E81" s="112"/>
+      <c r="F81" s="112"/>
+      <c r="G81" s="112"/>
+      <c r="H81" s="112"/>
+      <c r="I81" s="117"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="118"/>
-      <c r="B82" s="118"/>
-      <c r="C82" s="118"/>
-      <c r="D82" s="118"/>
-      <c r="E82" s="118"/>
-      <c r="F82" s="118"/>
-      <c r="G82" s="118"/>
-      <c r="H82" s="118"/>
-      <c r="I82" s="123"/>
+      <c r="A82" s="112"/>
+      <c r="B82" s="112"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="112"/>
+      <c r="E82" s="112"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="112"/>
+      <c r="I82" s="117"/>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="118"/>
-      <c r="B83" s="118"/>
-      <c r="C83" s="118"/>
-      <c r="D83" s="118"/>
-      <c r="E83" s="118"/>
-      <c r="F83" s="118"/>
-      <c r="G83" s="118"/>
-      <c r="H83" s="118"/>
-      <c r="I83" s="123"/>
+      <c r="A83" s="112"/>
+      <c r="B83" s="112"/>
+      <c r="C83" s="112"/>
+      <c r="D83" s="112"/>
+      <c r="E83" s="112"/>
+      <c r="F83" s="112"/>
+      <c r="G83" s="112"/>
+      <c r="H83" s="112"/>
+      <c r="I83" s="117"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="118"/>
-      <c r="B84" s="118"/>
-      <c r="C84" s="118"/>
-      <c r="D84" s="118"/>
-      <c r="E84" s="118"/>
-      <c r="F84" s="118"/>
-      <c r="G84" s="118"/>
-      <c r="H84" s="118"/>
-      <c r="I84" s="123"/>
+      <c r="A84" s="112"/>
+      <c r="B84" s="112"/>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
+      <c r="H84" s="112"/>
+      <c r="I84" s="117"/>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="118"/>
-      <c r="B85" s="118"/>
-      <c r="C85" s="118"/>
-      <c r="D85" s="118"/>
-      <c r="E85" s="118"/>
-      <c r="F85" s="118"/>
-      <c r="G85" s="118"/>
-      <c r="H85" s="118"/>
-      <c r="I85" s="123"/>
+      <c r="A85" s="112"/>
+      <c r="B85" s="112"/>
+      <c r="C85" s="112"/>
+      <c r="D85" s="112"/>
+      <c r="E85" s="112"/>
+      <c r="F85" s="112"/>
+      <c r="G85" s="112"/>
+      <c r="H85" s="112"/>
+      <c r="I85" s="117"/>
     </row>
     <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="118"/>
-      <c r="B86" s="118"/>
-      <c r="C86" s="118"/>
-      <c r="D86" s="118"/>
-      <c r="E86" s="118"/>
-      <c r="F86" s="118"/>
-      <c r="G86" s="118"/>
-      <c r="H86" s="118"/>
-      <c r="I86" s="123"/>
+      <c r="A86" s="112"/>
+      <c r="B86" s="112"/>
+      <c r="C86" s="112"/>
+      <c r="D86" s="112"/>
+      <c r="E86" s="112"/>
+      <c r="F86" s="112"/>
+      <c r="G86" s="112"/>
+      <c r="H86" s="112"/>
+      <c r="I86" s="117"/>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="118"/>
-      <c r="B87" s="118"/>
-      <c r="C87" s="118"/>
-      <c r="D87" s="118"/>
-      <c r="E87" s="118"/>
-      <c r="F87" s="118"/>
-      <c r="G87" s="118"/>
-      <c r="H87" s="118"/>
-      <c r="I87" s="123"/>
+      <c r="A87" s="112"/>
+      <c r="B87" s="112"/>
+      <c r="C87" s="112"/>
+      <c r="D87" s="112"/>
+      <c r="E87" s="112"/>
+      <c r="F87" s="112"/>
+      <c r="G87" s="112"/>
+      <c r="H87" s="112"/>
+      <c r="I87" s="117"/>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="118"/>
-      <c r="B88" s="118"/>
-      <c r="C88" s="118"/>
-      <c r="D88" s="118"/>
-      <c r="E88" s="118"/>
-      <c r="F88" s="118"/>
-      <c r="G88" s="118"/>
-      <c r="H88" s="118"/>
-      <c r="I88" s="123"/>
+      <c r="A88" s="112"/>
+      <c r="B88" s="112"/>
+      <c r="C88" s="112"/>
+      <c r="D88" s="112"/>
+      <c r="E88" s="112"/>
+      <c r="F88" s="112"/>
+      <c r="G88" s="112"/>
+      <c r="H88" s="112"/>
+      <c r="I88" s="117"/>
     </row>
     <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="118"/>
-      <c r="B89" s="118"/>
-      <c r="C89" s="118"/>
-      <c r="D89" s="118"/>
-      <c r="E89" s="118"/>
-      <c r="F89" s="118"/>
-      <c r="G89" s="118"/>
-      <c r="H89" s="118"/>
-      <c r="I89" s="123"/>
+      <c r="A89" s="112"/>
+      <c r="B89" s="112"/>
+      <c r="C89" s="112"/>
+      <c r="D89" s="112"/>
+      <c r="E89" s="112"/>
+      <c r="F89" s="112"/>
+      <c r="G89" s="112"/>
+      <c r="H89" s="112"/>
+      <c r="I89" s="117"/>
     </row>
     <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="118"/>
-      <c r="B90" s="118"/>
-      <c r="C90" s="118"/>
-      <c r="D90" s="118"/>
-      <c r="E90" s="118"/>
-      <c r="F90" s="118"/>
-      <c r="G90" s="118"/>
-      <c r="H90" s="118"/>
-      <c r="I90" s="123"/>
+      <c r="A90" s="112"/>
+      <c r="B90" s="112"/>
+      <c r="C90" s="112"/>
+      <c r="D90" s="112"/>
+      <c r="E90" s="112"/>
+      <c r="F90" s="112"/>
+      <c r="G90" s="112"/>
+      <c r="H90" s="112"/>
+      <c r="I90" s="117"/>
     </row>
     <row r="91" spans="1:9" ht="15.75">
-      <c r="A91" s="118"/>
-      <c r="B91" s="118"/>
-      <c r="C91" s="118"/>
-      <c r="D91" s="118"/>
-      <c r="E91" s="118"/>
-      <c r="F91" s="118"/>
-      <c r="G91" s="118"/>
-      <c r="H91" s="118"/>
-      <c r="I91" s="123"/>
+      <c r="A91" s="112"/>
+      <c r="B91" s="112"/>
+      <c r="C91" s="112"/>
+      <c r="D91" s="112"/>
+      <c r="E91" s="112"/>
+      <c r="F91" s="112"/>
+      <c r="G91" s="112"/>
+      <c r="H91" s="112"/>
+      <c r="I91" s="117"/>
     </row>
     <row r="92" spans="1:9" ht="15.75">
-      <c r="A92" s="118"/>
-      <c r="B92" s="118"/>
-      <c r="C92" s="118"/>
-      <c r="D92" s="118"/>
-      <c r="E92" s="118"/>
-      <c r="F92" s="118"/>
-      <c r="G92" s="118"/>
-      <c r="H92" s="118"/>
-      <c r="I92" s="123"/>
+      <c r="A92" s="112"/>
+      <c r="B92" s="112"/>
+      <c r="C92" s="112"/>
+      <c r="D92" s="112"/>
+      <c r="E92" s="112"/>
+      <c r="F92" s="112"/>
+      <c r="G92" s="112"/>
+      <c r="H92" s="112"/>
+      <c r="I92" s="117"/>
     </row>
     <row r="93" spans="1:9" ht="15.75">
-      <c r="A93" s="118"/>
-      <c r="B93" s="118"/>
-      <c r="C93" s="118"/>
-      <c r="D93" s="118"/>
-      <c r="E93" s="118"/>
-      <c r="F93" s="118"/>
-      <c r="G93" s="118"/>
-      <c r="H93" s="118"/>
-      <c r="I93" s="123"/>
+      <c r="A93" s="112"/>
+      <c r="B93" s="112"/>
+      <c r="C93" s="112"/>
+      <c r="D93" s="112"/>
+      <c r="E93" s="112"/>
+      <c r="F93" s="112"/>
+      <c r="G93" s="112"/>
+      <c r="H93" s="112"/>
+      <c r="I93" s="117"/>
     </row>
     <row r="94" spans="1:9" ht="15.75">
-      <c r="A94" s="118"/>
-      <c r="B94" s="118"/>
-      <c r="C94" s="118"/>
-      <c r="D94" s="118"/>
-      <c r="E94" s="118"/>
-      <c r="F94" s="118"/>
-      <c r="G94" s="118"/>
-      <c r="H94" s="118"/>
-      <c r="I94" s="123"/>
+      <c r="A94" s="112"/>
+      <c r="B94" s="112"/>
+      <c r="C94" s="112"/>
+      <c r="D94" s="112"/>
+      <c r="E94" s="112"/>
+      <c r="F94" s="112"/>
+      <c r="G94" s="112"/>
+      <c r="H94" s="112"/>
+      <c r="I94" s="117"/>
     </row>
     <row r="95" spans="1:9" ht="15.75">
-      <c r="A95" s="118"/>
-      <c r="B95" s="118"/>
-      <c r="C95" s="118"/>
-      <c r="D95" s="118"/>
-      <c r="E95" s="118"/>
-      <c r="F95" s="118"/>
-      <c r="G95" s="118"/>
-      <c r="H95" s="118"/>
-      <c r="I95" s="123"/>
+      <c r="A95" s="112"/>
+      <c r="B95" s="112"/>
+      <c r="C95" s="112"/>
+      <c r="D95" s="112"/>
+      <c r="E95" s="112"/>
+      <c r="F95" s="112"/>
+      <c r="G95" s="112"/>
+      <c r="H95" s="112"/>
+      <c r="I95" s="117"/>
     </row>
     <row r="96" spans="1:9" ht="15.75">
-      <c r="A96" s="118"/>
-      <c r="B96" s="118"/>
-      <c r="C96" s="118"/>
-      <c r="D96" s="118"/>
-      <c r="E96" s="118"/>
-      <c r="F96" s="118"/>
-      <c r="G96" s="118"/>
-      <c r="H96" s="118"/>
-      <c r="I96" s="123"/>
+      <c r="A96" s="112"/>
+      <c r="B96" s="112"/>
+      <c r="C96" s="112"/>
+      <c r="D96" s="112"/>
+      <c r="E96" s="112"/>
+      <c r="F96" s="112"/>
+      <c r="G96" s="112"/>
+      <c r="H96" s="112"/>
+      <c r="I96" s="117"/>
     </row>
     <row r="97" spans="1:9" ht="15.75">
-      <c r="A97" s="118"/>
-      <c r="B97" s="118"/>
-      <c r="C97" s="118"/>
-      <c r="D97" s="118"/>
-      <c r="E97" s="118"/>
-      <c r="F97" s="118"/>
-      <c r="G97" s="118"/>
-      <c r="H97" s="118"/>
-      <c r="I97" s="123"/>
+      <c r="A97" s="112"/>
+      <c r="B97" s="112"/>
+      <c r="C97" s="112"/>
+      <c r="D97" s="112"/>
+      <c r="E97" s="112"/>
+      <c r="F97" s="112"/>
+      <c r="G97" s="112"/>
+      <c r="H97" s="112"/>
+      <c r="I97" s="117"/>
     </row>
     <row r="98" spans="1:9" ht="15.75">
-      <c r="A98" s="118"/>
-      <c r="B98" s="118"/>
-      <c r="C98" s="118"/>
-      <c r="D98" s="118"/>
-      <c r="E98" s="118"/>
-      <c r="F98" s="118"/>
-      <c r="G98" s="118"/>
-      <c r="H98" s="118"/>
-      <c r="I98" s="123"/>
+      <c r="A98" s="112"/>
+      <c r="B98" s="112"/>
+      <c r="C98" s="112"/>
+      <c r="D98" s="112"/>
+      <c r="E98" s="112"/>
+      <c r="F98" s="112"/>
+      <c r="G98" s="112"/>
+      <c r="H98" s="112"/>
+      <c r="I98" s="117"/>
     </row>
     <row r="99" spans="1:9" ht="15.75">
-      <c r="A99" s="118"/>
-      <c r="B99" s="118"/>
-      <c r="C99" s="118"/>
-      <c r="D99" s="118"/>
-      <c r="E99" s="118"/>
-      <c r="F99" s="118"/>
-      <c r="G99" s="118"/>
-      <c r="H99" s="118"/>
-      <c r="I99" s="123"/>
+      <c r="A99" s="112"/>
+      <c r="B99" s="112"/>
+      <c r="C99" s="112"/>
+      <c r="D99" s="112"/>
+      <c r="E99" s="112"/>
+      <c r="F99" s="112"/>
+      <c r="G99" s="112"/>
+      <c r="H99" s="112"/>
+      <c r="I99" s="117"/>
     </row>
     <row r="100" spans="1:9" ht="15.75">
-      <c r="A100" s="118"/>
-      <c r="B100" s="118"/>
-      <c r="C100" s="118"/>
-      <c r="D100" s="118"/>
-      <c r="E100" s="118"/>
-      <c r="F100" s="118"/>
-      <c r="G100" s="118"/>
-      <c r="H100" s="118"/>
-      <c r="I100" s="123"/>
+      <c r="A100" s="112"/>
+      <c r="B100" s="112"/>
+      <c r="C100" s="112"/>
+      <c r="D100" s="112"/>
+      <c r="E100" s="112"/>
+      <c r="F100" s="112"/>
+      <c r="G100" s="112"/>
+      <c r="H100" s="112"/>
+      <c r="I100" s="117"/>
     </row>
     <row r="101" spans="1:9" ht="15.75">
-      <c r="A101" s="118"/>
-      <c r="B101" s="118"/>
-      <c r="C101" s="118"/>
-      <c r="D101" s="118"/>
-      <c r="E101" s="118"/>
-      <c r="F101" s="118"/>
-      <c r="G101" s="118"/>
-      <c r="H101" s="118"/>
-      <c r="I101" s="123"/>
+      <c r="A101" s="112"/>
+      <c r="B101" s="112"/>
+      <c r="C101" s="112"/>
+      <c r="D101" s="112"/>
+      <c r="E101" s="112"/>
+      <c r="F101" s="112"/>
+      <c r="G101" s="112"/>
+      <c r="H101" s="112"/>
+      <c r="I101" s="117"/>
     </row>
     <row r="102" spans="1:9" ht="15.75">
-      <c r="A102" s="118"/>
-      <c r="B102" s="118"/>
-      <c r="C102" s="118"/>
-      <c r="D102" s="118"/>
-      <c r="E102" s="118"/>
-      <c r="F102" s="118"/>
-      <c r="G102" s="118"/>
-      <c r="H102" s="118"/>
-      <c r="I102" s="123"/>
+      <c r="A102" s="112"/>
+      <c r="B102" s="112"/>
+      <c r="C102" s="112"/>
+      <c r="D102" s="112"/>
+      <c r="E102" s="112"/>
+      <c r="F102" s="112"/>
+      <c r="G102" s="112"/>
+      <c r="H102" s="112"/>
+      <c r="I102" s="117"/>
     </row>
     <row r="103" spans="1:9" ht="15.75">
-      <c r="A103" s="118"/>
-      <c r="B103" s="118"/>
-      <c r="C103" s="118"/>
-      <c r="D103" s="118"/>
-      <c r="E103" s="118"/>
-      <c r="F103" s="118"/>
-      <c r="G103" s="118"/>
-      <c r="H103" s="118"/>
-      <c r="I103" s="123"/>
+      <c r="A103" s="112"/>
+      <c r="B103" s="112"/>
+      <c r="C103" s="112"/>
+      <c r="D103" s="112"/>
+      <c r="E103" s="112"/>
+      <c r="F103" s="112"/>
+      <c r="G103" s="112"/>
+      <c r="H103" s="112"/>
+      <c r="I103" s="117"/>
     </row>
     <row r="104" spans="1:9" ht="15.75">
-      <c r="A104" s="118"/>
-      <c r="B104" s="118"/>
-      <c r="C104" s="118"/>
-      <c r="D104" s="118"/>
-      <c r="E104" s="118"/>
-      <c r="F104" s="118"/>
-      <c r="G104" s="118"/>
-      <c r="H104" s="118"/>
-      <c r="I104" s="123"/>
+      <c r="A104" s="112"/>
+      <c r="B104" s="112"/>
+      <c r="C104" s="112"/>
+      <c r="D104" s="112"/>
+      <c r="E104" s="112"/>
+      <c r="F104" s="112"/>
+      <c r="G104" s="112"/>
+      <c r="H104" s="112"/>
+      <c r="I104" s="117"/>
     </row>
     <row r="105" spans="1:9" ht="15.75">
-      <c r="A105" s="118"/>
-      <c r="B105" s="118"/>
-      <c r="C105" s="118"/>
-      <c r="D105" s="118"/>
-      <c r="E105" s="118"/>
-      <c r="F105" s="118"/>
-      <c r="G105" s="118"/>
-      <c r="H105" s="118"/>
-      <c r="I105" s="123"/>
+      <c r="A105" s="112"/>
+      <c r="B105" s="112"/>
+      <c r="C105" s="112"/>
+      <c r="D105" s="112"/>
+      <c r="E105" s="112"/>
+      <c r="F105" s="112"/>
+      <c r="G105" s="112"/>
+      <c r="H105" s="112"/>
+      <c r="I105" s="117"/>
     </row>
     <row r="106" spans="1:9" ht="15.75">
-      <c r="A106" s="118"/>
-      <c r="B106" s="118"/>
-      <c r="C106" s="118"/>
-      <c r="D106" s="118"/>
-      <c r="E106" s="118"/>
-      <c r="F106" s="118"/>
-      <c r="G106" s="118"/>
-      <c r="H106" s="118"/>
-      <c r="I106" s="123"/>
+      <c r="A106" s="112"/>
+      <c r="B106" s="112"/>
+      <c r="C106" s="112"/>
+      <c r="D106" s="112"/>
+      <c r="E106" s="112"/>
+      <c r="F106" s="112"/>
+      <c r="G106" s="112"/>
+      <c r="H106" s="112"/>
+      <c r="I106" s="117"/>
     </row>
     <row r="107" spans="1:9" ht="15.75">
-      <c r="A107" s="118"/>
-      <c r="B107" s="118"/>
-      <c r="C107" s="118"/>
-      <c r="D107" s="118"/>
-      <c r="E107" s="118"/>
-      <c r="F107" s="118"/>
-      <c r="G107" s="118"/>
-      <c r="H107" s="118"/>
-      <c r="I107" s="123"/>
+      <c r="A107" s="112"/>
+      <c r="B107" s="112"/>
+      <c r="C107" s="112"/>
+      <c r="D107" s="112"/>
+      <c r="E107" s="112"/>
+      <c r="F107" s="112"/>
+      <c r="G107" s="112"/>
+      <c r="H107" s="112"/>
+      <c r="I107" s="117"/>
     </row>
     <row r="108" spans="1:9" ht="15.75">
-      <c r="A108" s="118"/>
-      <c r="B108" s="118"/>
-      <c r="C108" s="118"/>
-      <c r="D108" s="118"/>
-      <c r="E108" s="118"/>
-      <c r="F108" s="118"/>
-      <c r="G108" s="118"/>
-      <c r="H108" s="118"/>
-      <c r="I108" s="123"/>
+      <c r="A108" s="112"/>
+      <c r="B108" s="112"/>
+      <c r="C108" s="112"/>
+      <c r="D108" s="112"/>
+      <c r="E108" s="112"/>
+      <c r="F108" s="112"/>
+      <c r="G108" s="112"/>
+      <c r="H108" s="112"/>
+      <c r="I108" s="117"/>
     </row>
     <row r="109" spans="1:9" ht="15.75">
-      <c r="A109" s="118"/>
-      <c r="B109" s="118"/>
-      <c r="C109" s="118"/>
-      <c r="D109" s="118"/>
-      <c r="E109" s="118"/>
-      <c r="F109" s="118"/>
-      <c r="G109" s="118"/>
-      <c r="H109" s="118"/>
-      <c r="I109" s="123"/>
+      <c r="A109" s="112"/>
+      <c r="B109" s="112"/>
+      <c r="C109" s="112"/>
+      <c r="D109" s="112"/>
+      <c r="E109" s="112"/>
+      <c r="F109" s="112"/>
+      <c r="G109" s="112"/>
+      <c r="H109" s="112"/>
+      <c r="I109" s="117"/>
     </row>
     <row r="110" spans="1:9" ht="15.75">
-      <c r="A110" s="118"/>
-      <c r="B110" s="118"/>
-      <c r="C110" s="118"/>
-      <c r="D110" s="118"/>
-      <c r="E110" s="118"/>
-      <c r="F110" s="118"/>
-      <c r="G110" s="118"/>
-      <c r="H110" s="118"/>
-      <c r="I110" s="123"/>
+      <c r="A110" s="112"/>
+      <c r="B110" s="112"/>
+      <c r="C110" s="112"/>
+      <c r="D110" s="112"/>
+      <c r="E110" s="112"/>
+      <c r="F110" s="112"/>
+      <c r="G110" s="112"/>
+      <c r="H110" s="112"/>
+      <c r="I110" s="117"/>
     </row>
     <row r="111" spans="1:9" ht="15.75">
-      <c r="A111" s="118"/>
-      <c r="B111" s="118"/>
-      <c r="C111" s="118"/>
-      <c r="D111" s="118"/>
-      <c r="E111" s="118"/>
-      <c r="F111" s="118"/>
-      <c r="G111" s="118"/>
-      <c r="H111" s="118"/>
-      <c r="I111" s="123"/>
+      <c r="A111" s="112"/>
+      <c r="B111" s="112"/>
+      <c r="C111" s="112"/>
+      <c r="D111" s="112"/>
+      <c r="E111" s="112"/>
+      <c r="F111" s="112"/>
+      <c r="G111" s="112"/>
+      <c r="H111" s="112"/>
+      <c r="I111" s="117"/>
     </row>
     <row r="112" spans="1:9" ht="15.75">
-      <c r="A112" s="118"/>
-      <c r="B112" s="118"/>
-      <c r="C112" s="118"/>
-      <c r="D112" s="118"/>
-      <c r="E112" s="118"/>
-      <c r="F112" s="118"/>
-      <c r="G112" s="118"/>
-      <c r="H112" s="118"/>
-      <c r="I112" s="123"/>
+      <c r="A112" s="112"/>
+      <c r="B112" s="112"/>
+      <c r="C112" s="112"/>
+      <c r="D112" s="112"/>
+      <c r="E112" s="112"/>
+      <c r="F112" s="112"/>
+      <c r="G112" s="112"/>
+      <c r="H112" s="112"/>
+      <c r="I112" s="117"/>
     </row>
     <row r="113" spans="1:9" ht="15.75">
-      <c r="A113" s="118"/>
-      <c r="B113" s="118"/>
-      <c r="C113" s="118"/>
-      <c r="D113" s="118"/>
-      <c r="E113" s="118"/>
-      <c r="F113" s="118"/>
-      <c r="G113" s="118"/>
-      <c r="H113" s="118"/>
-      <c r="I113" s="123"/>
+      <c r="A113" s="112"/>
+      <c r="B113" s="112"/>
+      <c r="C113" s="112"/>
+      <c r="D113" s="112"/>
+      <c r="E113" s="112"/>
+      <c r="F113" s="112"/>
+      <c r="G113" s="112"/>
+      <c r="H113" s="112"/>
+      <c r="I113" s="117"/>
     </row>
     <row r="114" spans="1:9" ht="15.75">
-      <c r="A114" s="118"/>
-      <c r="B114" s="118"/>
-      <c r="C114" s="118"/>
-      <c r="D114" s="118"/>
-      <c r="E114" s="118"/>
-      <c r="F114" s="118"/>
-      <c r="G114" s="118"/>
-      <c r="H114" s="118"/>
-      <c r="I114" s="123"/>
+      <c r="A114" s="112"/>
+      <c r="B114" s="112"/>
+      <c r="C114" s="112"/>
+      <c r="D114" s="112"/>
+      <c r="E114" s="112"/>
+      <c r="F114" s="112"/>
+      <c r="G114" s="112"/>
+      <c r="H114" s="112"/>
+      <c r="I114" s="117"/>
     </row>
     <row r="115" spans="1:9" ht="15.75">
-      <c r="A115" s="118"/>
-      <c r="B115" s="118"/>
-      <c r="C115" s="118"/>
-      <c r="D115" s="118"/>
-      <c r="E115" s="118"/>
-      <c r="F115" s="118"/>
-      <c r="G115" s="118"/>
-      <c r="H115" s="118"/>
-      <c r="I115" s="123"/>
+      <c r="A115" s="112"/>
+      <c r="B115" s="112"/>
+      <c r="C115" s="112"/>
+      <c r="D115" s="112"/>
+      <c r="E115" s="112"/>
+      <c r="F115" s="112"/>
+      <c r="G115" s="112"/>
+      <c r="H115" s="112"/>
+      <c r="I115" s="117"/>
     </row>
     <row r="116" spans="1:9" ht="15.75">
-      <c r="A116" s="118"/>
-      <c r="B116" s="118"/>
-      <c r="C116" s="118"/>
-      <c r="D116" s="118"/>
-      <c r="E116" s="118"/>
-      <c r="F116" s="118"/>
-      <c r="G116" s="118"/>
-      <c r="H116" s="118"/>
-      <c r="I116" s="123"/>
+      <c r="A116" s="112"/>
+      <c r="B116" s="112"/>
+      <c r="C116" s="112"/>
+      <c r="D116" s="112"/>
+      <c r="E116" s="112"/>
+      <c r="F116" s="112"/>
+      <c r="G116" s="112"/>
+      <c r="H116" s="112"/>
+      <c r="I116" s="117"/>
     </row>
     <row r="117" spans="1:9" ht="15.75">
-      <c r="A117" s="118"/>
-      <c r="B117" s="118"/>
-      <c r="C117" s="118"/>
-      <c r="D117" s="118"/>
-      <c r="E117" s="118"/>
-      <c r="F117" s="118"/>
-      <c r="G117" s="118"/>
-      <c r="H117" s="118"/>
-      <c r="I117" s="123"/>
+      <c r="A117" s="112"/>
+      <c r="B117" s="112"/>
+      <c r="C117" s="112"/>
+      <c r="D117" s="112"/>
+      <c r="E117" s="112"/>
+      <c r="F117" s="112"/>
+      <c r="G117" s="112"/>
+      <c r="H117" s="112"/>
+      <c r="I117" s="117"/>
     </row>
     <row r="118" spans="1:9" ht="15.75">
-      <c r="A118" s="118"/>
-      <c r="B118" s="118"/>
-      <c r="C118" s="118"/>
-      <c r="D118" s="118"/>
-      <c r="E118" s="118"/>
-      <c r="F118" s="118"/>
-      <c r="G118" s="118"/>
-      <c r="H118" s="118"/>
-      <c r="I118" s="123"/>
+      <c r="A118" s="112"/>
+      <c r="B118" s="112"/>
+      <c r="C118" s="112"/>
+      <c r="D118" s="112"/>
+      <c r="E118" s="112"/>
+      <c r="F118" s="112"/>
+      <c r="G118" s="112"/>
+      <c r="H118" s="112"/>
+      <c r="I118" s="117"/>
     </row>
     <row r="119" spans="1:9" ht="15.75">
-      <c r="A119" s="118"/>
-      <c r="B119" s="118"/>
-      <c r="C119" s="118"/>
-      <c r="D119" s="118"/>
-      <c r="E119" s="118"/>
-      <c r="F119" s="118"/>
-      <c r="G119" s="118"/>
-      <c r="H119" s="118"/>
-      <c r="I119" s="123"/>
+      <c r="A119" s="112"/>
+      <c r="B119" s="112"/>
+      <c r="C119" s="112"/>
+      <c r="D119" s="112"/>
+      <c r="E119" s="112"/>
+      <c r="F119" s="112"/>
+      <c r="G119" s="112"/>
+      <c r="H119" s="112"/>
+      <c r="I119" s="117"/>
     </row>
     <row r="120" spans="1:9" ht="15.75">
-      <c r="A120" s="118"/>
-      <c r="B120" s="118"/>
-      <c r="C120" s="118"/>
-      <c r="D120" s="118"/>
-      <c r="E120" s="118"/>
-      <c r="F120" s="118"/>
-      <c r="G120" s="118"/>
-      <c r="H120" s="118"/>
-      <c r="I120" s="123"/>
+      <c r="A120" s="112"/>
+      <c r="B120" s="112"/>
+      <c r="C120" s="112"/>
+      <c r="D120" s="112"/>
+      <c r="E120" s="112"/>
+      <c r="F120" s="112"/>
+      <c r="G120" s="112"/>
+      <c r="H120" s="112"/>
+      <c r="I120" s="117"/>
     </row>
     <row r="121" spans="1:9" ht="15.75">
-      <c r="A121" s="118"/>
-      <c r="B121" s="118"/>
-      <c r="C121" s="118"/>
-      <c r="D121" s="118"/>
-      <c r="E121" s="118"/>
-      <c r="F121" s="118"/>
-      <c r="G121" s="118"/>
-      <c r="H121" s="118"/>
-      <c r="I121" s="123"/>
+      <c r="A121" s="112"/>
+      <c r="B121" s="112"/>
+      <c r="C121" s="112"/>
+      <c r="D121" s="112"/>
+      <c r="E121" s="112"/>
+      <c r="F121" s="112"/>
+      <c r="G121" s="112"/>
+      <c r="H121" s="112"/>
+      <c r="I121" s="117"/>
     </row>
     <row r="122" spans="1:9" ht="15.75">
-      <c r="A122" s="118"/>
-      <c r="B122" s="118"/>
-      <c r="C122" s="118"/>
-      <c r="D122" s="118"/>
-      <c r="E122" s="118"/>
-      <c r="F122" s="118"/>
-      <c r="G122" s="118"/>
-      <c r="H122" s="118"/>
-      <c r="I122" s="123"/>
+      <c r="A122" s="112"/>
+      <c r="B122" s="112"/>
+      <c r="C122" s="112"/>
+      <c r="D122" s="112"/>
+      <c r="E122" s="112"/>
+      <c r="F122" s="112"/>
+      <c r="G122" s="112"/>
+      <c r="H122" s="112"/>
+      <c r="I122" s="117"/>
     </row>
     <row r="123" spans="1:9" ht="15.75">
-      <c r="A123" s="118"/>
-      <c r="B123" s="118"/>
-      <c r="C123" s="118"/>
-      <c r="D123" s="118"/>
-      <c r="E123" s="118"/>
-      <c r="F123" s="118"/>
-      <c r="G123" s="118"/>
-      <c r="H123" s="118"/>
-      <c r="I123" s="123"/>
+      <c r="A123" s="112"/>
+      <c r="B123" s="112"/>
+      <c r="C123" s="112"/>
+      <c r="D123" s="112"/>
+      <c r="E123" s="112"/>
+      <c r="F123" s="112"/>
+      <c r="G123" s="112"/>
+      <c r="H123" s="112"/>
+      <c r="I123" s="117"/>
     </row>
     <row r="124" spans="1:9" ht="15.75">
-      <c r="A124" s="118"/>
-      <c r="B124" s="118"/>
-      <c r="C124" s="118"/>
-      <c r="D124" s="118"/>
-      <c r="E124" s="118"/>
-      <c r="F124" s="118"/>
-      <c r="G124" s="118"/>
-      <c r="H124" s="118"/>
-      <c r="I124" s="123"/>
+      <c r="A124" s="112"/>
+      <c r="B124" s="112"/>
+      <c r="C124" s="112"/>
+      <c r="D124" s="112"/>
+      <c r="E124" s="112"/>
+      <c r="F124" s="112"/>
+      <c r="G124" s="112"/>
+      <c r="H124" s="112"/>
+      <c r="I124" s="117"/>
     </row>
     <row r="125" spans="1:9" ht="15.75">
-      <c r="A125" s="118"/>
-      <c r="B125" s="118"/>
-      <c r="C125" s="118"/>
-      <c r="D125" s="118"/>
-      <c r="E125" s="118"/>
-      <c r="F125" s="118"/>
-      <c r="G125" s="118"/>
-      <c r="H125" s="118"/>
-      <c r="I125" s="123"/>
+      <c r="A125" s="112"/>
+      <c r="B125" s="112"/>
+      <c r="C125" s="112"/>
+      <c r="D125" s="112"/>
+      <c r="E125" s="112"/>
+      <c r="F125" s="112"/>
+      <c r="G125" s="112"/>
+      <c r="H125" s="112"/>
+      <c r="I125" s="117"/>
     </row>
     <row r="126" spans="1:9" ht="15.75">
-      <c r="A126" s="118"/>
-      <c r="B126" s="118"/>
-      <c r="C126" s="118"/>
-      <c r="D126" s="118"/>
-      <c r="E126" s="118"/>
-      <c r="F126" s="118"/>
-      <c r="G126" s="118"/>
-      <c r="H126" s="118"/>
-      <c r="I126" s="123"/>
+      <c r="A126" s="112"/>
+      <c r="B126" s="112"/>
+      <c r="C126" s="112"/>
+      <c r="D126" s="112"/>
+      <c r="E126" s="112"/>
+      <c r="F126" s="112"/>
+      <c r="G126" s="112"/>
+      <c r="H126" s="112"/>
+      <c r="I126" s="117"/>
     </row>
     <row r="127" spans="1:9" ht="15.75">
-      <c r="A127" s="118"/>
-      <c r="B127" s="118"/>
-      <c r="C127" s="118"/>
-      <c r="D127" s="118"/>
-      <c r="E127" s="118"/>
-      <c r="F127" s="118"/>
-      <c r="G127" s="118"/>
-      <c r="H127" s="118"/>
-      <c r="I127" s="123"/>
+      <c r="A127" s="112"/>
+      <c r="B127" s="112"/>
+      <c r="C127" s="112"/>
+      <c r="D127" s="112"/>
+      <c r="E127" s="112"/>
+      <c r="F127" s="112"/>
+      <c r="G127" s="112"/>
+      <c r="H127" s="112"/>
+      <c r="I127" s="117"/>
     </row>
     <row r="128" spans="1:9" ht="15.75">
-      <c r="A128" s="118"/>
-      <c r="B128" s="118"/>
-      <c r="C128" s="118"/>
-      <c r="D128" s="118"/>
-      <c r="E128" s="118"/>
-      <c r="F128" s="118"/>
-      <c r="G128" s="118"/>
-      <c r="H128" s="118"/>
-      <c r="I128" s="123"/>
+      <c r="A128" s="112"/>
+      <c r="B128" s="112"/>
+      <c r="C128" s="112"/>
+      <c r="D128" s="112"/>
+      <c r="E128" s="112"/>
+      <c r="F128" s="112"/>
+      <c r="G128" s="112"/>
+      <c r="H128" s="112"/>
+      <c r="I128" s="117"/>
     </row>
     <row r="129" spans="1:9" ht="15.75">
-      <c r="A129" s="118"/>
-      <c r="B129" s="118"/>
-      <c r="C129" s="118"/>
-      <c r="D129" s="118"/>
-      <c r="E129" s="118"/>
-      <c r="F129" s="118"/>
-      <c r="G129" s="118"/>
-      <c r="H129" s="118"/>
-      <c r="I129" s="123"/>
+      <c r="A129" s="112"/>
+      <c r="B129" s="112"/>
+      <c r="C129" s="112"/>
+      <c r="D129" s="112"/>
+      <c r="E129" s="112"/>
+      <c r="F129" s="112"/>
+      <c r="G129" s="112"/>
+      <c r="H129" s="112"/>
+      <c r="I129" s="117"/>
     </row>
     <row r="130" spans="1:9" ht="15.75">
-      <c r="A130" s="118"/>
-      <c r="B130" s="118"/>
-      <c r="C130" s="118"/>
-      <c r="D130" s="118"/>
-      <c r="E130" s="118"/>
-      <c r="F130" s="118"/>
-      <c r="G130" s="118"/>
-      <c r="H130" s="118"/>
-      <c r="I130" s="123"/>
+      <c r="A130" s="112"/>
+      <c r="B130" s="112"/>
+      <c r="C130" s="112"/>
+      <c r="D130" s="112"/>
+      <c r="E130" s="112"/>
+      <c r="F130" s="112"/>
+      <c r="G130" s="112"/>
+      <c r="H130" s="112"/>
+      <c r="I130" s="117"/>
     </row>
     <row r="131" spans="1:9" ht="15.75">
-      <c r="A131" s="118"/>
-      <c r="B131" s="118"/>
-      <c r="C131" s="118"/>
-      <c r="D131" s="118"/>
-      <c r="E131" s="118"/>
-      <c r="F131" s="118"/>
-      <c r="G131" s="118"/>
-      <c r="H131" s="118"/>
-      <c r="I131" s="123"/>
+      <c r="A131" s="112"/>
+      <c r="B131" s="112"/>
+      <c r="C131" s="112"/>
+      <c r="D131" s="112"/>
+      <c r="E131" s="112"/>
+      <c r="F131" s="112"/>
+      <c r="G131" s="112"/>
+      <c r="H131" s="112"/>
+      <c r="I131" s="117"/>
     </row>
     <row r="132" spans="1:9" ht="15.75">
-      <c r="A132" s="118"/>
-      <c r="B132" s="118"/>
-      <c r="C132" s="118"/>
-      <c r="D132" s="118"/>
-      <c r="E132" s="118"/>
-      <c r="F132" s="118"/>
-      <c r="G132" s="118"/>
-      <c r="H132" s="118"/>
-      <c r="I132" s="123"/>
+      <c r="A132" s="112"/>
+      <c r="B132" s="112"/>
+      <c r="C132" s="112"/>
+      <c r="D132" s="112"/>
+      <c r="E132" s="112"/>
+      <c r="F132" s="112"/>
+      <c r="G132" s="112"/>
+      <c r="H132" s="112"/>
+      <c r="I132" s="117"/>
     </row>
     <row r="133" spans="1:9" ht="15.75">
-      <c r="A133" s="118"/>
-      <c r="B133" s="118"/>
-      <c r="C133" s="118"/>
-      <c r="D133" s="118"/>
-      <c r="E133" s="118"/>
-      <c r="F133" s="118"/>
-      <c r="G133" s="118"/>
-      <c r="H133" s="118"/>
-      <c r="I133" s="123"/>
+      <c r="A133" s="112"/>
+      <c r="B133" s="112"/>
+      <c r="C133" s="112"/>
+      <c r="D133" s="112"/>
+      <c r="E133" s="112"/>
+      <c r="F133" s="112"/>
+      <c r="G133" s="112"/>
+      <c r="H133" s="112"/>
+      <c r="I133" s="117"/>
     </row>
     <row r="134" spans="1:9" ht="15.75">
-      <c r="A134" s="118"/>
-      <c r="B134" s="118"/>
-      <c r="C134" s="118"/>
-      <c r="D134" s="118"/>
-      <c r="E134" s="118"/>
-      <c r="F134" s="118"/>
-      <c r="G134" s="118"/>
-      <c r="H134" s="118"/>
-      <c r="I134" s="123"/>
+      <c r="A134" s="112"/>
+      <c r="B134" s="112"/>
+      <c r="C134" s="112"/>
+      <c r="D134" s="112"/>
+      <c r="E134" s="112"/>
+      <c r="F134" s="112"/>
+      <c r="G134" s="112"/>
+      <c r="H134" s="112"/>
+      <c r="I134" s="117"/>
     </row>
     <row r="135" spans="1:9" ht="15.75">
-      <c r="A135" s="118"/>
-      <c r="B135" s="118"/>
-      <c r="C135" s="118"/>
-      <c r="D135" s="118"/>
-      <c r="E135" s="118"/>
-      <c r="F135" s="118"/>
-      <c r="G135" s="118"/>
-      <c r="H135" s="118"/>
-      <c r="I135" s="123"/>
+      <c r="A135" s="112"/>
+      <c r="B135" s="112"/>
+      <c r="C135" s="112"/>
+      <c r="D135" s="112"/>
+      <c r="E135" s="112"/>
+      <c r="F135" s="112"/>
+      <c r="G135" s="112"/>
+      <c r="H135" s="112"/>
+      <c r="I135" s="117"/>
     </row>
     <row r="136" spans="1:9" ht="15.75">
-      <c r="A136" s="118"/>
-      <c r="B136" s="118"/>
-      <c r="C136" s="118"/>
-      <c r="D136" s="118"/>
-      <c r="E136" s="118"/>
-      <c r="F136" s="118"/>
-      <c r="G136" s="118"/>
-      <c r="H136" s="118"/>
-      <c r="I136" s="123"/>
+      <c r="A136" s="112"/>
+      <c r="B136" s="112"/>
+      <c r="C136" s="112"/>
+      <c r="D136" s="112"/>
+      <c r="E136" s="112"/>
+      <c r="F136" s="112"/>
+      <c r="G136" s="112"/>
+      <c r="H136" s="112"/>
+      <c r="I136" s="117"/>
     </row>
     <row r="137" spans="1:9" ht="15.75">
-      <c r="A137" s="118"/>
-      <c r="B137" s="118"/>
-      <c r="C137" s="118"/>
-      <c r="D137" s="118"/>
-      <c r="E137" s="118"/>
-      <c r="F137" s="118"/>
-      <c r="G137" s="118"/>
-      <c r="H137" s="118"/>
-      <c r="I137" s="123"/>
+      <c r="A137" s="112"/>
+      <c r="B137" s="112"/>
+      <c r="C137" s="112"/>
+      <c r="D137" s="112"/>
+      <c r="E137" s="112"/>
+      <c r="F137" s="112"/>
+      <c r="G137" s="112"/>
+      <c r="H137" s="112"/>
+      <c r="I137" s="117"/>
     </row>
     <row r="138" spans="1:9" ht="15.75">
-      <c r="A138" s="118"/>
-      <c r="B138" s="118"/>
-      <c r="C138" s="118"/>
-      <c r="D138" s="118"/>
-      <c r="E138" s="118"/>
-      <c r="F138" s="118"/>
-      <c r="G138" s="118"/>
-      <c r="H138" s="118"/>
-      <c r="I138" s="123"/>
+      <c r="A138" s="112"/>
+      <c r="B138" s="112"/>
+      <c r="C138" s="112"/>
+      <c r="D138" s="112"/>
+      <c r="E138" s="112"/>
+      <c r="F138" s="112"/>
+      <c r="G138" s="112"/>
+      <c r="H138" s="112"/>
+      <c r="I138" s="117"/>
     </row>
     <row r="139" spans="1:9" ht="15.75">
-      <c r="A139" s="118"/>
-      <c r="B139" s="118"/>
-      <c r="C139" s="118"/>
-      <c r="D139" s="118"/>
-      <c r="E139" s="118"/>
-      <c r="F139" s="118"/>
-      <c r="G139" s="118"/>
-      <c r="H139" s="118"/>
-      <c r="I139" s="123"/>
+      <c r="A139" s="112"/>
+      <c r="B139" s="112"/>
+      <c r="C139" s="112"/>
+      <c r="D139" s="112"/>
+      <c r="E139" s="112"/>
+      <c r="F139" s="112"/>
+      <c r="G139" s="112"/>
+      <c r="H139" s="112"/>
+      <c r="I139" s="117"/>
     </row>
     <row r="140" spans="1:9" ht="15.75">
-      <c r="A140" s="118"/>
-      <c r="B140" s="118"/>
-      <c r="C140" s="118"/>
-      <c r="D140" s="118"/>
-      <c r="E140" s="118"/>
-      <c r="F140" s="118"/>
-      <c r="G140" s="118"/>
-      <c r="H140" s="118"/>
-      <c r="I140" s="123"/>
+      <c r="A140" s="112"/>
+      <c r="B140" s="112"/>
+      <c r="C140" s="112"/>
+      <c r="D140" s="112"/>
+      <c r="E140" s="112"/>
+      <c r="F140" s="112"/>
+      <c r="G140" s="112"/>
+      <c r="H140" s="112"/>
+      <c r="I140" s="117"/>
     </row>
     <row r="141" spans="1:9" ht="15.75">
-      <c r="A141" s="118"/>
-      <c r="B141" s="118"/>
-      <c r="C141" s="118"/>
-      <c r="D141" s="118"/>
-      <c r="E141" s="118"/>
-      <c r="F141" s="118"/>
-      <c r="G141" s="118"/>
-      <c r="H141" s="118"/>
-      <c r="I141" s="118"/>
+      <c r="A141" s="112"/>
+      <c r="B141" s="112"/>
+      <c r="C141" s="112"/>
+      <c r="D141" s="112"/>
+      <c r="E141" s="112"/>
+      <c r="F141" s="112"/>
+      <c r="G141" s="112"/>
+      <c r="H141" s="112"/>
+      <c r="I141" s="112"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Functional Tests - System administration module.xlsx - Minor changes.
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\Testowanie Oprogramowania (10)\Documents\System administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF965292-8D6F-47C1-AE41-459A284EE5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDD6199-BAE7-4F26-9272-2A8733AE12D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29505" yWindow="2565" windowWidth="21960" windowHeight="13035" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="336">
   <si>
     <t>Test scenario</t>
   </si>
@@ -993,10 +993,6 @@
     <t>1. The user's details have been changed.</t>
   </si>
   <si>
-    <t>1. An administrator makes changes to the details of a selected user.
-2. An administrator saves the changes by pressint the "Accept" button.</t>
-  </si>
-  <si>
     <t>Succesful change of user details.</t>
   </si>
   <si>
@@ -1047,10 +1043,6 @@
     <t>1. The selected user has been activated.</t>
   </si>
   <si>
-    <t>1. An administrator makes changes to the details of a selected user.
-2. An administrator saves the changes by pressing the "Accept" button.</t>
-  </si>
-  <si>
     <t>1. An administrator presses the "Active" button in the "Status" column belonging to the selected user.
 2. An administrator confirms their will to deactivate the selected user by pressing  the "Accept" button.</t>
   </si>
@@ -1177,6 +1169,10 @@
   </si>
   <si>
     <t>UMG_01.01</t>
+  </si>
+  <si>
+    <t>1. An administrator makes changes to the details of a selected user.
+2. An administrator saves the changes by pressing the "Save" button.</t>
   </si>
 </sst>
 </file>
@@ -3402,7 +3398,7 @@
     </row>
     <row r="39" spans="1:13" ht="149.25" customHeight="1">
       <c r="A39" s="121" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B39" s="103" t="s">
         <v>258</v>
@@ -3414,7 +3410,7 @@
         <v>12</v>
       </c>
       <c r="E39" s="103" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F39" s="103" t="s">
         <v>260</v>
@@ -3423,13 +3419,13 @@
         <v>261</v>
       </c>
       <c r="H39" s="132" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I39" s="106" t="s">
         <v>264</v>
       </c>
       <c r="J39" s="106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K39" s="112" t="s">
         <v>262</v>
@@ -3446,7 +3442,7 @@
       <c r="F40" s="128"/>
       <c r="G40" s="89"/>
       <c r="H40" s="132" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I40" s="126" t="s">
         <v>263</v>
@@ -3469,7 +3465,7 @@
       <c r="F41" s="114"/>
       <c r="G41" s="88"/>
       <c r="H41" s="119" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I41" s="117" t="s">
         <v>263</v>
@@ -3485,7 +3481,7 @@
     </row>
     <row r="42" spans="1:13" ht="102" customHeight="1" thickBot="1">
       <c r="A42" s="134" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B42" s="126" t="s">
         <v>269</v>
@@ -3497,7 +3493,7 @@
         <v>12</v>
       </c>
       <c r="E42" s="126" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F42" s="126" t="s">
         <v>271</v>
@@ -3506,7 +3502,7 @@
         <v>272</v>
       </c>
       <c r="H42" s="132" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I42" s="126" t="s">
         <v>273</v>
@@ -3522,7 +3518,7 @@
     </row>
     <row r="43" spans="1:13" ht="123" customHeight="1">
       <c r="A43" s="121" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B43" s="103" t="s">
         <v>275</v>
@@ -3540,19 +3536,19 @@
         <v>278</v>
       </c>
       <c r="G43" s="87" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="H43" s="131" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I43" s="106" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J43" s="82" t="s">
-        <v>279</v>
+        <v>335</v>
       </c>
       <c r="K43" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L43" s="94"/>
       <c r="M43" s="94"/>
@@ -3566,53 +3562,53 @@
       <c r="F44" s="114"/>
       <c r="G44" s="88"/>
       <c r="H44" s="119" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I44" s="117" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J44" s="68" t="s">
+        <v>282</v>
+      </c>
+      <c r="K44" s="85" t="s">
         <v>283</v>
-      </c>
-      <c r="K44" s="85" t="s">
-        <v>284</v>
       </c>
       <c r="L44" s="94"/>
       <c r="M44" s="94"/>
     </row>
     <row r="45" spans="1:13" ht="66.75" customHeight="1">
       <c r="A45" s="121" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B45" s="103" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C45" s="103" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D45" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="103" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F45" s="103" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G45" s="87" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H45" s="131" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I45" s="106" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J45" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="K45" s="107" t="s">
         <v>307</v>
-      </c>
-      <c r="K45" s="107" t="s">
-        <v>309</v>
       </c>
       <c r="L45" s="94"/>
       <c r="M45" s="94"/>
@@ -3626,29 +3622,29 @@
       <c r="F46" s="114"/>
       <c r="G46" s="88"/>
       <c r="H46" s="119" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I46" s="117" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J46" s="126" t="s">
+        <v>310</v>
+      </c>
+      <c r="K46" s="122" t="s">
         <v>312</v>
-      </c>
-      <c r="K46" s="122" t="s">
-        <v>314</v>
       </c>
       <c r="L46" s="94"/>
       <c r="M46" s="94"/>
     </row>
     <row r="47" spans="1:13" ht="66.75" customHeight="1">
       <c r="A47" s="121" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" s="103" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C47" s="103" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D47" s="103" t="s">
         <v>12</v>
@@ -3657,22 +3653,22 @@
         <v>277</v>
       </c>
       <c r="F47" s="103" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G47" s="136" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H47" s="131" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I47" s="106" t="s">
+        <v>303</v>
+      </c>
+      <c r="J47" s="106" t="s">
         <v>305</v>
       </c>
-      <c r="J47" s="106" t="s">
+      <c r="K47" s="107" t="s">
         <v>307</v>
-      </c>
-      <c r="K47" s="107" t="s">
-        <v>309</v>
       </c>
       <c r="L47" s="94"/>
       <c r="M47" s="94"/>
@@ -3686,53 +3682,53 @@
       <c r="F48" s="114"/>
       <c r="G48" s="137"/>
       <c r="H48" s="119" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I48" s="126" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J48" s="117" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K48" s="122" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L48" s="94"/>
       <c r="M48" s="94"/>
     </row>
     <row r="49" spans="1:13" ht="66.75" customHeight="1">
       <c r="A49" s="121" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B49" s="103" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C49" s="103" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D49" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="103" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F49" s="103" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G49" s="136" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H49" s="131" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I49" s="106" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J49" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="K49" s="107" t="s">
         <v>308</v>
-      </c>
-      <c r="K49" s="107" t="s">
-        <v>310</v>
       </c>
       <c r="L49" s="94"/>
       <c r="M49" s="94"/>
@@ -3746,29 +3742,29 @@
       <c r="F50" s="114"/>
       <c r="G50" s="137"/>
       <c r="H50" s="132" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I50" s="126" t="s">
+        <v>309</v>
+      </c>
+      <c r="J50" s="126" t="s">
         <v>311</v>
       </c>
-      <c r="J50" s="126" t="s">
-        <v>313</v>
-      </c>
       <c r="K50" s="112" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L50" s="94"/>
       <c r="M50" s="94"/>
     </row>
     <row r="51" spans="1:13" ht="72" customHeight="1">
       <c r="A51" s="133" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B51" s="128" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C51" s="128" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D51" s="128" t="s">
         <v>12</v>
@@ -3777,22 +3773,22 @@
         <v>277</v>
       </c>
       <c r="F51" s="103" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G51" s="135" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H51" s="131" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I51" s="106" t="s">
+        <v>304</v>
+      </c>
+      <c r="J51" s="106" t="s">
         <v>306</v>
       </c>
-      <c r="J51" s="106" t="s">
+      <c r="K51" s="107" t="s">
         <v>308</v>
-      </c>
-      <c r="K51" s="107" t="s">
-        <v>310</v>
       </c>
       <c r="L51" s="94"/>
       <c r="M51" s="94"/>
@@ -3806,16 +3802,16 @@
       <c r="F52" s="114"/>
       <c r="G52" s="137"/>
       <c r="H52" s="119" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I52" s="117" t="s">
+        <v>309</v>
+      </c>
+      <c r="J52" s="117" t="s">
         <v>311</v>
       </c>
-      <c r="J52" s="117" t="s">
-        <v>313</v>
-      </c>
       <c r="K52" s="122" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L52" s="94"/>
       <c r="M52" s="94"/>

</xml_diff>

<commit_message>
Updated Functional Tests - System administration module.xlsx  - edited the input data to be the same as in System Documentation
</commit_message>
<xml_diff>
--- a/Documents/System administration/Functional Tests - System administration module.xlsx
+++ b/Documents/System administration/Functional Tests - System administration module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F08CDC-0286-4220-A0EF-0EF663156B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C183D0-8EE7-4745-AF5A-7C2A27DB73F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Tests" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="377">
   <si>
     <t>Test scenario</t>
   </si>
@@ -324,9 +324,6 @@
 </t>
   </si>
   <si>
-    <t>LOG_08</t>
-  </si>
-  <si>
     <t>Setup the time to unlock login page</t>
   </si>
   <si>
@@ -350,12 +347,6 @@
   </si>
   <si>
     <t>Administrator changes the time before the login form unlocks by inserting a correct value.</t>
-  </si>
-  <si>
-    <t>LOG_08.02</t>
-  </si>
-  <si>
-    <t>LOG_08.01</t>
   </si>
   <si>
     <t>Administrator inserts an uncorrect value.</t>
@@ -751,16 +742,10 @@
 2. The system displays the filtered list of users that match the selected criteria.</t>
   </si>
   <si>
-    <t>1. Administrator clicks the name of a column.</t>
-  </si>
-  <si>
     <t>Successful display of the user list sorted in a descending order.</t>
   </si>
   <si>
     <t>Successful display of the user list sorted in a ascending order.</t>
-  </si>
-  <si>
-    <t>1. Administrator clicks the name of a column once again.</t>
   </si>
   <si>
     <t>1. System shows the list of users sorted in a descending order by the selected column.</t>
@@ -873,15 +858,6 @@
     <t>Successfully adding a new user.</t>
   </si>
   <si>
-    <t>1 An administrator selects the employee for whom they want to create a new user account.
-2. An administrator presses the "Cancel" button.</t>
-  </si>
-  <si>
-    <t>1 An administrator selects the employee for whom they want to create a new user account.
-2. An administrator presses the "Add new user" button.
-3. An administrator cancels the process of adding a new user by pressing the "Cancel" button.</t>
-  </si>
-  <si>
     <t>1. The system closes the adding new user form without adding a new user.</t>
   </si>
   <si>
@@ -932,11 +908,6 @@
     <t>1. The system closes the user's details edit form without implementing the changes.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. An administrator selects the employee for whom they want to create a new user account.
-2. An administrator presses the "Add new user" button.
-3. An administrator confirms their will by pressing the "Accept" button in a confirmation window. </t>
-  </si>
-  <si>
     <t>User deactivation from the list</t>
   </si>
   <si>
@@ -1005,12 +976,6 @@
     <t>Successful activation of a user from the user's details.</t>
   </si>
   <si>
-    <t>1. An administrator confirms their will to deactivate the selected user by pressing  the "Accept" button.</t>
-  </si>
-  <si>
-    <t>1. An administrator confirms their will to activate the selected user by pressing  the "Accept" button.</t>
-  </si>
-  <si>
     <t>1. The system deactivates the account of the selected user.</t>
   </si>
   <si>
@@ -1018,12 +983,6 @@
   </si>
   <si>
     <t>Cancellation of the deactivation process.</t>
-  </si>
-  <si>
-    <t>1. The administrator abandons the user deactivation process by pressing the "Cancel" button.</t>
-  </si>
-  <si>
-    <t>1. The administrator abandons the user activation process by pressing the "Cancel" button.</t>
   </si>
   <si>
     <t>1. The system closes the form and returns to the user list.</t>
@@ -1157,10 +1116,6 @@
   </si>
   <si>
     <t>1. The system informs the user that "Passwords must be the same".</t>
-  </si>
-  <si>
-    <t>1. An administrator presses the "Cancel" button at any point of the user's details change.
-2. An administrator confirms his will by pressing "Accept" button when systems asks "Do you want to leave Edit Page without saving changes?"</t>
   </si>
   <si>
     <t>1. The administrator presses the "Password" button beneath the "Change Password" label.
@@ -1267,10 +1222,6 @@
 2. The system closes the form and returns to the "Specialization management" form.</t>
   </si>
   <si>
-    <t>1. Administrator presses the "Cancel" button.
-2. Administrator confirms his will of leaving by pressing the "Confirm" button when asked by system whether he wants to leave changes without saving.</t>
-  </si>
-  <si>
     <t>1. The system closes the form and returns to the "Specialization management" form.</t>
   </si>
   <si>
@@ -1344,6 +1295,21 @@
 2. An administrator confirms their will by pressing the "Confirm" button.
 3. The system removes the specialization.
 4. The system closes the form and returns to the "Specialization management" form.</t>
+  </si>
+  <si>
+    <t>STL_01</t>
+  </si>
+  <si>
+    <t>STL_01.01</t>
+  </si>
+  <si>
+    <t>STL_01.02</t>
+  </si>
+  <si>
+    <t>note for J14 - The problem stems from the fact that the domain "eksocmed.com" does not actually exist and we used temporary emails for the presentation.</t>
+  </si>
+  <si>
+    <t>1. Changes in user's details.</t>
   </si>
 </sst>
 </file>
@@ -1422,12 +1388,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1592,7 +1564,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1844,6 +1816,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1862,12 +1855,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1877,50 +1894,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2243,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2260,24 +2235,25 @@
     <col min="9" max="9" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.140625" customWidth="1"/>
     <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="94" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="95"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="110"/>
       <c r="L1" s="28"/>
       <c r="M1" s="29"/>
     </row>
@@ -2319,25 +2295,25 @@
       <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="47.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="107" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="37" t="s">
@@ -2356,13 +2332,13 @@
       <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" ht="47.25">
-      <c r="A4" s="96"/>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="99"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="108"/>
       <c r="H4" s="34" t="s">
         <v>37</v>
       </c>
@@ -2379,13 +2355,13 @@
       <c r="M4" s="29"/>
     </row>
     <row r="5" spans="1:13" ht="48" thickBot="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="100"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="109"/>
       <c r="H5" s="43" t="s">
         <v>38</v>
       </c>
@@ -2513,25 +2489,25 @@
       <c r="M8" s="29"/>
     </row>
     <row r="9" spans="1:13" ht="47.25">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="98" t="s">
+      <c r="G9" s="107" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="37" t="s">
@@ -2550,13 +2526,13 @@
       <c r="M9" s="29"/>
     </row>
     <row r="10" spans="1:13" ht="48" thickBot="1">
-      <c r="A10" s="94"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="100"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="109"/>
       <c r="H10" s="45" t="s">
         <v>75</v>
       </c>
@@ -2589,10 +2565,10 @@
         <v>85</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H11" s="46" t="s">
         <v>77</v>
@@ -2601,7 +2577,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K11" s="48" t="s">
         <v>80</v>
@@ -2647,1597 +2623,1599 @@
       <c r="M12" s="29"/>
     </row>
     <row r="13" spans="1:13" ht="47.25">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="97" t="s">
+        <v>372</v>
+      </c>
+      <c r="B13" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="C13" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="F13" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>373</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" s="39" t="s">
         <v>91</v>
-      </c>
-      <c r="D13" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="I13" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>92</v>
       </c>
       <c r="L13" s="53"/>
       <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:13" ht="32.25" thickBot="1">
-      <c r="A14" s="92"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="100"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="109"/>
       <c r="H14" s="51" t="s">
-        <v>94</v>
+        <v>374</v>
       </c>
       <c r="I14" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="41" t="s">
         <v>96</v>
-      </c>
-      <c r="J14" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="K14" s="41" t="s">
-        <v>99</v>
       </c>
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
     <row r="15" spans="1:13" ht="71.25" customHeight="1">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="87" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="87" t="s">
+      <c r="B15" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" s="87" t="s">
+      <c r="E15" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="107" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="K15" s="39" t="s">
         <v>122</v>
-      </c>
-      <c r="G15" s="98" t="s">
-        <v>123</v>
-      </c>
-      <c r="H15" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="J15" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="K15" s="39" t="s">
-        <v>125</v>
       </c>
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" ht="71.25" customHeight="1">
-      <c r="A16" s="91"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="99"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="108"/>
       <c r="H16" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I16" s="40" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J16" s="52" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
     <row r="17" spans="1:13" ht="87.75" customHeight="1">
-      <c r="A17" s="91"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="99"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="108"/>
       <c r="H17" s="54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J17" s="52" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
     <row r="18" spans="1:13" ht="87.75" customHeight="1" thickBot="1">
-      <c r="A18" s="92"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="100"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="109"/>
       <c r="H18" s="54" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J18" s="52" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K18" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
     <row r="19" spans="1:13" ht="145.5" customHeight="1">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="101" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="104" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="87" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="87" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="101" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="55" t="s">
-        <v>112</v>
-      </c>
       <c r="I19" s="38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="29"/>
+        <v>134</v>
+      </c>
+      <c r="L19" s="113" t="s">
+        <v>375</v>
+      </c>
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="1:13" ht="74.25" customHeight="1" thickBot="1">
-      <c r="A20" s="94"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="102"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="105"/>
       <c r="H20" s="46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I20" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="K20" s="48" t="s">
         <v>135</v>
-      </c>
-      <c r="K20" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
     </row>
     <row r="21" spans="1:13" ht="96.6" customHeight="1" thickBot="1">
       <c r="A21" s="45" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D21" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F21" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="46" t="s">
-        <v>121</v>
-      </c>
       <c r="I21" s="44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J21" s="44" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="48" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
     </row>
     <row r="22" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="94" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="D22" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="F22" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="87" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="87" t="s">
+      <c r="G22" s="94" t="s">
+        <v>166</v>
+      </c>
+      <c r="H22" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="H22" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="I22" s="38" t="s">
-        <v>148</v>
-      </c>
       <c r="J22" s="38" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
     </row>
     <row r="23" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A23" s="91"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="56" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I23" s="52" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J23" s="52" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K23" s="41" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L23" s="29"/>
       <c r="M23" s="29"/>
     </row>
     <row r="24" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A24" s="91"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
       <c r="H24" s="56" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I24" s="52" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J24" s="52" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K24" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
     </row>
     <row r="25" spans="1:13" ht="121.5" customHeight="1">
-      <c r="A25" s="91"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
+      <c r="A25" s="98"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
       <c r="H25" s="56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I25" s="52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J25" s="52" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K25" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
     </row>
     <row r="26" spans="1:13" ht="126" customHeight="1">
-      <c r="A26" s="91"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
+      <c r="A26" s="98"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
       <c r="H26" s="56" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I26" s="52" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J26" s="52" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K26" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
     </row>
     <row r="27" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A27" s="91"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
+      <c r="A27" s="98"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
       <c r="H27" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="I27" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="I27" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="J27" s="52" t="s">
-        <v>181</v>
-      </c>
       <c r="K27" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A28" s="91"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
+      <c r="A28" s="98"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="95"/>
       <c r="H28" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="I28" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="J28" s="52" t="s">
-        <v>182</v>
-      </c>
       <c r="K28" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L28" s="29"/>
       <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" ht="102.75" customHeight="1">
-      <c r="A29" s="91"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
+      <c r="A29" s="98"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
       <c r="H29" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="52" t="s">
-        <v>175</v>
-      </c>
-      <c r="J29" s="52" t="s">
-        <v>183</v>
-      </c>
       <c r="K29" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L29" s="29"/>
       <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:13" ht="102.75" customHeight="1" thickBot="1">
-      <c r="A30" s="92"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="96"/>
       <c r="H30" s="46" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I30" s="44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J30" s="44" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K30" s="48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L30" s="29"/>
       <c r="M30" s="29"/>
     </row>
     <row r="31" spans="1:13" ht="156" customHeight="1" thickBot="1">
       <c r="A31" s="45" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D31" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F31" s="44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H31" s="46" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I31" s="44" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J31" s="44" t="s">
         <v>21</v>
       </c>
       <c r="K31" s="48" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
     </row>
     <row r="32" spans="1:13" ht="117.75" customHeight="1" thickBot="1">
       <c r="A32" s="45" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D32" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H32" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="I32" s="44" t="s">
         <v>160</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H32" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="I32" s="44" t="s">
-        <v>163</v>
       </c>
       <c r="J32" s="44" t="s">
         <v>21</v>
       </c>
       <c r="K32" s="48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L32" s="29"/>
       <c r="M32" s="29"/>
     </row>
     <row r="33" spans="1:13" ht="87" customHeight="1" thickBot="1">
       <c r="A33" s="45" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H33" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="I33" s="44" t="s">
         <v>188</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H33" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="I33" s="44" t="s">
-        <v>191</v>
       </c>
       <c r="J33" s="44" t="s">
         <v>21</v>
       </c>
       <c r="K33" s="48" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L33" s="29"/>
       <c r="M33" s="29"/>
     </row>
     <row r="34" spans="1:13" ht="74.25" customHeight="1">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="97" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="94" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="94" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="87" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" s="87" t="s">
-        <v>196</v>
-      </c>
-      <c r="D34" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="87" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="87" t="s">
-        <v>198</v>
-      </c>
-      <c r="G34" s="101" t="s">
-        <v>206</v>
+      <c r="F34" s="94" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="104" t="s">
+        <v>203</v>
       </c>
       <c r="H34" s="55" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I34" s="38" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="K34" s="39" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="L34" s="29"/>
       <c r="M34" s="29"/>
     </row>
     <row r="35" spans="1:13" ht="79.5" customHeight="1">
-      <c r="A35" s="91"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="103"/>
+      <c r="A35" s="98"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="106"/>
       <c r="H35" s="56" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="K35" s="27" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
     </row>
     <row r="36" spans="1:13" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A36" s="92"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="102"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="105"/>
       <c r="H36" s="46" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="K36" s="27" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="L36" s="29"/>
       <c r="M36" s="29"/>
     </row>
     <row r="37" spans="1:13" ht="94.5" customHeight="1">
-      <c r="A37" s="93" t="s">
-        <v>205</v>
-      </c>
-      <c r="B37" s="87" t="s">
-        <v>200</v>
-      </c>
-      <c r="C37" s="87" t="s">
+      <c r="A37" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="94" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" s="94" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="94" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="94" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" s="104" t="s">
+        <v>219</v>
+      </c>
+      <c r="H37" s="55" t="s">
         <v>201</v>
       </c>
-      <c r="D37" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="87" t="s">
-        <v>197</v>
-      </c>
-      <c r="F37" s="87" t="s">
-        <v>202</v>
-      </c>
-      <c r="G37" s="101" t="s">
-        <v>224</v>
-      </c>
-      <c r="H37" s="55" t="s">
+      <c r="I37" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="I37" s="38" t="s">
-        <v>208</v>
-      </c>
       <c r="J37" s="38" t="s">
-        <v>207</v>
+        <v>21</v>
       </c>
       <c r="K37" s="39" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
     </row>
     <row r="38" spans="1:13" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A38" s="94"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="102"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="105"/>
       <c r="H38" s="46" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I38" s="44" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J38" s="44" t="s">
-        <v>210</v>
+        <v>21</v>
       </c>
       <c r="K38" s="48" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L38" s="29"/>
       <c r="M38" s="29"/>
     </row>
     <row r="39" spans="1:13" ht="149.25" customHeight="1">
-      <c r="A39" s="93" t="s">
-        <v>289</v>
-      </c>
-      <c r="B39" s="87" t="s">
-        <v>234</v>
-      </c>
-      <c r="C39" s="87" t="s">
+      <c r="A39" s="101" t="s">
+        <v>277</v>
+      </c>
+      <c r="B39" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="D39" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="94" t="s">
+        <v>265</v>
+      </c>
+      <c r="F39" s="94" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="H39" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="I39" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="D39" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="87" t="s">
-        <v>273</v>
-      </c>
-      <c r="F39" s="87" t="s">
-        <v>236</v>
-      </c>
-      <c r="G39" s="101" t="s">
-        <v>237</v>
-      </c>
-      <c r="H39" s="56" t="s">
-        <v>309</v>
-      </c>
-      <c r="I39" s="38" t="s">
-        <v>240</v>
-      </c>
       <c r="J39" s="38" t="s">
-        <v>259</v>
+        <v>21</v>
       </c>
       <c r="K39" s="41" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="L39" s="29"/>
       <c r="M39" s="29"/>
     </row>
     <row r="40" spans="1:13" ht="93.75" customHeight="1">
-      <c r="A40" s="104"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="88"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="103"/>
+      <c r="A40" s="103"/>
+      <c r="B40" s="95"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="106"/>
       <c r="H40" s="56" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="I40" s="52" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J40" s="52" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
       <c r="K40" s="41" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="L40" s="29"/>
       <c r="M40" s="29"/>
     </row>
     <row r="41" spans="1:13" ht="156.75" customHeight="1" thickBot="1">
-      <c r="A41" s="94"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="102"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="96"/>
+      <c r="G41" s="105"/>
       <c r="H41" s="46" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I41" s="44" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J41" s="44" t="s">
-        <v>242</v>
+        <v>21</v>
       </c>
       <c r="K41" s="48" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="L41" s="29"/>
       <c r="M41" s="29"/>
     </row>
     <row r="42" spans="1:13" ht="102" customHeight="1" thickBot="1">
       <c r="A42" s="57" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D42" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="52" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H42" s="56" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="I42" s="52" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J42" s="52" t="s">
         <v>21</v>
       </c>
       <c r="K42" s="41" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L42" s="29"/>
       <c r="M42" s="29"/>
     </row>
     <row r="43" spans="1:13" ht="123" customHeight="1">
-      <c r="A43" s="93" t="s">
-        <v>291</v>
-      </c>
-      <c r="B43" s="87" t="s">
-        <v>251</v>
-      </c>
-      <c r="C43" s="87" t="s">
-        <v>252</v>
-      </c>
-      <c r="D43" s="87" t="s">
+      <c r="A43" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="B43" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="C43" s="94" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="87" t="s">
-        <v>253</v>
-      </c>
-      <c r="F43" s="87" t="s">
-        <v>254</v>
-      </c>
-      <c r="G43" s="101" t="s">
-        <v>310</v>
+      <c r="E43" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="F43" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="G43" s="104" t="s">
+        <v>298</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="I43" s="38" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J43" s="24" t="s">
-        <v>310</v>
+        <v>376</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="L43" s="29"/>
       <c r="M43" s="29"/>
     </row>
     <row r="44" spans="1:13" ht="148.5" customHeight="1" thickBot="1">
-      <c r="A44" s="94"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="102"/>
+      <c r="A44" s="102"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="96"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="105"/>
       <c r="H44" s="46" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="I44" s="44" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>331</v>
+        <v>21</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="L44" s="29"/>
       <c r="M44" s="29"/>
     </row>
     <row r="45" spans="1:13" ht="66.75" customHeight="1">
-      <c r="A45" s="93" t="s">
-        <v>292</v>
-      </c>
-      <c r="B45" s="87" t="s">
+      <c r="A45" s="101" t="s">
+        <v>280</v>
+      </c>
+      <c r="B45" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="C45" s="94" t="s">
+        <v>256</v>
+      </c>
+      <c r="D45" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="94" t="s">
+        <v>264</v>
+      </c>
+      <c r="F45" s="94" t="s">
         <v>260</v>
       </c>
-      <c r="C45" s="87" t="s">
-        <v>264</v>
-      </c>
-      <c r="D45" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="87" t="s">
+      <c r="G45" s="104" t="s">
+        <v>262</v>
+      </c>
+      <c r="H45" s="55" t="s">
+        <v>291</v>
+      </c>
+      <c r="I45" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="J45" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="39" t="s">
         <v>272</v>
-      </c>
-      <c r="F45" s="87" t="s">
-        <v>268</v>
-      </c>
-      <c r="G45" s="101" t="s">
-        <v>270</v>
-      </c>
-      <c r="H45" s="55" t="s">
-        <v>303</v>
-      </c>
-      <c r="I45" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="J45" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="K45" s="39" t="s">
-        <v>282</v>
       </c>
       <c r="L45" s="29"/>
       <c r="M45" s="29"/>
     </row>
     <row r="46" spans="1:13" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A46" s="94"/>
-      <c r="B46" s="89"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="102"/>
+      <c r="A46" s="102"/>
+      <c r="B46" s="96"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="105"/>
       <c r="H46" s="46" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="I46" s="44" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="J46" s="52" t="s">
-        <v>285</v>
+        <v>21</v>
       </c>
       <c r="K46" s="48" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="L46" s="29"/>
       <c r="M46" s="29"/>
     </row>
     <row r="47" spans="1:13" ht="66.75" customHeight="1">
-      <c r="A47" s="93" t="s">
-        <v>293</v>
-      </c>
-      <c r="B47" s="87" t="s">
-        <v>261</v>
-      </c>
-      <c r="C47" s="87" t="s">
+      <c r="A47" s="101" t="s">
+        <v>281</v>
+      </c>
+      <c r="B47" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C47" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="F47" s="94" t="s">
+        <v>260</v>
+      </c>
+      <c r="G47" s="92" t="s">
         <v>266</v>
       </c>
-      <c r="D47" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="87" t="s">
-        <v>253</v>
-      </c>
-      <c r="F47" s="87" t="s">
-        <v>268</v>
-      </c>
-      <c r="G47" s="105" t="s">
-        <v>274</v>
-      </c>
       <c r="H47" s="55" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="I47" s="38" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="J47" s="38" t="s">
-        <v>280</v>
+        <v>21</v>
       </c>
       <c r="K47" s="39" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="L47" s="29"/>
       <c r="M47" s="29"/>
     </row>
     <row r="48" spans="1:13" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A48" s="94"/>
-      <c r="B48" s="89"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="106"/>
+      <c r="A48" s="102"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="93"/>
       <c r="H48" s="46" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="I48" s="52" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="J48" s="44" t="s">
-        <v>285</v>
+        <v>21</v>
       </c>
       <c r="K48" s="48" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="L48" s="29"/>
       <c r="M48" s="29"/>
     </row>
     <row r="49" spans="1:13" ht="66.75" customHeight="1">
-      <c r="A49" s="93" t="s">
-        <v>294</v>
-      </c>
-      <c r="B49" s="87" t="s">
-        <v>262</v>
-      </c>
-      <c r="C49" s="87" t="s">
-        <v>265</v>
-      </c>
-      <c r="D49" s="87" t="s">
+      <c r="A49" s="101" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D49" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="87" t="s">
-        <v>272</v>
-      </c>
-      <c r="F49" s="87" t="s">
+      <c r="E49" s="94" t="s">
+        <v>264</v>
+      </c>
+      <c r="F49" s="94" t="s">
+        <v>261</v>
+      </c>
+      <c r="G49" s="92" t="s">
+        <v>263</v>
+      </c>
+      <c r="H49" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="I49" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="G49" s="105" t="s">
-        <v>271</v>
-      </c>
-      <c r="H49" s="55" t="s">
-        <v>299</v>
-      </c>
-      <c r="I49" s="38" t="s">
-        <v>277</v>
-      </c>
       <c r="J49" s="38" t="s">
-        <v>281</v>
+        <v>21</v>
       </c>
       <c r="K49" s="39" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="L49" s="29"/>
       <c r="M49" s="29"/>
     </row>
     <row r="50" spans="1:13" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A50" s="94"/>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="106"/>
+      <c r="A50" s="102"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="93"/>
       <c r="H50" s="56" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="I50" s="52" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="J50" s="52" t="s">
-        <v>286</v>
+        <v>21</v>
       </c>
       <c r="K50" s="41" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="L50" s="29"/>
       <c r="M50" s="29"/>
     </row>
     <row r="51" spans="1:13" ht="72" customHeight="1">
-      <c r="A51" s="104" t="s">
-        <v>295</v>
-      </c>
-      <c r="B51" s="88" t="s">
-        <v>263</v>
-      </c>
-      <c r="C51" s="88" t="s">
+      <c r="A51" s="103" t="s">
+        <v>283</v>
+      </c>
+      <c r="B51" s="95" t="s">
+        <v>255</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="D51" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="95" t="s">
+        <v>246</v>
+      </c>
+      <c r="F51" s="94" t="s">
+        <v>261</v>
+      </c>
+      <c r="G51" s="100" t="s">
         <v>267</v>
       </c>
-      <c r="D51" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="88" t="s">
-        <v>253</v>
-      </c>
-      <c r="F51" s="87" t="s">
-        <v>269</v>
-      </c>
-      <c r="G51" s="107" t="s">
-        <v>275</v>
-      </c>
       <c r="H51" s="55" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="I51" s="38" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="J51" s="38" t="s">
-        <v>281</v>
+        <v>21</v>
       </c>
       <c r="K51" s="39" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="L51" s="29"/>
       <c r="M51" s="29"/>
     </row>
     <row r="52" spans="1:13" ht="72" customHeight="1" thickBot="1">
-      <c r="A52" s="94"/>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="89"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="89"/>
-      <c r="G52" s="106"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="96"/>
+      <c r="F52" s="96"/>
+      <c r="G52" s="93"/>
       <c r="H52" s="46" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="I52" s="44" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="J52" s="44" t="s">
-        <v>286</v>
+        <v>21</v>
       </c>
       <c r="K52" s="48" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="L52" s="29"/>
       <c r="M52" s="29"/>
     </row>
     <row r="53" spans="1:13" ht="63">
-      <c r="A53" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="B53" s="87" t="s">
-        <v>327</v>
-      </c>
-      <c r="C53" s="87" t="s">
-        <v>328</v>
-      </c>
-      <c r="D53" s="87" t="s">
+      <c r="A53" s="97" t="s">
+        <v>314</v>
+      </c>
+      <c r="B53" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="C53" s="94" t="s">
+        <v>316</v>
+      </c>
+      <c r="D53" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="87" t="s">
-        <v>253</v>
-      </c>
-      <c r="F53" s="87" t="s">
+      <c r="E53" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="F53" s="94" t="s">
+        <v>317</v>
+      </c>
+      <c r="G53" s="94" t="s">
+        <v>319</v>
+      </c>
+      <c r="H53" s="55" t="s">
         <v>329</v>
       </c>
-      <c r="G53" s="87" t="s">
-        <v>332</v>
-      </c>
-      <c r="H53" s="55" t="s">
-        <v>342</v>
-      </c>
       <c r="I53" s="61" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J53" s="61" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="K53" s="67" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="L53" s="29"/>
       <c r="M53" s="29"/>
     </row>
     <row r="54" spans="1:13" ht="63">
-      <c r="A54" s="91"/>
-      <c r="B54" s="88"/>
-      <c r="C54" s="88"/>
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="88"/>
+      <c r="A54" s="98"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
       <c r="H54" s="56" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="I54" s="59" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J54" s="59" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K54" s="68" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="L54" s="29"/>
       <c r="M54" s="29"/>
     </row>
     <row r="55" spans="1:13" ht="63">
-      <c r="A55" s="91"/>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="88"/>
-      <c r="G55" s="88"/>
+      <c r="A55" s="98"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="95"/>
+      <c r="G55" s="95"/>
       <c r="H55" s="56" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="I55" s="59" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J55" s="59" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K55" s="68" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="L55" s="29"/>
       <c r="M55" s="29"/>
     </row>
     <row r="56" spans="1:13" ht="94.5">
-      <c r="A56" s="91"/>
-      <c r="B56" s="88"/>
-      <c r="C56" s="88"/>
-      <c r="D56" s="88"/>
-      <c r="E56" s="88"/>
-      <c r="F56" s="88"/>
-      <c r="G56" s="88"/>
+      <c r="A56" s="98"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="95"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="95"/>
       <c r="H56" s="56" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="I56" s="59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J56" s="59" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K56" s="68" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L56" s="29"/>
       <c r="M56" s="29"/>
     </row>
     <row r="57" spans="1:13" ht="94.5">
-      <c r="A57" s="91"/>
-      <c r="B57" s="88"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="88"/>
+      <c r="A57" s="98"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="95"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="95"/>
       <c r="H57" s="56" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="I57" s="59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J57" s="59" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="K57" s="68" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L57" s="29"/>
       <c r="M57" s="29"/>
     </row>
     <row r="58" spans="1:13" ht="78.75">
-      <c r="A58" s="91"/>
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="88"/>
+      <c r="A58" s="98"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
       <c r="H58" s="56" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="I58" s="59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J58" s="59" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K58" s="68" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L58" s="29"/>
       <c r="M58" s="29"/>
     </row>
     <row r="59" spans="1:13" ht="78.75">
-      <c r="A59" s="91"/>
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
+      <c r="A59" s="98"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="95"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="95"/>
+      <c r="F59" s="95"/>
+      <c r="G59" s="95"/>
       <c r="H59" s="56" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="I59" s="59" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J59" s="59" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K59" s="68" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L59" s="29"/>
       <c r="M59" s="29"/>
     </row>
     <row r="60" spans="1:13" ht="78.75">
-      <c r="A60" s="91"/>
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="88"/>
-      <c r="G60" s="88"/>
+      <c r="A60" s="98"/>
+      <c r="B60" s="95"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="95"/>
+      <c r="E60" s="95"/>
+      <c r="F60" s="95"/>
+      <c r="G60" s="95"/>
       <c r="H60" s="56" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="I60" s="59" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J60" s="59" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K60" s="68" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L60" s="29"/>
       <c r="M60" s="29"/>
     </row>
     <row r="61" spans="1:13" ht="79.5" thickBot="1">
-      <c r="A61" s="92"/>
-      <c r="B61" s="89"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="89"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="89"/>
-      <c r="G61" s="89"/>
+      <c r="A61" s="99"/>
+      <c r="B61" s="96"/>
+      <c r="C61" s="96"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
+      <c r="F61" s="96"/>
+      <c r="G61" s="96"/>
       <c r="H61" s="46" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="I61" s="60" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K61" s="69" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="L61" s="29"/>
       <c r="M61" s="29"/>
     </row>
     <row r="62" spans="1:13" ht="134.25" customHeight="1" thickBot="1">
       <c r="A62" s="66" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="B62" s="60" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C62" s="60" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="D62" s="60" t="s">
         <v>12</v>
       </c>
       <c r="E62" s="60" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="F62" s="60" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="G62" s="65" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="H62" s="46" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="I62" s="60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J62" s="60" t="s">
         <v>21</v>
       </c>
       <c r="K62" s="69" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="L62" s="29"/>
       <c r="M62" s="29"/>
     </row>
     <row r="63" spans="1:13" ht="99.75" customHeight="1">
-      <c r="A63" s="109" t="s">
-        <v>351</v>
-      </c>
-      <c r="B63" s="105" t="s">
-        <v>352</v>
-      </c>
-      <c r="C63" s="105" t="s">
-        <v>353</v>
-      </c>
-      <c r="D63" s="105" t="s">
+      <c r="A63" s="90" t="s">
+        <v>338</v>
+      </c>
+      <c r="B63" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C63" s="92" t="s">
+        <v>340</v>
+      </c>
+      <c r="D63" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="105" t="s">
-        <v>354</v>
-      </c>
-      <c r="F63" s="105" t="s">
-        <v>355</v>
-      </c>
-      <c r="G63" s="105" t="s">
-        <v>359</v>
-      </c>
-      <c r="H63" s="111" t="s">
-        <v>356</v>
+      <c r="E63" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="F63" s="92" t="s">
+        <v>342</v>
+      </c>
+      <c r="G63" s="92" t="s">
+        <v>346</v>
+      </c>
+      <c r="H63" s="88" t="s">
+        <v>343</v>
       </c>
       <c r="I63" s="62" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="J63" s="62" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="K63" s="64" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="L63" s="29"/>
       <c r="M63" s="29"/>
     </row>
     <row r="64" spans="1:13" ht="136.5" customHeight="1" thickBot="1">
-      <c r="A64" s="110"/>
-      <c r="B64" s="106"/>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="106"/>
-      <c r="F64" s="106"/>
-      <c r="G64" s="106"/>
-      <c r="H64" s="112" t="s">
-        <v>357</v>
+      <c r="A64" s="91"/>
+      <c r="B64" s="93"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="93"/>
+      <c r="E64" s="93"/>
+      <c r="F64" s="93"/>
+      <c r="G64" s="93"/>
+      <c r="H64" s="89" t="s">
+        <v>344</v>
       </c>
       <c r="I64" s="63" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="J64" s="63" t="s">
-        <v>363</v>
+        <v>21</v>
       </c>
       <c r="K64" s="65" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="L64" s="29"/>
       <c r="M64" s="29"/>
     </row>
     <row r="65" spans="1:13" ht="117" customHeight="1">
-      <c r="A65" s="109" t="s">
-        <v>365</v>
-      </c>
-      <c r="B65" s="105" t="s">
-        <v>370</v>
-      </c>
-      <c r="C65" s="105" t="s">
-        <v>371</v>
-      </c>
-      <c r="D65" s="105" t="s">
+      <c r="A65" s="90" t="s">
+        <v>351</v>
+      </c>
+      <c r="B65" s="92" t="s">
+        <v>356</v>
+      </c>
+      <c r="C65" s="92" t="s">
+        <v>357</v>
+      </c>
+      <c r="D65" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="105" t="s">
-        <v>354</v>
-      </c>
-      <c r="F65" s="105" t="s">
-        <v>372</v>
-      </c>
-      <c r="G65" s="105" t="s">
-        <v>373</v>
-      </c>
-      <c r="H65" s="111" t="s">
-        <v>366</v>
+      <c r="E65" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="F65" s="92" t="s">
+        <v>358</v>
+      </c>
+      <c r="G65" s="92" t="s">
+        <v>359</v>
+      </c>
+      <c r="H65" s="88" t="s">
+        <v>352</v>
       </c>
       <c r="I65" s="62" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="J65" s="62" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="K65" s="64" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="L65" s="29"/>
       <c r="M65" s="29"/>
     </row>
     <row r="66" spans="1:13" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A66" s="110"/>
-      <c r="B66" s="106"/>
-      <c r="C66" s="106"/>
-      <c r="D66" s="106"/>
-      <c r="E66" s="106"/>
-      <c r="F66" s="106"/>
-      <c r="G66" s="106"/>
-      <c r="H66" s="112" t="s">
-        <v>367</v>
+      <c r="A66" s="91"/>
+      <c r="B66" s="93"/>
+      <c r="C66" s="93"/>
+      <c r="D66" s="93"/>
+      <c r="E66" s="93"/>
+      <c r="F66" s="93"/>
+      <c r="G66" s="93"/>
+      <c r="H66" s="89" t="s">
+        <v>353</v>
       </c>
       <c r="I66" s="63" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="J66" s="63" t="s">
-        <v>363</v>
+        <v>21</v>
       </c>
       <c r="K66" s="65" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="L66" s="29"/>
       <c r="M66" s="29"/>
     </row>
     <row r="67" spans="1:13" ht="88.5" customHeight="1">
-      <c r="A67" s="109" t="s">
-        <v>376</v>
-      </c>
-      <c r="B67" s="105" t="s">
-        <v>377</v>
-      </c>
-      <c r="C67" s="105" t="s">
-        <v>378</v>
-      </c>
-      <c r="D67" s="105" t="s">
+      <c r="A67" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="B67" s="92" t="s">
+        <v>363</v>
+      </c>
+      <c r="C67" s="92" t="s">
+        <v>364</v>
+      </c>
+      <c r="D67" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="105" t="s">
-        <v>354</v>
-      </c>
-      <c r="F67" s="105" t="s">
-        <v>384</v>
-      </c>
-      <c r="G67" s="105" t="s">
-        <v>385</v>
-      </c>
-      <c r="H67" s="111" t="s">
-        <v>379</v>
+      <c r="E67" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="F67" s="92" t="s">
+        <v>370</v>
+      </c>
+      <c r="G67" s="92" t="s">
+        <v>371</v>
+      </c>
+      <c r="H67" s="88" t="s">
+        <v>365</v>
       </c>
       <c r="I67" s="62" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="J67" s="62" t="s">
         <v>21</v>
       </c>
       <c r="K67" s="64" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="L67" s="29"/>
       <c r="M67" s="29"/>
     </row>
     <row r="68" spans="1:13" ht="78" customHeight="1" thickBot="1">
-      <c r="A68" s="110"/>
-      <c r="B68" s="106"/>
-      <c r="C68" s="106"/>
-      <c r="D68" s="106"/>
-      <c r="E68" s="106"/>
-      <c r="F68" s="106"/>
-      <c r="G68" s="106"/>
-      <c r="H68" s="112" t="s">
-        <v>380</v>
+      <c r="A68" s="91"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="93"/>
+      <c r="D68" s="93"/>
+      <c r="E68" s="93"/>
+      <c r="F68" s="93"/>
+      <c r="G68" s="93"/>
+      <c r="H68" s="89" t="s">
+        <v>366</v>
       </c>
       <c r="I68" s="63" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="J68" s="63" t="s">
         <v>21</v>
       </c>
       <c r="K68" s="65" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="L68" s="29"/>
       <c r="M68" s="29"/>
@@ -4318,62 +4296,62 @@
       <c r="M73" s="29"/>
     </row>
     <row r="74" spans="1:13" ht="15.75">
-      <c r="A74" s="108"/>
-      <c r="B74" s="108"/>
-      <c r="C74" s="108"/>
-      <c r="D74" s="108"/>
-      <c r="E74" s="108"/>
-      <c r="F74" s="108"/>
-      <c r="G74" s="108"/>
-      <c r="H74" s="108"/>
-      <c r="I74" s="108"/>
-      <c r="J74" s="108"/>
-      <c r="K74" s="108"/>
+      <c r="A74" s="87"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="87"/>
+      <c r="E74" s="87"/>
+      <c r="F74" s="87"/>
+      <c r="G74" s="87"/>
+      <c r="H74" s="87"/>
+      <c r="I74" s="87"/>
+      <c r="J74" s="87"/>
+      <c r="K74" s="87"/>
       <c r="L74" s="29"/>
       <c r="M74" s="29"/>
     </row>
     <row r="75" spans="1:13" ht="15.75">
-      <c r="A75" s="108"/>
-      <c r="B75" s="108"/>
-      <c r="C75" s="108"/>
-      <c r="D75" s="108"/>
-      <c r="E75" s="108"/>
-      <c r="F75" s="108"/>
-      <c r="G75" s="108"/>
-      <c r="H75" s="108"/>
-      <c r="I75" s="108"/>
-      <c r="J75" s="108"/>
-      <c r="K75" s="108"/>
+      <c r="A75" s="87"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="87"/>
+      <c r="D75" s="87"/>
+      <c r="E75" s="87"/>
+      <c r="F75" s="87"/>
+      <c r="G75" s="87"/>
+      <c r="H75" s="87"/>
+      <c r="I75" s="87"/>
+      <c r="J75" s="87"/>
+      <c r="K75" s="87"/>
       <c r="L75" s="29"/>
       <c r="M75" s="29"/>
     </row>
     <row r="76" spans="1:13" ht="15.75">
-      <c r="A76" s="108"/>
-      <c r="B76" s="108"/>
-      <c r="C76" s="108"/>
-      <c r="D76" s="108"/>
-      <c r="E76" s="108"/>
-      <c r="F76" s="108"/>
-      <c r="G76" s="108"/>
-      <c r="H76" s="108"/>
-      <c r="I76" s="108"/>
-      <c r="J76" s="108"/>
-      <c r="K76" s="108"/>
+      <c r="A76" s="87"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="87"/>
+      <c r="D76" s="87"/>
+      <c r="E76" s="87"/>
+      <c r="F76" s="87"/>
+      <c r="G76" s="87"/>
+      <c r="H76" s="87"/>
+      <c r="I76" s="87"/>
+      <c r="J76" s="87"/>
+      <c r="K76" s="87"/>
       <c r="L76" s="29"/>
       <c r="M76" s="29"/>
     </row>
     <row r="77" spans="1:13" ht="15.75">
-      <c r="A77" s="108"/>
-      <c r="B77" s="108"/>
-      <c r="C77" s="108"/>
-      <c r="D77" s="108"/>
-      <c r="E77" s="108"/>
-      <c r="F77" s="108"/>
-      <c r="G77" s="108"/>
-      <c r="H77" s="108"/>
-      <c r="I77" s="108"/>
-      <c r="J77" s="108"/>
-      <c r="K77" s="108"/>
+      <c r="A77" s="87"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="87"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="87"/>
+      <c r="H77" s="87"/>
+      <c r="I77" s="87"/>
+      <c r="J77" s="87"/>
+      <c r="K77" s="87"/>
       <c r="L77" s="29"/>
       <c r="M77" s="29"/>
     </row>
@@ -5234,29 +5212,92 @@
     </row>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="F53:F61"/>
-    <mergeCell ref="G53:G61"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="G22:G30"/>
+    <mergeCell ref="F22:F30"/>
+    <mergeCell ref="E22:E30"/>
+    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="A53:A61"/>
     <mergeCell ref="B53:B61"/>
     <mergeCell ref="C53:C61"/>
@@ -5276,92 +5317,29 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="F49:F50"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="B22:B30"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="G22:G30"/>
-    <mergeCell ref="F22:F30"/>
-    <mergeCell ref="E22:E30"/>
-    <mergeCell ref="D22:D30"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="F53:F61"/>
+    <mergeCell ref="G53:G61"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5423,25 +5401,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="I2" s="11"/>
     </row>
@@ -5450,25 +5428,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H3" s="81" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="I3" s="12"/>
     </row>
@@ -5477,25 +5455,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F4" s="70" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="81" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="I4" s="12"/>
     </row>
@@ -5504,25 +5482,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H5" s="81" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I5" s="12"/>
     </row>
@@ -5531,25 +5509,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="F6" s="74" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H6" s="84" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I6" s="12"/>
       <c r="M6" s="6"/>
@@ -5559,25 +5537,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H7" s="81" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="I7" s="12"/>
       <c r="M7" s="3"/>
@@ -5587,25 +5565,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H8" s="81" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="I8" s="12"/>
     </row>
@@ -5614,25 +5592,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H9" s="81" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="I9" s="12"/>
     </row>
@@ -5641,25 +5619,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="F10" s="72" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H10" s="82" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="I10" s="76"/>
     </row>
@@ -5671,22 +5649,22 @@
         <v>67</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E11" s="71" t="s">
         <v>311</v>
       </c>
-      <c r="E11" s="71" t="s">
-        <v>323</v>
-      </c>
       <c r="F11" s="71" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>60</v>
       </c>
       <c r="H11" s="83" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="I11" s="11"/>
     </row>
@@ -5698,22 +5676,22 @@
         <v>67</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E12" s="85" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="F12" s="85" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H12" s="81" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -5725,22 +5703,22 @@
         <v>67</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E13" s="85" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="F13" s="85" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>60</v>
       </c>
       <c r="H13" s="81" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I13" s="12"/>
     </row>
@@ -5752,22 +5730,22 @@
         <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E14" s="86" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H14" s="82" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I14" s="76"/>
     </row>

</xml_diff>